<commit_message>
Preparing to synthesize full_mat unit to check for syntheis and fmax.
</commit_message>
<xml_diff>
--- a/doc/design/schedule.xlsx
+++ b/doc/design/schedule.xlsx
@@ -1498,18 +1498,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1523,6 +1511,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2555,7 +2555,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="AL1" sqref="AL1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AO26" sqref="AO26"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.1640625" defaultRowHeight="42" customHeight="1" x14ac:dyDescent="0"/>
@@ -2569,123 +2569,123 @@
       <c r="B1" s="3"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26"/>
-      <c r="V1" s="26"/>
-      <c r="W1" s="26"/>
-      <c r="X1" s="26"/>
-      <c r="Y1" s="26"/>
-      <c r="Z1" s="26"/>
-      <c r="AA1" s="26"/>
-      <c r="AB1" s="26"/>
-      <c r="AC1" s="26"/>
-      <c r="AD1" s="26"/>
-      <c r="AE1" s="26"/>
-      <c r="AF1" s="26"/>
-      <c r="AG1" s="26"/>
-      <c r="AH1" s="26"/>
-      <c r="AI1" s="26"/>
-      <c r="AJ1" s="26"/>
-      <c r="AK1" s="26"/>
-      <c r="AL1" s="26"/>
-      <c r="AM1" s="26"/>
-      <c r="AN1" s="26"/>
-      <c r="AO1" s="26"/>
-      <c r="AP1" s="26"/>
-      <c r="AQ1" s="26"/>
-      <c r="AR1" s="26"/>
-      <c r="AS1" s="26"/>
-      <c r="AT1" s="26"/>
-      <c r="AU1" s="26"/>
-      <c r="AV1" s="26"/>
-      <c r="AW1" s="26"/>
-      <c r="AX1" s="26"/>
-      <c r="AY1" s="26"/>
-      <c r="AZ1" s="26"/>
-      <c r="BA1" s="26"/>
-      <c r="BB1" s="26"/>
-      <c r="BC1" s="26"/>
-      <c r="BD1" s="26"/>
-      <c r="BE1" s="26"/>
-      <c r="BF1" s="26"/>
-      <c r="BG1" s="26"/>
-      <c r="BH1" s="26"/>
-      <c r="BI1" s="26"/>
-      <c r="BJ1" s="26"/>
-      <c r="BK1" s="26"/>
-      <c r="BL1" s="26"/>
-      <c r="BM1" s="26"/>
-      <c r="BN1" s="26"/>
-      <c r="BO1" s="26"/>
-      <c r="BP1" s="26"/>
-      <c r="BQ1" s="26"/>
-      <c r="BR1" s="26"/>
-      <c r="BS1" s="26"/>
-      <c r="BT1" s="26"/>
-      <c r="BU1" s="26"/>
-      <c r="BV1" s="26"/>
-      <c r="BW1" s="26"/>
-      <c r="BX1" s="26"/>
-      <c r="BY1" s="26"/>
-      <c r="BZ1" s="26"/>
-      <c r="CA1" s="26"/>
-      <c r="CB1" s="26"/>
-      <c r="CC1" s="26"/>
-      <c r="CD1" s="26"/>
-      <c r="CE1" s="26"/>
-      <c r="CF1" s="26"/>
-      <c r="CG1" s="26"/>
-      <c r="CH1" s="26"/>
-      <c r="CI1" s="26"/>
-      <c r="CJ1" s="26"/>
-      <c r="CK1" s="26"/>
-      <c r="CL1" s="26"/>
-      <c r="CM1" s="26"/>
-      <c r="CN1" s="26"/>
-      <c r="CO1" s="26"/>
-      <c r="CP1" s="26"/>
-      <c r="CQ1" s="26"/>
-      <c r="CR1" s="26"/>
-      <c r="CS1" s="26"/>
-      <c r="CT1" s="26"/>
-      <c r="CU1" s="26"/>
-      <c r="CV1" s="26"/>
-      <c r="CW1" s="26"/>
-      <c r="CX1" s="26"/>
-      <c r="CY1" s="26"/>
-      <c r="CZ1" s="26"/>
-      <c r="DA1" s="26"/>
-      <c r="DB1" s="26"/>
-      <c r="DC1" s="26"/>
-      <c r="DD1" s="26"/>
-      <c r="DE1" s="26"/>
-      <c r="DF1" s="26"/>
-      <c r="DG1" s="26"/>
-      <c r="DH1" s="26"/>
-      <c r="DI1" s="26"/>
-      <c r="DJ1" s="26"/>
-      <c r="DK1" s="26"/>
-      <c r="DL1" s="26"/>
-      <c r="DM1" s="26"/>
-      <c r="DN1" s="26"/>
-      <c r="DO1" s="27"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="31"/>
+      <c r="AC1" s="31"/>
+      <c r="AD1" s="31"/>
+      <c r="AE1" s="31"/>
+      <c r="AF1" s="31"/>
+      <c r="AG1" s="31"/>
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="31"/>
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="31"/>
+      <c r="AL1" s="31"/>
+      <c r="AM1" s="31"/>
+      <c r="AN1" s="31"/>
+      <c r="AO1" s="31"/>
+      <c r="AP1" s="31"/>
+      <c r="AQ1" s="31"/>
+      <c r="AR1" s="31"/>
+      <c r="AS1" s="31"/>
+      <c r="AT1" s="31"/>
+      <c r="AU1" s="31"/>
+      <c r="AV1" s="31"/>
+      <c r="AW1" s="31"/>
+      <c r="AX1" s="31"/>
+      <c r="AY1" s="31"/>
+      <c r="AZ1" s="31"/>
+      <c r="BA1" s="31"/>
+      <c r="BB1" s="31"/>
+      <c r="BC1" s="31"/>
+      <c r="BD1" s="31"/>
+      <c r="BE1" s="31"/>
+      <c r="BF1" s="31"/>
+      <c r="BG1" s="31"/>
+      <c r="BH1" s="31"/>
+      <c r="BI1" s="31"/>
+      <c r="BJ1" s="31"/>
+      <c r="BK1" s="31"/>
+      <c r="BL1" s="31"/>
+      <c r="BM1" s="31"/>
+      <c r="BN1" s="31"/>
+      <c r="BO1" s="31"/>
+      <c r="BP1" s="31"/>
+      <c r="BQ1" s="31"/>
+      <c r="BR1" s="31"/>
+      <c r="BS1" s="31"/>
+      <c r="BT1" s="31"/>
+      <c r="BU1" s="31"/>
+      <c r="BV1" s="31"/>
+      <c r="BW1" s="31"/>
+      <c r="BX1" s="31"/>
+      <c r="BY1" s="31"/>
+      <c r="BZ1" s="31"/>
+      <c r="CA1" s="31"/>
+      <c r="CB1" s="31"/>
+      <c r="CC1" s="31"/>
+      <c r="CD1" s="31"/>
+      <c r="CE1" s="31"/>
+      <c r="CF1" s="31"/>
+      <c r="CG1" s="31"/>
+      <c r="CH1" s="31"/>
+      <c r="CI1" s="31"/>
+      <c r="CJ1" s="31"/>
+      <c r="CK1" s="31"/>
+      <c r="CL1" s="31"/>
+      <c r="CM1" s="31"/>
+      <c r="CN1" s="31"/>
+      <c r="CO1" s="31"/>
+      <c r="CP1" s="31"/>
+      <c r="CQ1" s="31"/>
+      <c r="CR1" s="31"/>
+      <c r="CS1" s="31"/>
+      <c r="CT1" s="31"/>
+      <c r="CU1" s="31"/>
+      <c r="CV1" s="31"/>
+      <c r="CW1" s="31"/>
+      <c r="CX1" s="31"/>
+      <c r="CY1" s="31"/>
+      <c r="CZ1" s="31"/>
+      <c r="DA1" s="31"/>
+      <c r="DB1" s="31"/>
+      <c r="DC1" s="31"/>
+      <c r="DD1" s="31"/>
+      <c r="DE1" s="31"/>
+      <c r="DF1" s="31"/>
+      <c r="DG1" s="31"/>
+      <c r="DH1" s="31"/>
+      <c r="DI1" s="31"/>
+      <c r="DJ1" s="31"/>
+      <c r="DK1" s="31"/>
+      <c r="DL1" s="31"/>
+      <c r="DM1" s="31"/>
+      <c r="DN1" s="31"/>
+      <c r="DO1" s="32"/>
       <c r="DP1" s="22"/>
       <c r="DQ1" s="22"/>
       <c r="DR1" s="22"/>
@@ -3164,13 +3164,13 @@
       <c r="DR2" s="22"/>
     </row>
     <row r="3" spans="2:122" ht="42" customHeight="1">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="29">
+      <c r="C3" s="34">
         <v>2</v>
       </c>
-      <c r="D3" s="29">
+      <c r="D3" s="34">
         <v>23</v>
       </c>
       <c r="E3" s="9" t="s">
@@ -3360,9 +3360,9 @@
       <c r="DR3" s="23"/>
     </row>
     <row r="4" spans="2:122" ht="42" customHeight="1">
-      <c r="B4" s="28"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9" t="s">
         <v>4</v>
@@ -3539,9 +3539,9 @@
       <c r="DR4" s="23"/>
     </row>
     <row r="5" spans="2:122" ht="42" customHeight="1">
-      <c r="B5" s="28"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9" t="s">
@@ -3722,9 +3722,9 @@
       <c r="DR5" s="23"/>
     </row>
     <row r="6" spans="2:122" ht="42" customHeight="1">
-      <c r="B6" s="28"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
@@ -3892,9 +3892,9 @@
       <c r="DR6" s="23"/>
     </row>
     <row r="7" spans="2:122" ht="42" customHeight="1">
-      <c r="B7" s="28"/>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
@@ -4061,9 +4061,9 @@
       <c r="DR7" s="23"/>
     </row>
     <row r="8" spans="2:122" ht="42" customHeight="1">
-      <c r="B8" s="28"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
@@ -4231,13 +4231,13 @@
       <c r="DR8" s="23"/>
     </row>
     <row r="9" spans="2:122" ht="42" customHeight="1">
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="29">
-        <v>9</v>
-      </c>
-      <c r="D9" s="29">
+      <c r="C9" s="34">
+        <v>15</v>
+      </c>
+      <c r="D9" s="34">
         <v>4</v>
       </c>
       <c r="E9" s="9"/>
@@ -4418,9 +4418,9 @@
       <c r="DR9" s="23"/>
     </row>
     <row r="10" spans="2:122" ht="42" customHeight="1">
-      <c r="B10" s="28"/>
-      <c r="C10" s="29"/>
-      <c r="D10" s="29"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
@@ -4550,9 +4550,9 @@
       <c r="DR10" s="23"/>
     </row>
     <row r="11" spans="2:122" ht="42" customHeight="1">
-      <c r="B11" s="28"/>
-      <c r="C11" s="29"/>
-      <c r="D11" s="29"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
@@ -4684,9 +4684,9 @@
       <c r="DR11" s="23"/>
     </row>
     <row r="12" spans="2:122" ht="42" customHeight="1">
-      <c r="B12" s="28"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
@@ -4716,13 +4716,13 @@
       <c r="AE12" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="AF12" s="33" t="s">
+      <c r="AF12" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="AG12" s="33" t="s">
+      <c r="AG12" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="AH12" s="33" t="s">
+      <c r="AH12" s="29" t="s">
         <v>6</v>
       </c>
       <c r="AI12" s="18"/>
@@ -4815,9 +4815,9 @@
       <c r="DR12" s="23"/>
     </row>
     <row r="13" spans="2:122" ht="42" customHeight="1">
-      <c r="B13" s="28"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
@@ -4948,9 +4948,9 @@
       <c r="DR13" s="23"/>
     </row>
     <row r="14" spans="2:122" ht="42" customHeight="1">
-      <c r="B14" s="28"/>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
@@ -4982,13 +4982,13 @@
       <c r="AG14" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="AH14" s="33" t="s">
+      <c r="AH14" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="AI14" s="33" t="s">
+      <c r="AI14" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="AJ14" s="33" t="s">
+      <c r="AJ14" s="29" t="s">
         <v>8</v>
       </c>
       <c r="AK14" s="18"/>
@@ -5185,7 +5185,7 @@
       <c r="BC15" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="BD15" s="30" t="s">
+      <c r="BD15" s="26" t="s">
         <v>166</v>
       </c>
       <c r="BE15" s="1" t="s">
@@ -5303,22 +5303,22 @@
       <c r="CS15" s="9"/>
       <c r="CT15" s="9"/>
       <c r="CU15" s="9"/>
-      <c r="CV15" s="31" t="s">
+      <c r="CV15" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="CW15" s="31" t="s">
+      <c r="CW15" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="CX15" s="31" t="s">
+      <c r="CX15" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="CY15" s="31" t="s">
+      <c r="CY15" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="CZ15" s="32" t="s">
+      <c r="CZ15" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="DA15" s="32" t="s">
+      <c r="DA15" s="28" t="s">
         <v>104</v>
       </c>
       <c r="DB15" s="9"/>
@@ -5352,10 +5352,10 @@
       <c r="DL15" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="DM15" s="30" t="s">
+      <c r="DM15" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="DN15" s="30" t="s">
+      <c r="DN15" s="26" t="s">
         <v>123</v>
       </c>
       <c r="DO15" s="10"/>
@@ -5527,121 +5527,121 @@
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="26" t="s">
+      <c r="E18" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="26"/>
-      <c r="M18" s="26"/>
-      <c r="N18" s="26"/>
-      <c r="O18" s="26"/>
-      <c r="P18" s="26"/>
-      <c r="Q18" s="26"/>
-      <c r="R18" s="26"/>
-      <c r="S18" s="26"/>
-      <c r="T18" s="26"/>
-      <c r="U18" s="26"/>
-      <c r="V18" s="26"/>
-      <c r="W18" s="26"/>
-      <c r="X18" s="26"/>
-      <c r="Y18" s="26"/>
-      <c r="Z18" s="26"/>
-      <c r="AA18" s="26"/>
-      <c r="AB18" s="26"/>
-      <c r="AC18" s="26"/>
-      <c r="AD18" s="26"/>
-      <c r="AE18" s="26"/>
-      <c r="AF18" s="26"/>
-      <c r="AG18" s="26"/>
-      <c r="AH18" s="26"/>
-      <c r="AI18" s="26"/>
-      <c r="AJ18" s="26"/>
-      <c r="AK18" s="26"/>
-      <c r="AL18" s="26"/>
-      <c r="AM18" s="26"/>
-      <c r="AN18" s="26"/>
-      <c r="AO18" s="26"/>
-      <c r="AP18" s="26"/>
-      <c r="AQ18" s="26"/>
-      <c r="AR18" s="26"/>
-      <c r="AS18" s="26"/>
-      <c r="AT18" s="26"/>
-      <c r="AU18" s="26"/>
-      <c r="AV18" s="26"/>
-      <c r="AW18" s="26"/>
-      <c r="AX18" s="26"/>
-      <c r="AY18" s="26"/>
-      <c r="AZ18" s="26"/>
-      <c r="BA18" s="26"/>
-      <c r="BB18" s="26"/>
-      <c r="BC18" s="26"/>
-      <c r="BD18" s="26"/>
-      <c r="BE18" s="26"/>
-      <c r="BF18" s="26"/>
-      <c r="BG18" s="26"/>
-      <c r="BH18" s="26"/>
-      <c r="BI18" s="26"/>
-      <c r="BJ18" s="26"/>
-      <c r="BK18" s="26"/>
-      <c r="BL18" s="26"/>
-      <c r="BM18" s="26"/>
-      <c r="BN18" s="26"/>
-      <c r="BO18" s="26"/>
-      <c r="BP18" s="26"/>
-      <c r="BQ18" s="26"/>
-      <c r="BR18" s="26"/>
-      <c r="BS18" s="26"/>
-      <c r="BT18" s="26"/>
-      <c r="BU18" s="26"/>
-      <c r="BV18" s="26"/>
-      <c r="BW18" s="26"/>
-      <c r="BX18" s="26"/>
-      <c r="BY18" s="26"/>
-      <c r="BZ18" s="26"/>
-      <c r="CA18" s="26"/>
-      <c r="CB18" s="26"/>
-      <c r="CC18" s="26"/>
-      <c r="CD18" s="26"/>
-      <c r="CE18" s="26"/>
-      <c r="CF18" s="26"/>
-      <c r="CG18" s="26"/>
-      <c r="CH18" s="26"/>
-      <c r="CI18" s="26"/>
-      <c r="CJ18" s="26"/>
-      <c r="CK18" s="26"/>
-      <c r="CL18" s="26"/>
-      <c r="CM18" s="26"/>
-      <c r="CN18" s="26"/>
-      <c r="CO18" s="26"/>
-      <c r="CP18" s="26"/>
-      <c r="CQ18" s="26"/>
-      <c r="CR18" s="26"/>
-      <c r="CS18" s="26"/>
-      <c r="CT18" s="26"/>
-      <c r="CU18" s="26"/>
-      <c r="CV18" s="26"/>
-      <c r="CW18" s="26"/>
-      <c r="CX18" s="26"/>
-      <c r="CY18" s="26"/>
-      <c r="CZ18" s="26"/>
-      <c r="DA18" s="26"/>
-      <c r="DB18" s="26"/>
-      <c r="DC18" s="26"/>
-      <c r="DD18" s="26"/>
-      <c r="DE18" s="26"/>
-      <c r="DF18" s="26"/>
-      <c r="DG18" s="26"/>
-      <c r="DH18" s="26"/>
-      <c r="DI18" s="26"/>
-      <c r="DJ18" s="26"/>
-      <c r="DK18" s="26"/>
-      <c r="DL18" s="26"/>
-      <c r="DM18" s="27"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="31"/>
+      <c r="L18" s="31"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="31"/>
+      <c r="O18" s="31"/>
+      <c r="P18" s="31"/>
+      <c r="Q18" s="31"/>
+      <c r="R18" s="31"/>
+      <c r="S18" s="31"/>
+      <c r="T18" s="31"/>
+      <c r="U18" s="31"/>
+      <c r="V18" s="31"/>
+      <c r="W18" s="31"/>
+      <c r="X18" s="31"/>
+      <c r="Y18" s="31"/>
+      <c r="Z18" s="31"/>
+      <c r="AA18" s="31"/>
+      <c r="AB18" s="31"/>
+      <c r="AC18" s="31"/>
+      <c r="AD18" s="31"/>
+      <c r="AE18" s="31"/>
+      <c r="AF18" s="31"/>
+      <c r="AG18" s="31"/>
+      <c r="AH18" s="31"/>
+      <c r="AI18" s="31"/>
+      <c r="AJ18" s="31"/>
+      <c r="AK18" s="31"/>
+      <c r="AL18" s="31"/>
+      <c r="AM18" s="31"/>
+      <c r="AN18" s="31"/>
+      <c r="AO18" s="31"/>
+      <c r="AP18" s="31"/>
+      <c r="AQ18" s="31"/>
+      <c r="AR18" s="31"/>
+      <c r="AS18" s="31"/>
+      <c r="AT18" s="31"/>
+      <c r="AU18" s="31"/>
+      <c r="AV18" s="31"/>
+      <c r="AW18" s="31"/>
+      <c r="AX18" s="31"/>
+      <c r="AY18" s="31"/>
+      <c r="AZ18" s="31"/>
+      <c r="BA18" s="31"/>
+      <c r="BB18" s="31"/>
+      <c r="BC18" s="31"/>
+      <c r="BD18" s="31"/>
+      <c r="BE18" s="31"/>
+      <c r="BF18" s="31"/>
+      <c r="BG18" s="31"/>
+      <c r="BH18" s="31"/>
+      <c r="BI18" s="31"/>
+      <c r="BJ18" s="31"/>
+      <c r="BK18" s="31"/>
+      <c r="BL18" s="31"/>
+      <c r="BM18" s="31"/>
+      <c r="BN18" s="31"/>
+      <c r="BO18" s="31"/>
+      <c r="BP18" s="31"/>
+      <c r="BQ18" s="31"/>
+      <c r="BR18" s="31"/>
+      <c r="BS18" s="31"/>
+      <c r="BT18" s="31"/>
+      <c r="BU18" s="31"/>
+      <c r="BV18" s="31"/>
+      <c r="BW18" s="31"/>
+      <c r="BX18" s="31"/>
+      <c r="BY18" s="31"/>
+      <c r="BZ18" s="31"/>
+      <c r="CA18" s="31"/>
+      <c r="CB18" s="31"/>
+      <c r="CC18" s="31"/>
+      <c r="CD18" s="31"/>
+      <c r="CE18" s="31"/>
+      <c r="CF18" s="31"/>
+      <c r="CG18" s="31"/>
+      <c r="CH18" s="31"/>
+      <c r="CI18" s="31"/>
+      <c r="CJ18" s="31"/>
+      <c r="CK18" s="31"/>
+      <c r="CL18" s="31"/>
+      <c r="CM18" s="31"/>
+      <c r="CN18" s="31"/>
+      <c r="CO18" s="31"/>
+      <c r="CP18" s="31"/>
+      <c r="CQ18" s="31"/>
+      <c r="CR18" s="31"/>
+      <c r="CS18" s="31"/>
+      <c r="CT18" s="31"/>
+      <c r="CU18" s="31"/>
+      <c r="CV18" s="31"/>
+      <c r="CW18" s="31"/>
+      <c r="CX18" s="31"/>
+      <c r="CY18" s="31"/>
+      <c r="CZ18" s="31"/>
+      <c r="DA18" s="31"/>
+      <c r="DB18" s="31"/>
+      <c r="DC18" s="31"/>
+      <c r="DD18" s="31"/>
+      <c r="DE18" s="31"/>
+      <c r="DF18" s="31"/>
+      <c r="DG18" s="31"/>
+      <c r="DH18" s="31"/>
+      <c r="DI18" s="31"/>
+      <c r="DJ18" s="31"/>
+      <c r="DK18" s="31"/>
+      <c r="DL18" s="31"/>
+      <c r="DM18" s="32"/>
     </row>
     <row r="19" spans="2:117" s="2" customFormat="1" ht="42" customHeight="1">
       <c r="B19" s="20" t="s">
@@ -6111,7 +6111,7 @@
         <v>2</v>
       </c>
       <c r="C20" s="6">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="D20" s="6">
         <v>4</v>
@@ -6314,7 +6314,7 @@
       <c r="DL20" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="DM20" s="34" t="s">
+      <c r="DM20" s="30" t="s">
         <v>100</v>
       </c>
     </row>
@@ -7054,6 +7054,7 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="E1:DO1"/>
     <mergeCell ref="E18:DM18"/>
     <mergeCell ref="B3:B8"/>
     <mergeCell ref="C3:C8"/>
@@ -7061,7 +7062,6 @@
     <mergeCell ref="B9:B14"/>
     <mergeCell ref="C9:C14"/>
     <mergeCell ref="D9:D14"/>
-    <mergeCell ref="E1:DO1"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Jacobian block now passes individual validatioJacobian block now passes individual validationn
</commit_message>
<xml_diff>
--- a/doc/design/schedule.xlsx
+++ b/doc/design/schedule.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="165">
   <si>
     <t>sincos</t>
   </si>
@@ -219,9 +219,6 @@
     <t>T05 x Z0</t>
   </si>
   <si>
-    <t>T06 x Z0</t>
-  </si>
-  <si>
     <t>JJT cyc 1</t>
   </si>
   <si>
@@ -382,9 +379,6 @@
   </si>
   <si>
     <t>T05 x Z0 accum</t>
-  </si>
-  <si>
-    <t>T06 x Z0 accum</t>
   </si>
   <si>
     <t>JJT cyc 11</t>
@@ -728,7 +722,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="691">
+  <cellStyleXfs count="781">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1420,8 +1414,98 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1492,12 +1576,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1525,8 +1603,23 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="691">
+  <cellStyles count="781">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1872,6 +1965,51 @@
     <cellStyle name="Followed Hyperlink" xfId="686" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="688" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="690" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="692" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="694" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="696" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="698" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="700" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="702" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="704" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="706" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="708" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="710" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="712" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="714" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="716" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="718" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="720" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="722" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="724" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="726" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="728" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="730" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="732" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="734" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="736" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="738" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="740" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="742" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="744" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="746" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="748" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="750" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="752" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="754" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="756" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="758" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="760" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="762" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="764" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="766" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="768" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="770" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="772" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="774" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="776" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="778" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="780" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2217,6 +2355,51 @@
     <cellStyle name="Hyperlink" xfId="685" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="687" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="689" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="691" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="693" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="695" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="697" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="699" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="701" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="703" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="705" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="707" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="709" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="711" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="713" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="715" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="717" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="719" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="721" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="723" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="725" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="727" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="729" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="731" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="733" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="735" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="737" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="739" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="741" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="743" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="745" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="747" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="749" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="751" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="753" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="755" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="757" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="759" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="761" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="763" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="765" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="767" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="769" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="771" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="773" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="775" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="777" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="779" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2549,628 +2732,610 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:DR24"/>
+  <dimension ref="A1:DM24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="50" workbookViewId="0">
       <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="AL1" sqref="AL1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.1640625" defaultRowHeight="42" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.33203125" style="8" customWidth="1"/>
     <col min="2" max="4" width="10.33203125" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="4.1640625" style="11"/>
+    <col min="5" max="5" width="4.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="4.1640625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:122" s="2" customFormat="1" ht="42" customHeight="1">
+    <row r="1" spans="2:117" s="2" customFormat="1" ht="42" customHeight="1">
       <c r="B1" s="3"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
-      <c r="E1" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31"/>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31"/>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31"/>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="31"/>
-      <c r="AJ1" s="31"/>
-      <c r="AK1" s="31"/>
-      <c r="AL1" s="31"/>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="31"/>
-      <c r="AO1" s="31"/>
-      <c r="AP1" s="31"/>
-      <c r="AQ1" s="31"/>
-      <c r="AR1" s="31"/>
-      <c r="AS1" s="31"/>
-      <c r="AT1" s="31"/>
-      <c r="AU1" s="31"/>
-      <c r="AV1" s="31"/>
-      <c r="AW1" s="31"/>
-      <c r="AX1" s="31"/>
-      <c r="AY1" s="31"/>
-      <c r="AZ1" s="31"/>
-      <c r="BA1" s="31"/>
-      <c r="BB1" s="31"/>
-      <c r="BC1" s="31"/>
-      <c r="BD1" s="31"/>
-      <c r="BE1" s="31"/>
-      <c r="BF1" s="31"/>
-      <c r="BG1" s="31"/>
-      <c r="BH1" s="31"/>
-      <c r="BI1" s="31"/>
-      <c r="BJ1" s="31"/>
-      <c r="BK1" s="31"/>
-      <c r="BL1" s="31"/>
-      <c r="BM1" s="31"/>
-      <c r="BN1" s="31"/>
-      <c r="BO1" s="31"/>
-      <c r="BP1" s="31"/>
-      <c r="BQ1" s="31"/>
-      <c r="BR1" s="31"/>
-      <c r="BS1" s="31"/>
-      <c r="BT1" s="31"/>
-      <c r="BU1" s="31"/>
-      <c r="BV1" s="31"/>
-      <c r="BW1" s="31"/>
-      <c r="BX1" s="31"/>
-      <c r="BY1" s="31"/>
-      <c r="BZ1" s="31"/>
-      <c r="CA1" s="31"/>
-      <c r="CB1" s="31"/>
-      <c r="CC1" s="31"/>
-      <c r="CD1" s="31"/>
-      <c r="CE1" s="31"/>
-      <c r="CF1" s="31"/>
-      <c r="CG1" s="31"/>
-      <c r="CH1" s="31"/>
-      <c r="CI1" s="31"/>
-      <c r="CJ1" s="31"/>
-      <c r="CK1" s="31"/>
-      <c r="CL1" s="31"/>
-      <c r="CM1" s="31"/>
-      <c r="CN1" s="31"/>
-      <c r="CO1" s="31"/>
-      <c r="CP1" s="31"/>
-      <c r="CQ1" s="31"/>
-      <c r="CR1" s="31"/>
-      <c r="CS1" s="31"/>
-      <c r="CT1" s="31"/>
-      <c r="CU1" s="31"/>
-      <c r="CV1" s="31"/>
-      <c r="CW1" s="31"/>
-      <c r="CX1" s="31"/>
-      <c r="CY1" s="31"/>
-      <c r="CZ1" s="31"/>
-      <c r="DA1" s="31"/>
-      <c r="DB1" s="31"/>
-      <c r="DC1" s="31"/>
-      <c r="DD1" s="31"/>
-      <c r="DE1" s="31"/>
-      <c r="DF1" s="31"/>
-      <c r="DG1" s="31"/>
-      <c r="DH1" s="31"/>
-      <c r="DI1" s="31"/>
-      <c r="DJ1" s="31"/>
-      <c r="DK1" s="31"/>
-      <c r="DL1" s="31"/>
-      <c r="DM1" s="31"/>
-      <c r="DN1" s="31"/>
-      <c r="DO1" s="32"/>
-      <c r="DP1" s="22"/>
-      <c r="DQ1" s="22"/>
-      <c r="DR1" s="22"/>
+      <c r="E1" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
+      <c r="AC1" s="29"/>
+      <c r="AD1" s="29"/>
+      <c r="AE1" s="29"/>
+      <c r="AF1" s="29"/>
+      <c r="AG1" s="29"/>
+      <c r="AH1" s="29"/>
+      <c r="AI1" s="29"/>
+      <c r="AJ1" s="29"/>
+      <c r="AK1" s="29"/>
+      <c r="AL1" s="29"/>
+      <c r="AM1" s="29"/>
+      <c r="AN1" s="29"/>
+      <c r="AO1" s="29"/>
+      <c r="AP1" s="29"/>
+      <c r="AQ1" s="29"/>
+      <c r="AR1" s="29"/>
+      <c r="AS1" s="29"/>
+      <c r="AT1" s="29"/>
+      <c r="AU1" s="29"/>
+      <c r="AV1" s="29"/>
+      <c r="AW1" s="29"/>
+      <c r="AX1" s="29"/>
+      <c r="AY1" s="29"/>
+      <c r="AZ1" s="29"/>
+      <c r="BA1" s="29"/>
+      <c r="BB1" s="29"/>
+      <c r="BC1" s="29"/>
+      <c r="BD1" s="29"/>
+      <c r="BE1" s="29"/>
+      <c r="BF1" s="29"/>
+      <c r="BG1" s="29"/>
+      <c r="BH1" s="29"/>
+      <c r="BI1" s="29"/>
+      <c r="BJ1" s="29"/>
+      <c r="BK1" s="29"/>
+      <c r="BL1" s="29"/>
+      <c r="BM1" s="29"/>
+      <c r="BN1" s="29"/>
+      <c r="BO1" s="29"/>
+      <c r="BP1" s="29"/>
+      <c r="BQ1" s="29"/>
+      <c r="BR1" s="29"/>
+      <c r="BS1" s="29"/>
+      <c r="BT1" s="29"/>
+      <c r="BU1" s="29"/>
+      <c r="BV1" s="29"/>
+      <c r="BW1" s="29"/>
+      <c r="BX1" s="29"/>
+      <c r="BY1" s="29"/>
+      <c r="BZ1" s="29"/>
+      <c r="CA1" s="29"/>
+      <c r="CB1" s="29"/>
+      <c r="CC1" s="29"/>
+      <c r="CD1" s="29"/>
+      <c r="CE1" s="29"/>
+      <c r="CF1" s="29"/>
+      <c r="CG1" s="29"/>
+      <c r="CH1" s="29"/>
+      <c r="CI1" s="29"/>
+      <c r="CJ1" s="29"/>
+      <c r="CK1" s="29"/>
+      <c r="CL1" s="29"/>
+      <c r="CM1" s="29"/>
+      <c r="CN1" s="29"/>
+      <c r="CO1" s="29"/>
+      <c r="CP1" s="29"/>
+      <c r="CQ1" s="29"/>
+      <c r="CR1" s="29"/>
+      <c r="CS1" s="29"/>
+      <c r="CT1" s="29"/>
+      <c r="CU1" s="29"/>
+      <c r="CV1" s="29"/>
+      <c r="CW1" s="29"/>
+      <c r="CX1" s="29"/>
+      <c r="CY1" s="29"/>
+      <c r="CZ1" s="29"/>
+      <c r="DA1" s="29"/>
+      <c r="DB1" s="29"/>
+      <c r="DC1" s="29"/>
+      <c r="DD1" s="29"/>
+      <c r="DE1" s="29"/>
+      <c r="DF1" s="29"/>
+      <c r="DG1" s="29"/>
+      <c r="DH1" s="29"/>
+      <c r="DI1" s="29"/>
+      <c r="DJ1" s="29"/>
+      <c r="DK1" s="29"/>
+      <c r="DL1" s="30"/>
+      <c r="DM1" s="37"/>
     </row>
-    <row r="2" spans="2:122" s="2" customFormat="1" ht="42" customHeight="1">
-      <c r="B2" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="C2" s="25" t="s">
+    <row r="2" spans="2:117" s="2" customFormat="1" ht="42" customHeight="1">
+      <c r="B2" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="25">
+      <c r="E2" s="32">
         <v>1</v>
       </c>
-      <c r="F2" s="25">
+      <c r="F2" s="32">
         <f>E2+1</f>
         <v>2</v>
       </c>
-      <c r="G2" s="25">
+      <c r="G2" s="32">
         <f t="shared" ref="G2:BR2" si="0">F2+1</f>
         <v>3</v>
       </c>
-      <c r="H2" s="25">
+      <c r="H2" s="32">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="I2" s="25">
+      <c r="I2" s="32">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="J2" s="25">
+      <c r="J2" s="32">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="K2" s="25">
+      <c r="K2" s="32">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="L2" s="25">
+      <c r="L2" s="32">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="M2" s="25">
+      <c r="M2" s="32">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="N2" s="25">
+      <c r="N2" s="32">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="O2" s="25">
+      <c r="O2" s="32">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="P2" s="25">
+      <c r="P2" s="32">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="Q2" s="25">
+      <c r="Q2" s="32">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="R2" s="25">
+      <c r="R2" s="32">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="S2" s="25">
+      <c r="S2" s="32">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="T2" s="25">
+      <c r="T2" s="32">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="U2" s="25">
+      <c r="U2" s="32">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="V2" s="25">
+      <c r="V2" s="32">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="W2" s="25">
+      <c r="W2" s="32">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="X2" s="25">
+      <c r="X2" s="32">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="Y2" s="25">
+      <c r="Y2" s="32">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="Z2" s="25">
+      <c r="Z2" s="32">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="AA2" s="25">
+      <c r="AA2" s="32">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="AB2" s="25">
+      <c r="AB2" s="32">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AC2" s="25">
+      <c r="AC2" s="32">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="AD2" s="25">
+      <c r="AD2" s="32">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="AE2" s="25">
+      <c r="AE2" s="32">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="AF2" s="25">
+      <c r="AF2" s="32">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="AG2" s="25">
+      <c r="AG2" s="32">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="AH2" s="25">
+      <c r="AH2" s="32">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="AI2" s="25">
+      <c r="AI2" s="32">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="AJ2" s="25">
+      <c r="AJ2" s="32">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="AK2" s="25">
+      <c r="AK2" s="32">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="AL2" s="25">
+      <c r="AL2" s="32">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="AM2" s="25">
+      <c r="AM2" s="32">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="AN2" s="25">
+      <c r="AN2" s="32">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="AO2" s="25">
+      <c r="AO2" s="32">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="AP2" s="25">
+      <c r="AP2" s="32">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="AQ2" s="25">
+      <c r="AQ2" s="32">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="AR2" s="25">
+      <c r="AR2" s="32">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="AS2" s="25">
+      <c r="AS2" s="32">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="AT2" s="25">
+      <c r="AT2" s="32">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="AU2" s="25">
+      <c r="AU2" s="32">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="AV2" s="25">
+      <c r="AV2" s="32">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="AW2" s="25">
+      <c r="AW2" s="32">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="AX2" s="25">
+      <c r="AX2" s="32">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="AY2" s="25">
+      <c r="AY2" s="32">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="AZ2" s="25">
+      <c r="AZ2" s="32">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="BA2" s="25">
+      <c r="BA2" s="32">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="BB2" s="25">
+      <c r="BB2" s="32">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="BC2" s="25">
+      <c r="BC2" s="32">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="BD2" s="25">
+      <c r="BD2" s="32">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="BE2" s="25">
+      <c r="BE2" s="32">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="BF2" s="25">
+      <c r="BF2" s="32">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="BG2" s="25">
+      <c r="BG2" s="32">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="BH2" s="25">
+      <c r="BH2" s="32">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="BI2" s="25">
+      <c r="BI2" s="32">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-      <c r="BJ2" s="25">
+      <c r="BJ2" s="32">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="BK2" s="25">
+      <c r="BK2" s="32">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="BL2" s="25">
+      <c r="BL2" s="32">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="BM2" s="25">
+      <c r="BM2" s="32">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="BN2" s="25">
+      <c r="BN2" s="32">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="BO2" s="25">
+      <c r="BO2" s="32">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="BP2" s="25">
+      <c r="BP2" s="32">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="BQ2" s="25">
+      <c r="BQ2" s="32">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-      <c r="BR2" s="25">
+      <c r="BR2" s="32">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="BS2" s="25">
+      <c r="BS2" s="32">
         <f t="shared" ref="BS2:BZ2" si="1">BR2+1</f>
         <v>67</v>
       </c>
-      <c r="BT2" s="25">
+      <c r="BT2" s="32">
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
-      <c r="BU2" s="25">
+      <c r="BU2" s="32">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-      <c r="BV2" s="25">
+      <c r="BV2" s="32">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
-      <c r="BW2" s="25">
+      <c r="BW2" s="32">
         <f t="shared" si="1"/>
         <v>71</v>
       </c>
-      <c r="BX2" s="25">
+      <c r="BX2" s="32">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
-      <c r="BY2" s="25">
+      <c r="BY2" s="32">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
-      <c r="BZ2" s="25">
+      <c r="BZ2" s="32">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
-      <c r="CA2" s="25">
+      <c r="CA2" s="32">
         <f t="shared" ref="CA2" si="2">BZ2+1</f>
         <v>75</v>
       </c>
-      <c r="CB2" s="25">
+      <c r="CB2" s="32">
         <f t="shared" ref="CB2" si="3">CA2+1</f>
         <v>76</v>
       </c>
-      <c r="CC2" s="25">
+      <c r="CC2" s="32">
         <f t="shared" ref="CC2" si="4">CB2+1</f>
         <v>77</v>
       </c>
-      <c r="CD2" s="25">
+      <c r="CD2" s="32">
         <f t="shared" ref="CD2" si="5">CC2+1</f>
         <v>78</v>
       </c>
-      <c r="CE2" s="25">
+      <c r="CE2" s="32">
         <f t="shared" ref="CE2" si="6">CD2+1</f>
         <v>79</v>
       </c>
-      <c r="CF2" s="25">
+      <c r="CF2" s="32">
         <f t="shared" ref="CF2" si="7">CE2+1</f>
         <v>80</v>
       </c>
-      <c r="CG2" s="25">
+      <c r="CG2" s="32">
         <f t="shared" ref="CG2" si="8">CF2+1</f>
         <v>81</v>
       </c>
-      <c r="CH2" s="25">
+      <c r="CH2" s="32">
         <f t="shared" ref="CH2" si="9">CG2+1</f>
         <v>82</v>
       </c>
-      <c r="CI2" s="25">
+      <c r="CI2" s="32">
         <f t="shared" ref="CI2" si="10">CH2+1</f>
         <v>83</v>
       </c>
-      <c r="CJ2" s="25">
+      <c r="CJ2" s="32">
         <f t="shared" ref="CJ2" si="11">CI2+1</f>
         <v>84</v>
       </c>
-      <c r="CK2" s="25">
+      <c r="CK2" s="32">
         <f t="shared" ref="CK2" si="12">CJ2+1</f>
         <v>85</v>
       </c>
-      <c r="CL2" s="25">
+      <c r="CL2" s="32">
         <f t="shared" ref="CL2" si="13">CK2+1</f>
         <v>86</v>
       </c>
-      <c r="CM2" s="25">
+      <c r="CM2" s="32">
         <f t="shared" ref="CM2" si="14">CL2+1</f>
         <v>87</v>
       </c>
-      <c r="CN2" s="25">
+      <c r="CN2" s="32">
         <f t="shared" ref="CN2" si="15">CM2+1</f>
         <v>88</v>
       </c>
-      <c r="CO2" s="25">
+      <c r="CO2" s="32">
         <f t="shared" ref="CO2" si="16">CN2+1</f>
         <v>89</v>
       </c>
-      <c r="CP2" s="25">
+      <c r="CP2" s="32">
         <f t="shared" ref="CP2" si="17">CO2+1</f>
         <v>90</v>
       </c>
-      <c r="CQ2" s="25">
+      <c r="CQ2" s="32">
         <f t="shared" ref="CQ2" si="18">CP2+1</f>
         <v>91</v>
       </c>
-      <c r="CR2" s="25">
+      <c r="CR2" s="32">
         <f t="shared" ref="CR2" si="19">CQ2+1</f>
         <v>92</v>
       </c>
-      <c r="CS2" s="25">
+      <c r="CS2" s="32">
         <f t="shared" ref="CS2" si="20">CR2+1</f>
         <v>93</v>
       </c>
-      <c r="CT2" s="25">
+      <c r="CT2" s="32">
         <f t="shared" ref="CT2" si="21">CS2+1</f>
         <v>94</v>
       </c>
-      <c r="CU2" s="25">
+      <c r="CU2" s="32">
         <f t="shared" ref="CU2" si="22">CT2+1</f>
         <v>95</v>
       </c>
-      <c r="CV2" s="25">
+      <c r="CV2" s="32">
         <f t="shared" ref="CV2" si="23">CU2+1</f>
         <v>96</v>
       </c>
-      <c r="CW2" s="25">
+      <c r="CW2" s="32">
         <f t="shared" ref="CW2" si="24">CV2+1</f>
         <v>97</v>
       </c>
-      <c r="CX2" s="25">
+      <c r="CX2" s="32">
         <f t="shared" ref="CX2" si="25">CW2+1</f>
         <v>98</v>
       </c>
-      <c r="CY2" s="25">
+      <c r="CY2" s="32">
         <f t="shared" ref="CY2" si="26">CX2+1</f>
         <v>99</v>
       </c>
-      <c r="CZ2" s="25">
+      <c r="CZ2" s="32">
         <f t="shared" ref="CZ2" si="27">CY2+1</f>
         <v>100</v>
       </c>
-      <c r="DA2" s="25">
+      <c r="DA2" s="32">
         <f t="shared" ref="DA2" si="28">CZ2+1</f>
         <v>101</v>
       </c>
-      <c r="DB2" s="25">
+      <c r="DB2" s="32">
         <f t="shared" ref="DB2" si="29">DA2+1</f>
         <v>102</v>
       </c>
-      <c r="DC2" s="25">
+      <c r="DC2" s="32">
         <f t="shared" ref="DC2" si="30">DB2+1</f>
         <v>103</v>
       </c>
-      <c r="DD2" s="25">
+      <c r="DD2" s="32">
         <f t="shared" ref="DD2" si="31">DC2+1</f>
         <v>104</v>
       </c>
-      <c r="DE2" s="25">
+      <c r="DE2" s="32">
         <f t="shared" ref="DE2" si="32">DD2+1</f>
         <v>105</v>
       </c>
-      <c r="DF2" s="25">
+      <c r="DF2" s="32">
         <f t="shared" ref="DF2" si="33">DE2+1</f>
         <v>106</v>
       </c>
-      <c r="DG2" s="25">
+      <c r="DG2" s="32">
         <f t="shared" ref="DG2" si="34">DF2+1</f>
         <v>107</v>
       </c>
-      <c r="DH2" s="25">
+      <c r="DH2" s="32">
         <f t="shared" ref="DH2" si="35">DG2+1</f>
         <v>108</v>
       </c>
-      <c r="DI2" s="25">
+      <c r="DI2" s="32">
         <f t="shared" ref="DI2" si="36">DH2+1</f>
         <v>109</v>
       </c>
-      <c r="DJ2" s="25">
+      <c r="DJ2" s="32">
         <f t="shared" ref="DJ2" si="37">DI2+1</f>
         <v>110</v>
       </c>
-      <c r="DK2" s="25">
+      <c r="DK2" s="32">
         <f t="shared" ref="DK2" si="38">DJ2+1</f>
         <v>111</v>
       </c>
-      <c r="DL2" s="25">
+      <c r="DL2" s="7">
         <f t="shared" ref="DL2" si="39">DK2+1</f>
         <v>112</v>
       </c>
-      <c r="DM2" s="25">
-        <f t="shared" ref="DM2" si="40">DL2+1</f>
-        <v>113</v>
-      </c>
-      <c r="DN2" s="25">
-        <f t="shared" ref="DN2" si="41">DM2+1</f>
-        <v>114</v>
-      </c>
-      <c r="DO2" s="7">
-        <f t="shared" ref="DO2" si="42">DN2+1</f>
-        <v>115</v>
-      </c>
-      <c r="DP2" s="22"/>
-      <c r="DQ2" s="22"/>
-      <c r="DR2" s="22"/>
+      <c r="DM2" s="22"/>
     </row>
-    <row r="3" spans="2:122" ht="42" customHeight="1">
-      <c r="B3" s="33" t="s">
+    <row r="3" spans="2:117" ht="42" customHeight="1">
+      <c r="B3" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="34">
+      <c r="C3" s="36">
         <v>2</v>
       </c>
-      <c r="D3" s="34">
+      <c r="D3" s="36">
         <v>23</v>
       </c>
       <c r="E3" s="9" t="s">
@@ -3181,23 +3346,23 @@
         <v>joint 1</v>
       </c>
       <c r="G3" s="9" t="str">
-        <f t="shared" ref="G3:K3" si="43">F3</f>
+        <f t="shared" ref="G3:K3" si="40">F3</f>
         <v>joint 1</v>
       </c>
       <c r="H3" s="9" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="40"/>
         <v>joint 1</v>
       </c>
       <c r="I3" s="9" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="40"/>
         <v>joint 1</v>
       </c>
       <c r="J3" s="9" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="40"/>
         <v>joint 1</v>
       </c>
       <c r="K3" s="9" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="40"/>
         <v>joint 1</v>
       </c>
       <c r="L3" s="9" t="s">
@@ -3208,59 +3373,59 @@
         <v>joint 1</v>
       </c>
       <c r="N3" s="9" t="str">
-        <f t="shared" ref="N3" si="44">M3</f>
+        <f t="shared" ref="N3" si="41">M3</f>
         <v>joint 1</v>
       </c>
       <c r="O3" s="9" t="str">
-        <f t="shared" ref="O3" si="45">N3</f>
+        <f t="shared" ref="O3" si="42">N3</f>
         <v>joint 1</v>
       </c>
       <c r="P3" s="9" t="str">
-        <f t="shared" ref="P3" si="46">O3</f>
+        <f t="shared" ref="P3" si="43">O3</f>
         <v>joint 1</v>
       </c>
       <c r="Q3" s="9" t="str">
-        <f t="shared" ref="Q3" si="47">P3</f>
+        <f t="shared" ref="Q3" si="44">P3</f>
         <v>joint 1</v>
       </c>
       <c r="R3" s="9" t="str">
-        <f t="shared" ref="R3" si="48">Q3</f>
+        <f t="shared" ref="R3" si="45">Q3</f>
         <v>joint 1</v>
       </c>
       <c r="S3" s="9" t="str">
-        <f t="shared" ref="S3" si="49">R3</f>
+        <f t="shared" ref="S3" si="46">R3</f>
         <v>joint 1</v>
       </c>
       <c r="T3" s="9" t="str">
-        <f t="shared" ref="T3" si="50">S3</f>
+        <f t="shared" ref="T3" si="47">S3</f>
         <v>joint 1</v>
       </c>
       <c r="U3" s="9" t="str">
-        <f t="shared" ref="U3" si="51">T3</f>
+        <f t="shared" ref="U3" si="48">T3</f>
         <v>joint 1</v>
       </c>
       <c r="V3" s="9" t="str">
-        <f t="shared" ref="V3" si="52">U3</f>
+        <f t="shared" ref="V3" si="49">U3</f>
         <v>joint 1</v>
       </c>
       <c r="W3" s="9" t="str">
-        <f t="shared" ref="W3" si="53">V3</f>
+        <f t="shared" ref="W3" si="50">V3</f>
         <v>joint 1</v>
       </c>
       <c r="X3" s="9" t="str">
-        <f t="shared" ref="X3" si="54">W3</f>
+        <f t="shared" ref="X3" si="51">W3</f>
         <v>joint 1</v>
       </c>
       <c r="Y3" s="9" t="str">
-        <f t="shared" ref="Y3" si="55">X3</f>
+        <f t="shared" ref="Y3" si="52">X3</f>
         <v>joint 1</v>
       </c>
       <c r="Z3" s="9" t="str">
-        <f t="shared" ref="Z3:AA3" si="56">Y3</f>
+        <f t="shared" ref="Z3:AA3" si="53">Y3</f>
         <v>joint 1</v>
       </c>
       <c r="AA3" s="9" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="53"/>
         <v>joint 1</v>
       </c>
       <c r="AB3" s="9"/>
@@ -3351,44 +3516,39 @@
       <c r="DI3" s="9"/>
       <c r="DJ3" s="9"/>
       <c r="DK3" s="9"/>
-      <c r="DL3" s="9"/>
-      <c r="DM3" s="9"/>
-      <c r="DN3" s="9"/>
-      <c r="DO3" s="10"/>
-      <c r="DP3" s="23"/>
-      <c r="DQ3" s="23"/>
-      <c r="DR3" s="23"/>
+      <c r="DL3" s="10"/>
+      <c r="DM3" s="23"/>
     </row>
-    <row r="4" spans="2:122" ht="42" customHeight="1">
-      <c r="B4" s="33"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
+    <row r="4" spans="2:117" ht="42" customHeight="1">
+      <c r="B4" s="35"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9" t="s">
         <v>4</v>
       </c>
       <c r="G4" s="9" t="str">
-        <f t="shared" ref="G4:L4" si="57">F4</f>
+        <f t="shared" ref="G4:L4" si="54">F4</f>
         <v>joint 2</v>
       </c>
       <c r="H4" s="9" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="54"/>
         <v>joint 2</v>
       </c>
       <c r="I4" s="9" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="54"/>
         <v>joint 2</v>
       </c>
       <c r="J4" s="9" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="54"/>
         <v>joint 2</v>
       </c>
       <c r="K4" s="9" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="54"/>
         <v>joint 2</v>
       </c>
       <c r="L4" s="9" t="str">
-        <f t="shared" si="57"/>
+        <f t="shared" si="54"/>
         <v>joint 2</v>
       </c>
       <c r="M4" s="9" t="str">
@@ -3396,15 +3556,15 @@
         <v>joint 2</v>
       </c>
       <c r="N4" s="9" t="str">
-        <f t="shared" ref="N4:P5" si="58">M4</f>
+        <f t="shared" ref="N4:P5" si="55">M4</f>
         <v>joint 2</v>
       </c>
       <c r="O4" s="9" t="str">
-        <f t="shared" si="58"/>
+        <f t="shared" si="55"/>
         <v>joint 2</v>
       </c>
       <c r="P4" s="9" t="str">
-        <f t="shared" si="58"/>
+        <f t="shared" si="55"/>
         <v>joint 2</v>
       </c>
       <c r="Q4" s="9" t="s">
@@ -3530,18 +3690,13 @@
       <c r="DI4" s="9"/>
       <c r="DJ4" s="9"/>
       <c r="DK4" s="9"/>
-      <c r="DL4" s="9"/>
-      <c r="DM4" s="9"/>
-      <c r="DN4" s="9"/>
-      <c r="DO4" s="10"/>
-      <c r="DP4" s="23"/>
-      <c r="DQ4" s="23"/>
-      <c r="DR4" s="23"/>
+      <c r="DL4" s="10"/>
+      <c r="DM4" s="23"/>
     </row>
-    <row r="5" spans="2:122" ht="42" customHeight="1">
-      <c r="B5" s="33"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
+    <row r="5" spans="2:117" ht="42" customHeight="1">
+      <c r="B5" s="35"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="9" t="s">
@@ -3572,15 +3727,15 @@
         <v>joint 3</v>
       </c>
       <c r="N5" s="9" t="str">
-        <f t="shared" si="58"/>
+        <f t="shared" si="55"/>
         <v>joint 3</v>
       </c>
       <c r="O5" s="9" t="str">
-        <f t="shared" si="58"/>
+        <f t="shared" si="55"/>
         <v>joint 3</v>
       </c>
       <c r="P5" s="9" t="str">
-        <f t="shared" si="58"/>
+        <f t="shared" si="55"/>
         <v>joint 3</v>
       </c>
       <c r="Q5" s="9" t="str">
@@ -3713,18 +3868,13 @@
       <c r="DI5" s="9"/>
       <c r="DJ5" s="9"/>
       <c r="DK5" s="9"/>
-      <c r="DL5" s="9"/>
-      <c r="DM5" s="9"/>
-      <c r="DN5" s="9"/>
-      <c r="DO5" s="10"/>
-      <c r="DP5" s="23"/>
-      <c r="DQ5" s="23"/>
-      <c r="DR5" s="23"/>
+      <c r="DL5" s="10"/>
+      <c r="DM5" s="23"/>
     </row>
-    <row r="6" spans="2:122" ht="42" customHeight="1">
-      <c r="B6" s="33"/>
-      <c r="C6" s="34"/>
-      <c r="D6" s="34"/>
+    <row r="6" spans="2:117" ht="42" customHeight="1">
+      <c r="B6" s="35"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
       <c r="E6" s="9"/>
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
@@ -3883,18 +4033,13 @@
       <c r="DI6" s="9"/>
       <c r="DJ6" s="9"/>
       <c r="DK6" s="9"/>
-      <c r="DL6" s="9"/>
-      <c r="DM6" s="9"/>
-      <c r="DN6" s="9"/>
-      <c r="DO6" s="10"/>
-      <c r="DP6" s="23"/>
-      <c r="DQ6" s="23"/>
-      <c r="DR6" s="23"/>
+      <c r="DL6" s="10"/>
+      <c r="DM6" s="23"/>
     </row>
-    <row r="7" spans="2:122" ht="42" customHeight="1">
-      <c r="B7" s="33"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="34"/>
+    <row r="7" spans="2:117" ht="42" customHeight="1">
+      <c r="B7" s="35"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
@@ -4052,18 +4197,13 @@
       <c r="DI7" s="9"/>
       <c r="DJ7" s="9"/>
       <c r="DK7" s="9"/>
-      <c r="DL7" s="9"/>
-      <c r="DM7" s="9"/>
-      <c r="DN7" s="9"/>
-      <c r="DO7" s="10"/>
-      <c r="DP7" s="23"/>
-      <c r="DQ7" s="23"/>
-      <c r="DR7" s="23"/>
+      <c r="DL7" s="10"/>
+      <c r="DM7" s="23"/>
     </row>
-    <row r="8" spans="2:122" ht="42" customHeight="1">
-      <c r="B8" s="33"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
+    <row r="8" spans="2:117" ht="42" customHeight="1">
+      <c r="B8" s="35"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
       <c r="E8" s="9"/>
       <c r="F8" s="9"/>
       <c r="G8" s="9"/>
@@ -4222,22 +4362,17 @@
       <c r="DI8" s="9"/>
       <c r="DJ8" s="9"/>
       <c r="DK8" s="9"/>
-      <c r="DL8" s="9"/>
-      <c r="DM8" s="9"/>
-      <c r="DN8" s="9"/>
-      <c r="DO8" s="10"/>
-      <c r="DP8" s="23"/>
-      <c r="DQ8" s="23"/>
-      <c r="DR8" s="23"/>
+      <c r="DL8" s="10"/>
+      <c r="DM8" s="23"/>
     </row>
-    <row r="9" spans="2:122" ht="42" customHeight="1">
-      <c r="B9" s="33" t="s">
+    <row r="9" spans="2:117" ht="42" customHeight="1">
+      <c r="B9" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="34">
+      <c r="C9" s="36">
         <v>15</v>
       </c>
-      <c r="D9" s="34">
+      <c r="D9" s="36">
         <v>4</v>
       </c>
       <c r="E9" s="9"/>
@@ -4266,18 +4401,20 @@
       <c r="AB9" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="AC9" s="18" t="str">
-        <f>AB9</f>
-        <v>joint 1</v>
+      <c r="AC9" s="18" t="s">
+        <v>3</v>
       </c>
       <c r="AD9" s="18" t="str">
         <f>AC9</f>
         <v>joint 1</v>
       </c>
-      <c r="AE9" s="18" t="s">
+      <c r="AE9" s="18" t="str">
+        <f>AD9</f>
+        <v>joint 1</v>
+      </c>
+      <c r="AF9" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="AF9" s="18"/>
       <c r="AG9" s="18"/>
       <c r="AH9" s="18" t="s">
         <v>61</v>
@@ -4291,105 +4428,107 @@
       <c r="AK9" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="AL9" s="18"/>
+      <c r="AL9" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="AM9" s="18"/>
       <c r="AN9" s="18"/>
       <c r="AO9" s="18"/>
       <c r="AP9" s="18"/>
       <c r="AQ9" s="18"/>
       <c r="AR9" s="18"/>
-      <c r="AS9" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="AT9" s="18" t="s">
-        <v>62</v>
-      </c>
+      <c r="AS9" s="18"/>
+      <c r="AT9" s="18"/>
       <c r="AU9" s="18" t="s">
         <v>62</v>
       </c>
       <c r="AV9" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="AW9" s="18"/>
-      <c r="AX9" s="18"/>
-      <c r="AY9" s="18"/>
+      <c r="AW9" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="AX9" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="AY9" s="18" t="s">
+        <v>62</v>
+      </c>
       <c r="AZ9" s="18"/>
       <c r="BA9" s="18"/>
       <c r="BB9" s="18"/>
       <c r="BC9" s="18"/>
       <c r="BD9" s="18"/>
-      <c r="BE9" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="BF9" s="18" t="s">
-        <v>63</v>
-      </c>
+      <c r="BE9" s="18"/>
+      <c r="BF9" s="18"/>
       <c r="BG9" s="18" t="s">
         <v>63</v>
       </c>
       <c r="BH9" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="BI9" s="18"/>
-      <c r="BJ9" s="18"/>
-      <c r="BK9" s="18"/>
+      <c r="BI9" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="BJ9" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="BK9" s="18" t="s">
+        <v>63</v>
+      </c>
       <c r="BL9" s="18"/>
       <c r="BM9" s="18"/>
       <c r="BN9" s="18"/>
       <c r="BO9" s="18"/>
       <c r="BP9" s="18"/>
-      <c r="BQ9" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="BR9" s="18" t="s">
-        <v>64</v>
-      </c>
+      <c r="BQ9" s="18"/>
+      <c r="BR9" s="18"/>
       <c r="BS9" s="18" t="s">
         <v>64</v>
       </c>
       <c r="BT9" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="BU9" s="18"/>
-      <c r="BV9" s="18"/>
-      <c r="BW9" s="18"/>
+      <c r="BU9" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="BV9" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="BW9" s="18" t="s">
+        <v>64</v>
+      </c>
       <c r="BX9" s="18"/>
       <c r="BY9" s="18"/>
       <c r="BZ9" s="18"/>
       <c r="CA9" s="18"/>
       <c r="CB9" s="18"/>
-      <c r="CC9" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="CD9" s="18" t="s">
-        <v>65</v>
-      </c>
+      <c r="CC9" s="18"/>
+      <c r="CD9" s="18"/>
       <c r="CE9" s="18" t="s">
         <v>65</v>
       </c>
       <c r="CF9" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="CG9" s="18"/>
-      <c r="CH9" s="18"/>
-      <c r="CI9" s="18"/>
-      <c r="CJ9" s="18"/>
-      <c r="CK9" s="18"/>
-      <c r="CL9" s="18"/>
-      <c r="CM9" s="18"/>
-      <c r="CN9" s="18"/>
-      <c r="CO9" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="CP9" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="CQ9" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="CR9" s="18" t="s">
-        <v>66</v>
-      </c>
+      <c r="CG9" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="CH9" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="CI9" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="CJ9" s="9"/>
+      <c r="CK9" s="9"/>
+      <c r="CL9" s="9"/>
+      <c r="CM9" s="9"/>
+      <c r="CN9" s="9"/>
+      <c r="CO9" s="9"/>
+      <c r="CP9" s="9"/>
+      <c r="CQ9" s="9"/>
+      <c r="CR9" s="9"/>
       <c r="CS9" s="9"/>
       <c r="CT9" s="9"/>
       <c r="CU9" s="9"/>
@@ -4409,18 +4548,13 @@
       <c r="DI9" s="9"/>
       <c r="DJ9" s="9"/>
       <c r="DK9" s="9"/>
-      <c r="DL9" s="9"/>
-      <c r="DM9" s="9"/>
-      <c r="DN9" s="9"/>
-      <c r="DO9" s="10"/>
-      <c r="DP9" s="23"/>
-      <c r="DQ9" s="23"/>
-      <c r="DR9" s="23"/>
+      <c r="DL9" s="10"/>
+      <c r="DM9" s="23"/>
     </row>
-    <row r="10" spans="2:122" ht="42" customHeight="1">
-      <c r="B10" s="33"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
+    <row r="10" spans="2:117" ht="42" customHeight="1">
+      <c r="B10" s="35"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
@@ -4448,17 +4582,19 @@
       <c r="AC10" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="AD10" s="18" t="str">
-        <f>AC10</f>
+      <c r="AD10" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE10" s="18" t="str">
+        <f>AD10</f>
         <v>joint 2</v>
-      </c>
-      <c r="AE10" s="18" t="s">
-        <v>4</v>
       </c>
       <c r="AF10" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="AG10" s="18"/>
+      <c r="AG10" s="18" t="s">
+        <v>4</v>
+      </c>
       <c r="AH10" s="18"/>
       <c r="AI10" s="18"/>
       <c r="AJ10" s="18"/>
@@ -4513,15 +4649,15 @@
       <c r="CG10" s="18"/>
       <c r="CH10" s="18"/>
       <c r="CI10" s="18"/>
-      <c r="CJ10" s="18"/>
-      <c r="CK10" s="18"/>
-      <c r="CL10" s="18"/>
-      <c r="CM10" s="18"/>
-      <c r="CN10" s="18"/>
-      <c r="CO10" s="18"/>
-      <c r="CP10" s="18"/>
-      <c r="CQ10" s="18"/>
-      <c r="CR10" s="18"/>
+      <c r="CJ10" s="9"/>
+      <c r="CK10" s="9"/>
+      <c r="CL10" s="9"/>
+      <c r="CM10" s="9"/>
+      <c r="CN10" s="9"/>
+      <c r="CO10" s="9"/>
+      <c r="CP10" s="9"/>
+      <c r="CQ10" s="9"/>
+      <c r="CR10" s="9"/>
       <c r="CS10" s="9"/>
       <c r="CT10" s="9"/>
       <c r="CU10" s="9"/>
@@ -4541,18 +4677,13 @@
       <c r="DI10" s="9"/>
       <c r="DJ10" s="9"/>
       <c r="DK10" s="9"/>
-      <c r="DL10" s="9"/>
-      <c r="DM10" s="9"/>
-      <c r="DN10" s="9"/>
-      <c r="DO10" s="10"/>
-      <c r="DP10" s="23"/>
-      <c r="DQ10" s="23"/>
-      <c r="DR10" s="23"/>
+      <c r="DL10" s="10"/>
+      <c r="DM10" s="23"/>
     </row>
-    <row r="11" spans="2:122" ht="42" customHeight="1">
-      <c r="B11" s="33"/>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
+    <row r="11" spans="2:117" ht="42" customHeight="1">
+      <c r="B11" s="35"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
@@ -4581,9 +4712,8 @@
       <c r="AD11" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="AE11" s="18" t="str">
-        <f>AD11</f>
-        <v>joint 3</v>
+      <c r="AE11" s="18" t="s">
+        <v>5</v>
       </c>
       <c r="AF11" s="18" t="str">
         <f>AE11</f>
@@ -4593,7 +4723,10 @@
         <f>AF11</f>
         <v>joint 3</v>
       </c>
-      <c r="AH11" s="18"/>
+      <c r="AH11" s="18" t="str">
+        <f>AG11</f>
+        <v>joint 3</v>
+      </c>
       <c r="AI11" s="18"/>
       <c r="AJ11" s="18"/>
       <c r="AK11" s="18"/>
@@ -4647,15 +4780,15 @@
       <c r="CG11" s="18"/>
       <c r="CH11" s="18"/>
       <c r="CI11" s="18"/>
-      <c r="CJ11" s="18"/>
-      <c r="CK11" s="18"/>
-      <c r="CL11" s="18"/>
-      <c r="CM11" s="18"/>
-      <c r="CN11" s="18"/>
-      <c r="CO11" s="18"/>
-      <c r="CP11" s="18"/>
-      <c r="CQ11" s="18"/>
-      <c r="CR11" s="18"/>
+      <c r="CJ11" s="9"/>
+      <c r="CK11" s="9"/>
+      <c r="CL11" s="9"/>
+      <c r="CM11" s="9"/>
+      <c r="CN11" s="9"/>
+      <c r="CO11" s="9"/>
+      <c r="CP11" s="9"/>
+      <c r="CQ11" s="9"/>
+      <c r="CR11" s="9"/>
       <c r="CS11" s="9"/>
       <c r="CT11" s="9"/>
       <c r="CU11" s="9"/>
@@ -4675,18 +4808,13 @@
       <c r="DI11" s="9"/>
       <c r="DJ11" s="9"/>
       <c r="DK11" s="9"/>
-      <c r="DL11" s="9"/>
-      <c r="DM11" s="9"/>
-      <c r="DN11" s="9"/>
-      <c r="DO11" s="10"/>
-      <c r="DP11" s="23"/>
-      <c r="DQ11" s="23"/>
-      <c r="DR11" s="23"/>
+      <c r="DL11" s="10"/>
+      <c r="DM11" s="23"/>
     </row>
-    <row r="12" spans="2:122" ht="42" customHeight="1">
-      <c r="B12" s="33"/>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
+    <row r="12" spans="2:117" ht="42" customHeight="1">
+      <c r="B12" s="35"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9"/>
@@ -4716,16 +4844,18 @@
       <c r="AE12" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="AF12" s="29" t="s">
+      <c r="AF12" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="AG12" s="29" t="s">
+      <c r="AG12" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="AH12" s="29" t="s">
+      <c r="AH12" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="AI12" s="18"/>
+      <c r="AI12" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="AJ12" s="18"/>
       <c r="AK12" s="18"/>
       <c r="AL12" s="18"/>
@@ -4778,15 +4908,15 @@
       <c r="CG12" s="18"/>
       <c r="CH12" s="18"/>
       <c r="CI12" s="18"/>
-      <c r="CJ12" s="18"/>
-      <c r="CK12" s="18"/>
-      <c r="CL12" s="18"/>
-      <c r="CM12" s="18"/>
-      <c r="CN12" s="18"/>
-      <c r="CO12" s="18"/>
-      <c r="CP12" s="18"/>
-      <c r="CQ12" s="18"/>
-      <c r="CR12" s="18"/>
+      <c r="CJ12" s="9"/>
+      <c r="CK12" s="9"/>
+      <c r="CL12" s="9"/>
+      <c r="CM12" s="9"/>
+      <c r="CN12" s="9"/>
+      <c r="CO12" s="9"/>
+      <c r="CP12" s="9"/>
+      <c r="CQ12" s="9"/>
+      <c r="CR12" s="9"/>
       <c r="CS12" s="9"/>
       <c r="CT12" s="9"/>
       <c r="CU12" s="9"/>
@@ -4806,18 +4936,13 @@
       <c r="DI12" s="9"/>
       <c r="DJ12" s="9"/>
       <c r="DK12" s="9"/>
-      <c r="DL12" s="9"/>
-      <c r="DM12" s="9"/>
-      <c r="DN12" s="9"/>
-      <c r="DO12" s="10"/>
-      <c r="DP12" s="23"/>
-      <c r="DQ12" s="23"/>
-      <c r="DR12" s="23"/>
+      <c r="DL12" s="10"/>
+      <c r="DM12" s="23"/>
     </row>
-    <row r="13" spans="2:122" ht="42" customHeight="1">
-      <c r="B13" s="33"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
+    <row r="13" spans="2:117" ht="42" customHeight="1">
+      <c r="B13" s="35"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
@@ -4851,15 +4976,17 @@
       <c r="AG13" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="AH13" s="18" t="str">
-        <f>AG13</f>
-        <v>joint 5</v>
+      <c r="AH13" s="18" t="s">
+        <v>7</v>
       </c>
       <c r="AI13" s="18" t="str">
         <f>AH13</f>
         <v>joint 5</v>
       </c>
-      <c r="AJ13" s="18"/>
+      <c r="AJ13" s="18" t="str">
+        <f>AI13</f>
+        <v>joint 5</v>
+      </c>
       <c r="AK13" s="18"/>
       <c r="AL13" s="18"/>
       <c r="AM13" s="18"/>
@@ -4911,15 +5038,15 @@
       <c r="CG13" s="18"/>
       <c r="CH13" s="18"/>
       <c r="CI13" s="18"/>
-      <c r="CJ13" s="18"/>
-      <c r="CK13" s="18"/>
-      <c r="CL13" s="18"/>
-      <c r="CM13" s="18"/>
-      <c r="CN13" s="18"/>
-      <c r="CO13" s="18"/>
-      <c r="CP13" s="18"/>
-      <c r="CQ13" s="18"/>
-      <c r="CR13" s="18"/>
+      <c r="CJ13" s="9"/>
+      <c r="CK13" s="9"/>
+      <c r="CL13" s="9"/>
+      <c r="CM13" s="9"/>
+      <c r="CN13" s="9"/>
+      <c r="CO13" s="9"/>
+      <c r="CP13" s="9"/>
+      <c r="CQ13" s="9"/>
+      <c r="CR13" s="9"/>
       <c r="CS13" s="9"/>
       <c r="CT13" s="9"/>
       <c r="CU13" s="9"/>
@@ -4939,18 +5066,13 @@
       <c r="DI13" s="9"/>
       <c r="DJ13" s="9"/>
       <c r="DK13" s="9"/>
-      <c r="DL13" s="9"/>
-      <c r="DM13" s="9"/>
-      <c r="DN13" s="9"/>
-      <c r="DO13" s="10"/>
-      <c r="DP13" s="23"/>
-      <c r="DQ13" s="23"/>
-      <c r="DR13" s="23"/>
+      <c r="DL13" s="10"/>
+      <c r="DM13" s="23"/>
     </row>
-    <row r="14" spans="2:122" ht="42" customHeight="1">
-      <c r="B14" s="33"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
+    <row r="14" spans="2:117" ht="42" customHeight="1">
+      <c r="B14" s="35"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
       <c r="E14" s="9"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
@@ -4982,16 +5104,18 @@
       <c r="AG14" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="AH14" s="29" t="s">
+      <c r="AH14" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="AI14" s="29" t="s">
+      <c r="AI14" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="AJ14" s="29" t="s">
+      <c r="AJ14" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="AK14" s="18"/>
+      <c r="AK14" s="27" t="s">
+        <v>8</v>
+      </c>
       <c r="AL14" s="18"/>
       <c r="AM14" s="18"/>
       <c r="AN14" s="18"/>
@@ -5042,15 +5166,15 @@
       <c r="CG14" s="18"/>
       <c r="CH14" s="18"/>
       <c r="CI14" s="18"/>
-      <c r="CJ14" s="18"/>
-      <c r="CK14" s="18"/>
-      <c r="CL14" s="18"/>
-      <c r="CM14" s="18"/>
-      <c r="CN14" s="18"/>
-      <c r="CO14" s="18"/>
-      <c r="CP14" s="18"/>
-      <c r="CQ14" s="18"/>
-      <c r="CR14" s="18"/>
+      <c r="CJ14" s="9"/>
+      <c r="CK14" s="9"/>
+      <c r="CL14" s="9"/>
+      <c r="CM14" s="9"/>
+      <c r="CN14" s="9"/>
+      <c r="CO14" s="9"/>
+      <c r="CP14" s="9"/>
+      <c r="CQ14" s="9"/>
+      <c r="CR14" s="9"/>
       <c r="CS14" s="9"/>
       <c r="CT14" s="9"/>
       <c r="CU14" s="9"/>
@@ -5070,23 +5194,18 @@
       <c r="DI14" s="9"/>
       <c r="DJ14" s="9"/>
       <c r="DK14" s="9"/>
-      <c r="DL14" s="9"/>
-      <c r="DM14" s="9"/>
-      <c r="DN14" s="9"/>
-      <c r="DO14" s="10"/>
-      <c r="DP14" s="23"/>
-      <c r="DQ14" s="23"/>
-      <c r="DR14" s="23"/>
+      <c r="DL14" s="10"/>
+      <c r="DM14" s="23"/>
     </row>
-    <row r="15" spans="2:122" ht="42" customHeight="1">
-      <c r="B15" s="24" t="s">
+    <row r="15" spans="2:117" ht="42" customHeight="1">
+      <c r="B15" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="25">
+      <c r="C15" s="32">
         <v>36</v>
       </c>
-      <c r="D15" s="25" t="s">
-        <v>165</v>
+      <c r="D15" s="32" t="s">
+        <v>163</v>
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9"/>
@@ -5116,256 +5235,253 @@
       <c r="AD15" s="9"/>
       <c r="AE15" s="9"/>
       <c r="AF15" s="9"/>
-      <c r="AG15" s="1" t="s">
+      <c r="AG15" s="9"/>
+      <c r="AH15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AH15" s="1" t="s">
+      <c r="AI15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AI15" s="1" t="s">
+      <c r="AJ15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AJ15" s="1" t="s">
+      <c r="AK15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AK15" s="1" t="s">
+      <c r="AL15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AL15" s="1" t="s">
+      <c r="AM15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AM15" s="1" t="s">
+      <c r="AN15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AN15" s="1" t="s">
+      <c r="AO15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AO15" s="1" t="s">
+      <c r="AP15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AP15" s="1" t="s">
+      <c r="AQ15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AQ15" s="1" t="s">
+      <c r="AR15" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="AS15" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AT15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AU15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AW15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AX15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AY15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AZ15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="BA15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="BB15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="BC15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="BD15" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="AR15" s="1" t="s">
+      <c r="BE15" s="24" t="s">
+        <v>164</v>
+      </c>
+      <c r="BF15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="BG15" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="BH15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="BI15" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="BJ15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="BK15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="BL15" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="BM15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="BN15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="BO15" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="BP15" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="BQ15" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="AS15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AT15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AU15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AV15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AW15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AX15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AY15" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AZ15" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="BA15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="BB15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="BC15" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="BD15" s="26" t="s">
-        <v>166</v>
-      </c>
-      <c r="BE15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="BF15" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="BG15" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="BH15" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="BI15" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="BJ15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="BK15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="BL15" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="BM15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="BN15" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="BO15" s="1" t="s">
+      <c r="BR15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="BS15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="BT15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="BU15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="BV15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="BW15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="BX15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="BY15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="BZ15" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="CA15" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="CB15" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="BP15" s="1" t="s">
+      <c r="CC15" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="BQ15" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="BR15" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="BS15" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="BT15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="BU15" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="BV15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="BW15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="BX15" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="BY15" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="BZ15" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="CA15" s="1" t="s">
+      <c r="CD15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="CE15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="CF15" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="CG15" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="CH15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="CI15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="CJ15" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="CK15" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="CL15" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="CM15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="CN15" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="CB15" s="1" t="s">
+      <c r="CO15" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="CC15" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="CD15" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="CE15" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="CF15" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="CG15" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="CH15" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="CI15" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="CJ15" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="CK15" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="CL15" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="CM15" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="CN15" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="CO15" s="9"/>
       <c r="CP15" s="9"/>
       <c r="CQ15" s="9"/>
-      <c r="CR15" s="9"/>
-      <c r="CS15" s="9"/>
-      <c r="CT15" s="9"/>
-      <c r="CU15" s="9"/>
-      <c r="CV15" s="27" t="s">
-        <v>104</v>
-      </c>
-      <c r="CW15" s="27" t="s">
-        <v>104</v>
-      </c>
-      <c r="CX15" s="27" t="s">
-        <v>104</v>
-      </c>
-      <c r="CY15" s="27" t="s">
-        <v>104</v>
-      </c>
-      <c r="CZ15" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="DA15" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="DB15" s="9"/>
+      <c r="CR15" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="CS15" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="CT15" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="CU15" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="CV15" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="CW15" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="CX15" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="CY15" s="9"/>
+      <c r="CZ15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="DA15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="DB15" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="DC15" s="1" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="DD15" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="DE15" s="1" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="DF15" s="1" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="DG15" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="DH15" s="1" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="DI15" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="DJ15" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="DK15" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="DL15" s="1" t="s">
+      <c r="DJ15" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="DK15" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="DL15" s="10"/>
+      <c r="DM15" s="23"/>
+    </row>
+    <row r="16" spans="2:117" ht="42" customHeight="1" thickBot="1">
+      <c r="B16" s="13" t="s">
         <v>76</v>
-      </c>
-      <c r="DM15" s="26" t="s">
-        <v>122</v>
-      </c>
-      <c r="DN15" s="26" t="s">
-        <v>123</v>
-      </c>
-      <c r="DO15" s="10"/>
-      <c r="DP15" s="23"/>
-      <c r="DQ15" s="23"/>
-      <c r="DR15" s="23"/>
-    </row>
-    <row r="16" spans="2:122" ht="42" customHeight="1" thickBot="1">
-      <c r="B16" s="13" t="s">
-        <v>77</v>
       </c>
       <c r="C16" s="14">
         <v>36</v>
@@ -5407,10 +5523,10 @@
       <c r="AJ16" s="15"/>
       <c r="AK16" s="15"/>
       <c r="AL16" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AM16" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AN16" s="15"/>
       <c r="AO16" s="15"/>
@@ -5421,14 +5537,14 @@
       <c r="AT16" s="15"/>
       <c r="AU16" s="15"/>
       <c r="AV16" s="15"/>
-      <c r="AW16" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="AX16" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="AY16" s="15"/>
-      <c r="AZ16" s="15"/>
+      <c r="AW16" s="15"/>
+      <c r="AX16" s="15"/>
+      <c r="AY16" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="AZ16" s="15" t="s">
+        <v>116</v>
+      </c>
       <c r="BA16" s="15"/>
       <c r="BB16" s="15"/>
       <c r="BC16" s="15"/>
@@ -5437,14 +5553,14 @@
       <c r="BF16" s="15"/>
       <c r="BG16" s="15"/>
       <c r="BH16" s="15"/>
-      <c r="BI16" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="BJ16" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="BK16" s="15"/>
-      <c r="BL16" s="15"/>
+      <c r="BI16" s="15"/>
+      <c r="BJ16" s="15"/>
+      <c r="BK16" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="BL16" s="16" t="s">
+        <v>117</v>
+      </c>
       <c r="BM16" s="15"/>
       <c r="BN16" s="15"/>
       <c r="BO16" s="15"/>
@@ -5453,14 +5569,14 @@
       <c r="BR16" s="15"/>
       <c r="BS16" s="15"/>
       <c r="BT16" s="15"/>
-      <c r="BU16" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="BV16" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="BW16" s="15"/>
-      <c r="BX16" s="15"/>
+      <c r="BU16" s="15"/>
+      <c r="BV16" s="15"/>
+      <c r="BW16" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="BX16" s="16" t="s">
+        <v>118</v>
+      </c>
       <c r="BY16" s="15"/>
       <c r="BZ16" s="15"/>
       <c r="CA16" s="15"/>
@@ -5469,40 +5585,36 @@
       <c r="CD16" s="15"/>
       <c r="CE16" s="15"/>
       <c r="CF16" s="15"/>
-      <c r="CG16" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="CH16" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="CI16" s="15"/>
-      <c r="CJ16" s="15"/>
+      <c r="CG16" s="15"/>
+      <c r="CH16" s="15"/>
+      <c r="CI16" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="CJ16" s="16" t="s">
+        <v>119</v>
+      </c>
       <c r="CK16" s="15"/>
       <c r="CL16" s="15"/>
       <c r="CM16" s="15"/>
       <c r="CN16" s="15"/>
       <c r="CO16" s="15"/>
-      <c r="CP16" s="15"/>
+      <c r="CP16" s="15" t="s">
+        <v>102</v>
+      </c>
       <c r="CQ16" s="15"/>
       <c r="CR16" s="15"/>
-      <c r="CS16" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="CT16" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="CU16" s="15" t="s">
-        <v>103</v>
-      </c>
+      <c r="CS16" s="15"/>
+      <c r="CT16" s="16"/>
+      <c r="CU16" s="16"/>
       <c r="CV16" s="15"/>
       <c r="CW16" s="15"/>
-      <c r="CX16" s="15"/>
+      <c r="CX16" s="15" t="s">
+        <v>104</v>
+      </c>
       <c r="CY16" s="15"/>
       <c r="CZ16" s="15"/>
       <c r="DA16" s="15"/>
-      <c r="DB16" s="15" t="s">
-        <v>105</v>
-      </c>
+      <c r="DB16" s="15"/>
       <c r="DC16" s="15"/>
       <c r="DD16" s="15"/>
       <c r="DE16" s="15"/>
@@ -5512,140 +5624,135 @@
       <c r="DI16" s="15"/>
       <c r="DJ16" s="15"/>
       <c r="DK16" s="15"/>
-      <c r="DL16" s="15"/>
-      <c r="DM16" s="15"/>
-      <c r="DN16" s="15"/>
-      <c r="DO16" s="17" t="s">
-        <v>106</v>
-      </c>
-      <c r="DP16" s="23"/>
-      <c r="DQ16" s="23"/>
-      <c r="DR16" s="23"/>
+      <c r="DL16" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="DM16" s="23"/>
     </row>
     <row r="17" spans="2:117" ht="42" customHeight="1" thickBot="1"/>
     <row r="18" spans="2:117" s="2" customFormat="1" ht="42" customHeight="1">
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="31"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="31"/>
-      <c r="N18" s="31"/>
-      <c r="O18" s="31"/>
-      <c r="P18" s="31"/>
-      <c r="Q18" s="31"/>
-      <c r="R18" s="31"/>
-      <c r="S18" s="31"/>
-      <c r="T18" s="31"/>
-      <c r="U18" s="31"/>
-      <c r="V18" s="31"/>
-      <c r="W18" s="31"/>
-      <c r="X18" s="31"/>
-      <c r="Y18" s="31"/>
-      <c r="Z18" s="31"/>
-      <c r="AA18" s="31"/>
-      <c r="AB18" s="31"/>
-      <c r="AC18" s="31"/>
-      <c r="AD18" s="31"/>
-      <c r="AE18" s="31"/>
-      <c r="AF18" s="31"/>
-      <c r="AG18" s="31"/>
-      <c r="AH18" s="31"/>
-      <c r="AI18" s="31"/>
-      <c r="AJ18" s="31"/>
-      <c r="AK18" s="31"/>
-      <c r="AL18" s="31"/>
-      <c r="AM18" s="31"/>
-      <c r="AN18" s="31"/>
-      <c r="AO18" s="31"/>
-      <c r="AP18" s="31"/>
-      <c r="AQ18" s="31"/>
-      <c r="AR18" s="31"/>
-      <c r="AS18" s="31"/>
-      <c r="AT18" s="31"/>
-      <c r="AU18" s="31"/>
-      <c r="AV18" s="31"/>
-      <c r="AW18" s="31"/>
-      <c r="AX18" s="31"/>
-      <c r="AY18" s="31"/>
-      <c r="AZ18" s="31"/>
-      <c r="BA18" s="31"/>
-      <c r="BB18" s="31"/>
-      <c r="BC18" s="31"/>
-      <c r="BD18" s="31"/>
-      <c r="BE18" s="31"/>
-      <c r="BF18" s="31"/>
-      <c r="BG18" s="31"/>
-      <c r="BH18" s="31"/>
-      <c r="BI18" s="31"/>
-      <c r="BJ18" s="31"/>
-      <c r="BK18" s="31"/>
-      <c r="BL18" s="31"/>
-      <c r="BM18" s="31"/>
-      <c r="BN18" s="31"/>
-      <c r="BO18" s="31"/>
-      <c r="BP18" s="31"/>
-      <c r="BQ18" s="31"/>
-      <c r="BR18" s="31"/>
-      <c r="BS18" s="31"/>
-      <c r="BT18" s="31"/>
-      <c r="BU18" s="31"/>
-      <c r="BV18" s="31"/>
-      <c r="BW18" s="31"/>
-      <c r="BX18" s="31"/>
-      <c r="BY18" s="31"/>
-      <c r="BZ18" s="31"/>
-      <c r="CA18" s="31"/>
-      <c r="CB18" s="31"/>
-      <c r="CC18" s="31"/>
-      <c r="CD18" s="31"/>
-      <c r="CE18" s="31"/>
-      <c r="CF18" s="31"/>
-      <c r="CG18" s="31"/>
-      <c r="CH18" s="31"/>
-      <c r="CI18" s="31"/>
-      <c r="CJ18" s="31"/>
-      <c r="CK18" s="31"/>
-      <c r="CL18" s="31"/>
-      <c r="CM18" s="31"/>
-      <c r="CN18" s="31"/>
-      <c r="CO18" s="31"/>
-      <c r="CP18" s="31"/>
-      <c r="CQ18" s="31"/>
-      <c r="CR18" s="31"/>
-      <c r="CS18" s="31"/>
-      <c r="CT18" s="31"/>
-      <c r="CU18" s="31"/>
-      <c r="CV18" s="31"/>
-      <c r="CW18" s="31"/>
-      <c r="CX18" s="31"/>
-      <c r="CY18" s="31"/>
-      <c r="CZ18" s="31"/>
-      <c r="DA18" s="31"/>
-      <c r="DB18" s="31"/>
-      <c r="DC18" s="31"/>
-      <c r="DD18" s="31"/>
-      <c r="DE18" s="31"/>
-      <c r="DF18" s="31"/>
-      <c r="DG18" s="31"/>
-      <c r="DH18" s="31"/>
-      <c r="DI18" s="31"/>
-      <c r="DJ18" s="31"/>
-      <c r="DK18" s="31"/>
-      <c r="DL18" s="31"/>
-      <c r="DM18" s="32"/>
+      <c r="E18" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33"/>
+      <c r="K18" s="33"/>
+      <c r="L18" s="33"/>
+      <c r="M18" s="33"/>
+      <c r="N18" s="33"/>
+      <c r="O18" s="33"/>
+      <c r="P18" s="33"/>
+      <c r="Q18" s="33"/>
+      <c r="R18" s="33"/>
+      <c r="S18" s="33"/>
+      <c r="T18" s="33"/>
+      <c r="U18" s="33"/>
+      <c r="V18" s="33"/>
+      <c r="W18" s="33"/>
+      <c r="X18" s="33"/>
+      <c r="Y18" s="33"/>
+      <c r="Z18" s="33"/>
+      <c r="AA18" s="33"/>
+      <c r="AB18" s="33"/>
+      <c r="AC18" s="33"/>
+      <c r="AD18" s="33"/>
+      <c r="AE18" s="33"/>
+      <c r="AF18" s="33"/>
+      <c r="AG18" s="33"/>
+      <c r="AH18" s="33"/>
+      <c r="AI18" s="33"/>
+      <c r="AJ18" s="33"/>
+      <c r="AK18" s="33"/>
+      <c r="AL18" s="33"/>
+      <c r="AM18" s="33"/>
+      <c r="AN18" s="33"/>
+      <c r="AO18" s="33"/>
+      <c r="AP18" s="33"/>
+      <c r="AQ18" s="33"/>
+      <c r="AR18" s="33"/>
+      <c r="AS18" s="33"/>
+      <c r="AT18" s="33"/>
+      <c r="AU18" s="33"/>
+      <c r="AV18" s="33"/>
+      <c r="AW18" s="33"/>
+      <c r="AX18" s="33"/>
+      <c r="AY18" s="33"/>
+      <c r="AZ18" s="33"/>
+      <c r="BA18" s="33"/>
+      <c r="BB18" s="33"/>
+      <c r="BC18" s="33"/>
+      <c r="BD18" s="33"/>
+      <c r="BE18" s="33"/>
+      <c r="BF18" s="33"/>
+      <c r="BG18" s="33"/>
+      <c r="BH18" s="33"/>
+      <c r="BI18" s="33"/>
+      <c r="BJ18" s="33"/>
+      <c r="BK18" s="33"/>
+      <c r="BL18" s="33"/>
+      <c r="BM18" s="33"/>
+      <c r="BN18" s="33"/>
+      <c r="BO18" s="33"/>
+      <c r="BP18" s="33"/>
+      <c r="BQ18" s="33"/>
+      <c r="BR18" s="33"/>
+      <c r="BS18" s="33"/>
+      <c r="BT18" s="33"/>
+      <c r="BU18" s="33"/>
+      <c r="BV18" s="33"/>
+      <c r="BW18" s="33"/>
+      <c r="BX18" s="33"/>
+      <c r="BY18" s="33"/>
+      <c r="BZ18" s="33"/>
+      <c r="CA18" s="33"/>
+      <c r="CB18" s="33"/>
+      <c r="CC18" s="33"/>
+      <c r="CD18" s="33"/>
+      <c r="CE18" s="33"/>
+      <c r="CF18" s="33"/>
+      <c r="CG18" s="33"/>
+      <c r="CH18" s="33"/>
+      <c r="CI18" s="33"/>
+      <c r="CJ18" s="33"/>
+      <c r="CK18" s="33"/>
+      <c r="CL18" s="33"/>
+      <c r="CM18" s="33"/>
+      <c r="CN18" s="33"/>
+      <c r="CO18" s="33"/>
+      <c r="CP18" s="33"/>
+      <c r="CQ18" s="33"/>
+      <c r="CR18" s="33"/>
+      <c r="CS18" s="33"/>
+      <c r="CT18" s="33"/>
+      <c r="CU18" s="33"/>
+      <c r="CV18" s="33"/>
+      <c r="CW18" s="33"/>
+      <c r="CX18" s="33"/>
+      <c r="CY18" s="33"/>
+      <c r="CZ18" s="33"/>
+      <c r="DA18" s="33"/>
+      <c r="DB18" s="33"/>
+      <c r="DC18" s="33"/>
+      <c r="DD18" s="33"/>
+      <c r="DE18" s="33"/>
+      <c r="DF18" s="33"/>
+      <c r="DG18" s="33"/>
+      <c r="DH18" s="33"/>
+      <c r="DI18" s="33"/>
+      <c r="DJ18" s="33"/>
+      <c r="DK18" s="33"/>
+      <c r="DL18" s="33"/>
+      <c r="DM18" s="34"/>
     </row>
     <row r="19" spans="2:117" s="2" customFormat="1" ht="42" customHeight="1">
       <c r="B19" s="20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C19" s="21" t="s">
         <v>1</v>
@@ -5654,456 +5761,456 @@
         <v>10</v>
       </c>
       <c r="E19" s="21">
-        <f>DO2+1</f>
+        <f>MAX(2:2)</f>
+        <v>112</v>
+      </c>
+      <c r="F19" s="21">
+        <f t="shared" ref="F19" si="56">E19+1</f>
+        <v>113</v>
+      </c>
+      <c r="G19" s="21">
+        <f t="shared" ref="G19" si="57">F19+1</f>
+        <v>114</v>
+      </c>
+      <c r="H19" s="21">
+        <f t="shared" ref="H19" si="58">G19+1</f>
+        <v>115</v>
+      </c>
+      <c r="I19" s="21">
+        <f t="shared" ref="I19" si="59">H19+1</f>
         <v>116</v>
       </c>
-      <c r="F19" s="21">
-        <f t="shared" ref="F19" si="59">E19+1</f>
+      <c r="J19" s="21">
+        <f t="shared" ref="J19" si="60">I19+1</f>
         <v>117</v>
       </c>
-      <c r="G19" s="21">
-        <f t="shared" ref="G19" si="60">F19+1</f>
+      <c r="K19" s="21">
+        <f t="shared" ref="K19" si="61">J19+1</f>
         <v>118</v>
       </c>
-      <c r="H19" s="21">
-        <f t="shared" ref="H19" si="61">G19+1</f>
+      <c r="L19" s="21">
+        <f t="shared" ref="L19" si="62">K19+1</f>
         <v>119</v>
       </c>
-      <c r="I19" s="21">
-        <f t="shared" ref="I19" si="62">H19+1</f>
+      <c r="M19" s="21">
+        <f t="shared" ref="M19" si="63">L19+1</f>
         <v>120</v>
       </c>
-      <c r="J19" s="21">
-        <f t="shared" ref="J19" si="63">I19+1</f>
+      <c r="N19" s="21">
+        <f t="shared" ref="N19" si="64">M19+1</f>
         <v>121</v>
       </c>
-      <c r="K19" s="21">
-        <f t="shared" ref="K19" si="64">J19+1</f>
+      <c r="O19" s="21">
+        <f t="shared" ref="O19" si="65">N19+1</f>
         <v>122</v>
       </c>
-      <c r="L19" s="21">
-        <f t="shared" ref="L19" si="65">K19+1</f>
+      <c r="P19" s="21">
+        <f t="shared" ref="P19" si="66">O19+1</f>
         <v>123</v>
       </c>
-      <c r="M19" s="21">
-        <f t="shared" ref="M19" si="66">L19+1</f>
+      <c r="Q19" s="21">
+        <f t="shared" ref="Q19" si="67">P19+1</f>
         <v>124</v>
       </c>
-      <c r="N19" s="21">
-        <f t="shared" ref="N19" si="67">M19+1</f>
+      <c r="R19" s="21">
+        <f t="shared" ref="R19" si="68">Q19+1</f>
         <v>125</v>
       </c>
-      <c r="O19" s="21">
-        <f t="shared" ref="O19" si="68">N19+1</f>
+      <c r="S19" s="21">
+        <f t="shared" ref="S19" si="69">R19+1</f>
         <v>126</v>
       </c>
-      <c r="P19" s="21">
-        <f t="shared" ref="P19" si="69">O19+1</f>
+      <c r="T19" s="21">
+        <f t="shared" ref="T19" si="70">S19+1</f>
         <v>127</v>
       </c>
-      <c r="Q19" s="21">
-        <f t="shared" ref="Q19" si="70">P19+1</f>
+      <c r="U19" s="21">
+        <f t="shared" ref="U19" si="71">T19+1</f>
         <v>128</v>
       </c>
-      <c r="R19" s="21">
-        <f t="shared" ref="R19" si="71">Q19+1</f>
+      <c r="V19" s="21">
+        <f t="shared" ref="V19" si="72">U19+1</f>
         <v>129</v>
       </c>
-      <c r="S19" s="21">
-        <f t="shared" ref="S19" si="72">R19+1</f>
+      <c r="W19" s="21">
+        <f t="shared" ref="W19" si="73">V19+1</f>
         <v>130</v>
       </c>
-      <c r="T19" s="21">
-        <f t="shared" ref="T19" si="73">S19+1</f>
+      <c r="X19" s="21">
+        <f t="shared" ref="X19" si="74">W19+1</f>
         <v>131</v>
       </c>
-      <c r="U19" s="21">
-        <f t="shared" ref="U19" si="74">T19+1</f>
+      <c r="Y19" s="21">
+        <f t="shared" ref="Y19" si="75">X19+1</f>
         <v>132</v>
       </c>
-      <c r="V19" s="21">
-        <f t="shared" ref="V19" si="75">U19+1</f>
+      <c r="Z19" s="21">
+        <f t="shared" ref="Z19" si="76">Y19+1</f>
         <v>133</v>
       </c>
-      <c r="W19" s="21">
-        <f t="shared" ref="W19" si="76">V19+1</f>
+      <c r="AA19" s="21">
+        <f t="shared" ref="AA19" si="77">Z19+1</f>
         <v>134</v>
       </c>
-      <c r="X19" s="21">
-        <f t="shared" ref="X19" si="77">W19+1</f>
+      <c r="AB19" s="21">
+        <f t="shared" ref="AB19" si="78">AA19+1</f>
         <v>135</v>
       </c>
-      <c r="Y19" s="21">
-        <f t="shared" ref="Y19" si="78">X19+1</f>
+      <c r="AC19" s="21">
+        <f t="shared" ref="AC19" si="79">AB19+1</f>
         <v>136</v>
       </c>
-      <c r="Z19" s="21">
-        <f t="shared" ref="Z19" si="79">Y19+1</f>
+      <c r="AD19" s="21">
+        <f t="shared" ref="AD19" si="80">AC19+1</f>
         <v>137</v>
       </c>
-      <c r="AA19" s="21">
-        <f t="shared" ref="AA19" si="80">Z19+1</f>
+      <c r="AE19" s="21">
+        <f t="shared" ref="AE19" si="81">AD19+1</f>
         <v>138</v>
       </c>
-      <c r="AB19" s="21">
-        <f t="shared" ref="AB19" si="81">AA19+1</f>
+      <c r="AF19" s="21">
+        <f t="shared" ref="AF19" si="82">AE19+1</f>
         <v>139</v>
       </c>
-      <c r="AC19" s="21">
-        <f t="shared" ref="AC19" si="82">AB19+1</f>
+      <c r="AG19" s="21">
+        <f t="shared" ref="AG19" si="83">AF19+1</f>
         <v>140</v>
       </c>
-      <c r="AD19" s="21">
-        <f t="shared" ref="AD19" si="83">AC19+1</f>
+      <c r="AH19" s="21">
+        <f t="shared" ref="AH19" si="84">AG19+1</f>
         <v>141</v>
       </c>
-      <c r="AE19" s="21">
-        <f t="shared" ref="AE19" si="84">AD19+1</f>
+      <c r="AI19" s="21">
+        <f t="shared" ref="AI19" si="85">AH19+1</f>
         <v>142</v>
       </c>
-      <c r="AF19" s="21">
-        <f t="shared" ref="AF19" si="85">AE19+1</f>
+      <c r="AJ19" s="21">
+        <f t="shared" ref="AJ19" si="86">AI19+1</f>
         <v>143</v>
       </c>
-      <c r="AG19" s="21">
-        <f t="shared" ref="AG19" si="86">AF19+1</f>
+      <c r="AK19" s="21">
+        <f t="shared" ref="AK19" si="87">AJ19+1</f>
         <v>144</v>
       </c>
-      <c r="AH19" s="21">
-        <f t="shared" ref="AH19" si="87">AG19+1</f>
+      <c r="AL19" s="21">
+        <f t="shared" ref="AL19" si="88">AK19+1</f>
         <v>145</v>
       </c>
-      <c r="AI19" s="21">
-        <f t="shared" ref="AI19" si="88">AH19+1</f>
+      <c r="AM19" s="21">
+        <f t="shared" ref="AM19" si="89">AL19+1</f>
         <v>146</v>
       </c>
-      <c r="AJ19" s="21">
-        <f t="shared" ref="AJ19" si="89">AI19+1</f>
+      <c r="AN19" s="21">
+        <f t="shared" ref="AN19" si="90">AM19+1</f>
         <v>147</v>
       </c>
-      <c r="AK19" s="21">
-        <f t="shared" ref="AK19" si="90">AJ19+1</f>
+      <c r="AO19" s="21">
+        <f t="shared" ref="AO19" si="91">AN19+1</f>
         <v>148</v>
       </c>
-      <c r="AL19" s="21">
-        <f t="shared" ref="AL19" si="91">AK19+1</f>
+      <c r="AP19" s="21">
+        <f t="shared" ref="AP19" si="92">AO19+1</f>
         <v>149</v>
       </c>
-      <c r="AM19" s="21">
-        <f t="shared" ref="AM19" si="92">AL19+1</f>
+      <c r="AQ19" s="21">
+        <f t="shared" ref="AQ19" si="93">AP19+1</f>
         <v>150</v>
       </c>
-      <c r="AN19" s="21">
-        <f t="shared" ref="AN19" si="93">AM19+1</f>
+      <c r="AR19" s="21">
+        <f t="shared" ref="AR19" si="94">AQ19+1</f>
         <v>151</v>
       </c>
-      <c r="AO19" s="21">
-        <f t="shared" ref="AO19" si="94">AN19+1</f>
+      <c r="AS19" s="21">
+        <f t="shared" ref="AS19" si="95">AR19+1</f>
         <v>152</v>
       </c>
-      <c r="AP19" s="21">
-        <f t="shared" ref="AP19" si="95">AO19+1</f>
+      <c r="AT19" s="21">
+        <f t="shared" ref="AT19" si="96">AS19+1</f>
         <v>153</v>
       </c>
-      <c r="AQ19" s="21">
-        <f t="shared" ref="AQ19" si="96">AP19+1</f>
+      <c r="AU19" s="21">
+        <f t="shared" ref="AU19" si="97">AT19+1</f>
         <v>154</v>
       </c>
-      <c r="AR19" s="21">
-        <f t="shared" ref="AR19" si="97">AQ19+1</f>
+      <c r="AV19" s="21">
+        <f t="shared" ref="AV19" si="98">AU19+1</f>
         <v>155</v>
       </c>
-      <c r="AS19" s="21">
-        <f t="shared" ref="AS19" si="98">AR19+1</f>
+      <c r="AW19" s="21">
+        <f t="shared" ref="AW19" si="99">AV19+1</f>
         <v>156</v>
       </c>
-      <c r="AT19" s="21">
-        <f t="shared" ref="AT19" si="99">AS19+1</f>
+      <c r="AX19" s="21">
+        <f t="shared" ref="AX19" si="100">AW19+1</f>
         <v>157</v>
       </c>
-      <c r="AU19" s="21">
-        <f t="shared" ref="AU19" si="100">AT19+1</f>
+      <c r="AY19" s="21">
+        <f t="shared" ref="AY19" si="101">AX19+1</f>
         <v>158</v>
       </c>
-      <c r="AV19" s="21">
-        <f t="shared" ref="AV19" si="101">AU19+1</f>
+      <c r="AZ19" s="21">
+        <f t="shared" ref="AZ19" si="102">AY19+1</f>
         <v>159</v>
       </c>
-      <c r="AW19" s="21">
-        <f t="shared" ref="AW19" si="102">AV19+1</f>
+      <c r="BA19" s="21">
+        <f t="shared" ref="BA19" si="103">AZ19+1</f>
         <v>160</v>
       </c>
-      <c r="AX19" s="21">
-        <f t="shared" ref="AX19" si="103">AW19+1</f>
+      <c r="BB19" s="21">
+        <f t="shared" ref="BB19" si="104">BA19+1</f>
         <v>161</v>
       </c>
-      <c r="AY19" s="21">
-        <f t="shared" ref="AY19" si="104">AX19+1</f>
+      <c r="BC19" s="21">
+        <f t="shared" ref="BC19" si="105">BB19+1</f>
         <v>162</v>
       </c>
-      <c r="AZ19" s="21">
-        <f t="shared" ref="AZ19" si="105">AY19+1</f>
+      <c r="BD19" s="21">
+        <f t="shared" ref="BD19" si="106">BC19+1</f>
         <v>163</v>
       </c>
-      <c r="BA19" s="21">
-        <f t="shared" ref="BA19" si="106">AZ19+1</f>
+      <c r="BE19" s="21">
+        <f t="shared" ref="BE19" si="107">BD19+1</f>
         <v>164</v>
       </c>
-      <c r="BB19" s="21">
-        <f t="shared" ref="BB19" si="107">BA19+1</f>
+      <c r="BF19" s="21">
+        <f t="shared" ref="BF19" si="108">BE19+1</f>
         <v>165</v>
       </c>
-      <c r="BC19" s="21">
-        <f t="shared" ref="BC19" si="108">BB19+1</f>
+      <c r="BG19" s="21">
+        <f t="shared" ref="BG19" si="109">BF19+1</f>
         <v>166</v>
       </c>
-      <c r="BD19" s="21">
-        <f t="shared" ref="BD19" si="109">BC19+1</f>
+      <c r="BH19" s="21">
+        <f t="shared" ref="BH19" si="110">BG19+1</f>
         <v>167</v>
       </c>
-      <c r="BE19" s="21">
-        <f t="shared" ref="BE19" si="110">BD19+1</f>
+      <c r="BI19" s="21">
+        <f t="shared" ref="BI19" si="111">BH19+1</f>
         <v>168</v>
       </c>
-      <c r="BF19" s="21">
-        <f t="shared" ref="BF19" si="111">BE19+1</f>
+      <c r="BJ19" s="21">
+        <f t="shared" ref="BJ19" si="112">BI19+1</f>
         <v>169</v>
       </c>
-      <c r="BG19" s="21">
-        <f t="shared" ref="BG19" si="112">BF19+1</f>
+      <c r="BK19" s="21">
+        <f t="shared" ref="BK19" si="113">BJ19+1</f>
         <v>170</v>
       </c>
-      <c r="BH19" s="21">
-        <f t="shared" ref="BH19" si="113">BG19+1</f>
+      <c r="BL19" s="21">
+        <f t="shared" ref="BL19" si="114">BK19+1</f>
         <v>171</v>
       </c>
-      <c r="BI19" s="21">
-        <f t="shared" ref="BI19" si="114">BH19+1</f>
+      <c r="BM19" s="21">
+        <f t="shared" ref="BM19" si="115">BL19+1</f>
         <v>172</v>
       </c>
-      <c r="BJ19" s="21">
-        <f t="shared" ref="BJ19" si="115">BI19+1</f>
+      <c r="BN19" s="21">
+        <f t="shared" ref="BN19" si="116">BM19+1</f>
         <v>173</v>
       </c>
-      <c r="BK19" s="21">
-        <f t="shared" ref="BK19" si="116">BJ19+1</f>
+      <c r="BO19" s="21">
+        <f t="shared" ref="BO19" si="117">BN19+1</f>
         <v>174</v>
       </c>
-      <c r="BL19" s="21">
-        <f t="shared" ref="BL19" si="117">BK19+1</f>
+      <c r="BP19" s="21">
+        <f t="shared" ref="BP19" si="118">BO19+1</f>
         <v>175</v>
       </c>
-      <c r="BM19" s="21">
-        <f t="shared" ref="BM19" si="118">BL19+1</f>
+      <c r="BQ19" s="21">
+        <f t="shared" ref="BQ19" si="119">BP19+1</f>
         <v>176</v>
       </c>
-      <c r="BN19" s="21">
-        <f t="shared" ref="BN19" si="119">BM19+1</f>
+      <c r="BR19" s="21">
+        <f t="shared" ref="BR19" si="120">BQ19+1</f>
         <v>177</v>
       </c>
-      <c r="BO19" s="21">
-        <f t="shared" ref="BO19" si="120">BN19+1</f>
+      <c r="BS19" s="21">
+        <f t="shared" ref="BS19" si="121">BR19+1</f>
         <v>178</v>
       </c>
-      <c r="BP19" s="21">
-        <f t="shared" ref="BP19" si="121">BO19+1</f>
+      <c r="BT19" s="21">
+        <f t="shared" ref="BT19" si="122">BS19+1</f>
         <v>179</v>
       </c>
-      <c r="BQ19" s="21">
-        <f t="shared" ref="BQ19" si="122">BP19+1</f>
+      <c r="BU19" s="21">
+        <f t="shared" ref="BU19" si="123">BT19+1</f>
         <v>180</v>
       </c>
-      <c r="BR19" s="21">
-        <f t="shared" ref="BR19" si="123">BQ19+1</f>
+      <c r="BV19" s="21">
+        <f t="shared" ref="BV19" si="124">BU19+1</f>
         <v>181</v>
       </c>
-      <c r="BS19" s="21">
-        <f t="shared" ref="BS19" si="124">BR19+1</f>
+      <c r="BW19" s="21">
+        <f t="shared" ref="BW19" si="125">BV19+1</f>
         <v>182</v>
       </c>
-      <c r="BT19" s="21">
-        <f t="shared" ref="BT19" si="125">BS19+1</f>
+      <c r="BX19" s="21">
+        <f t="shared" ref="BX19" si="126">BW19+1</f>
         <v>183</v>
       </c>
-      <c r="BU19" s="21">
-        <f t="shared" ref="BU19" si="126">BT19+1</f>
+      <c r="BY19" s="21">
+        <f t="shared" ref="BY19" si="127">BX19+1</f>
         <v>184</v>
       </c>
-      <c r="BV19" s="21">
-        <f t="shared" ref="BV19" si="127">BU19+1</f>
+      <c r="BZ19" s="21">
+        <f t="shared" ref="BZ19" si="128">BY19+1</f>
         <v>185</v>
       </c>
-      <c r="BW19" s="21">
-        <f t="shared" ref="BW19" si="128">BV19+1</f>
+      <c r="CA19" s="21">
+        <f t="shared" ref="CA19" si="129">BZ19+1</f>
         <v>186</v>
       </c>
-      <c r="BX19" s="21">
-        <f t="shared" ref="BX19" si="129">BW19+1</f>
+      <c r="CB19" s="21">
+        <f t="shared" ref="CB19" si="130">CA19+1</f>
         <v>187</v>
       </c>
-      <c r="BY19" s="21">
-        <f t="shared" ref="BY19" si="130">BX19+1</f>
+      <c r="CC19" s="21">
+        <f t="shared" ref="CC19" si="131">CB19+1</f>
         <v>188</v>
       </c>
-      <c r="BZ19" s="21">
-        <f t="shared" ref="BZ19" si="131">BY19+1</f>
+      <c r="CD19" s="21">
+        <f t="shared" ref="CD19" si="132">CC19+1</f>
         <v>189</v>
       </c>
-      <c r="CA19" s="21">
-        <f t="shared" ref="CA19" si="132">BZ19+1</f>
+      <c r="CE19" s="21">
+        <f t="shared" ref="CE19" si="133">CD19+1</f>
         <v>190</v>
       </c>
-      <c r="CB19" s="21">
-        <f t="shared" ref="CB19" si="133">CA19+1</f>
+      <c r="CF19" s="21">
+        <f t="shared" ref="CF19" si="134">CE19+1</f>
         <v>191</v>
       </c>
-      <c r="CC19" s="21">
-        <f t="shared" ref="CC19" si="134">CB19+1</f>
+      <c r="CG19" s="21">
+        <f t="shared" ref="CG19" si="135">CF19+1</f>
         <v>192</v>
       </c>
-      <c r="CD19" s="21">
-        <f t="shared" ref="CD19" si="135">CC19+1</f>
+      <c r="CH19" s="21">
+        <f t="shared" ref="CH19" si="136">CG19+1</f>
         <v>193</v>
       </c>
-      <c r="CE19" s="21">
-        <f t="shared" ref="CE19" si="136">CD19+1</f>
+      <c r="CI19" s="21">
+        <f t="shared" ref="CI19" si="137">CH19+1</f>
         <v>194</v>
       </c>
-      <c r="CF19" s="21">
-        <f t="shared" ref="CF19" si="137">CE19+1</f>
+      <c r="CJ19" s="21">
+        <f t="shared" ref="CJ19" si="138">CI19+1</f>
         <v>195</v>
       </c>
-      <c r="CG19" s="21">
-        <f t="shared" ref="CG19" si="138">CF19+1</f>
+      <c r="CK19" s="21">
+        <f t="shared" ref="CK19" si="139">CJ19+1</f>
         <v>196</v>
       </c>
-      <c r="CH19" s="21">
-        <f t="shared" ref="CH19" si="139">CG19+1</f>
+      <c r="CL19" s="21">
+        <f t="shared" ref="CL19" si="140">CK19+1</f>
         <v>197</v>
       </c>
-      <c r="CI19" s="21">
-        <f t="shared" ref="CI19" si="140">CH19+1</f>
+      <c r="CM19" s="21">
+        <f t="shared" ref="CM19" si="141">CL19+1</f>
         <v>198</v>
       </c>
-      <c r="CJ19" s="21">
-        <f t="shared" ref="CJ19" si="141">CI19+1</f>
+      <c r="CN19" s="21">
+        <f t="shared" ref="CN19" si="142">CM19+1</f>
         <v>199</v>
       </c>
-      <c r="CK19" s="21">
-        <f t="shared" ref="CK19" si="142">CJ19+1</f>
+      <c r="CO19" s="21">
+        <f t="shared" ref="CO19" si="143">CN19+1</f>
         <v>200</v>
       </c>
-      <c r="CL19" s="21">
-        <f t="shared" ref="CL19" si="143">CK19+1</f>
+      <c r="CP19" s="21">
+        <f t="shared" ref="CP19" si="144">CO19+1</f>
         <v>201</v>
       </c>
-      <c r="CM19" s="21">
-        <f t="shared" ref="CM19" si="144">CL19+1</f>
+      <c r="CQ19" s="21">
+        <f t="shared" ref="CQ19" si="145">CP19+1</f>
         <v>202</v>
-      </c>
-      <c r="CN19" s="21">
-        <f t="shared" ref="CN19" si="145">CM19+1</f>
-        <v>203</v>
-      </c>
-      <c r="CO19" s="21">
-        <f t="shared" ref="CO19" si="146">CN19+1</f>
-        <v>204</v>
-      </c>
-      <c r="CP19" s="21">
-        <f t="shared" ref="CP19" si="147">CO19+1</f>
-        <v>205</v>
-      </c>
-      <c r="CQ19" s="21">
-        <f t="shared" ref="CQ19" si="148">CP19+1</f>
-        <v>206</v>
       </c>
       <c r="CR19" s="21">
         <f>CQ19+1</f>
+        <v>203</v>
+      </c>
+      <c r="CS19" s="21">
+        <f t="shared" ref="CS19" si="146">CR19+1</f>
+        <v>204</v>
+      </c>
+      <c r="CT19" s="21">
+        <f t="shared" ref="CT19" si="147">CS19+1</f>
+        <v>205</v>
+      </c>
+      <c r="CU19" s="21">
+        <f t="shared" ref="CU19" si="148">CT19+1</f>
+        <v>206</v>
+      </c>
+      <c r="CV19" s="21">
+        <f t="shared" ref="CV19" si="149">CU19+1</f>
         <v>207</v>
       </c>
-      <c r="CS19" s="21">
-        <f t="shared" ref="CS19" si="149">CR19+1</f>
+      <c r="CW19" s="21">
+        <f t="shared" ref="CW19" si="150">CV19+1</f>
         <v>208</v>
       </c>
-      <c r="CT19" s="21">
-        <f t="shared" ref="CT19" si="150">CS19+1</f>
+      <c r="CX19" s="21">
+        <f t="shared" ref="CX19" si="151">CW19+1</f>
         <v>209</v>
       </c>
-      <c r="CU19" s="21">
-        <f t="shared" ref="CU19" si="151">CT19+1</f>
+      <c r="CY19" s="21">
+        <f t="shared" ref="CY19" si="152">CX19+1</f>
         <v>210</v>
       </c>
-      <c r="CV19" s="21">
-        <f t="shared" ref="CV19" si="152">CU19+1</f>
+      <c r="CZ19" s="21">
+        <f t="shared" ref="CZ19" si="153">CY19+1</f>
         <v>211</v>
       </c>
-      <c r="CW19" s="21">
-        <f t="shared" ref="CW19" si="153">CV19+1</f>
+      <c r="DA19" s="21">
+        <f t="shared" ref="DA19" si="154">CZ19+1</f>
         <v>212</v>
       </c>
-      <c r="CX19" s="21">
-        <f t="shared" ref="CX19" si="154">CW19+1</f>
+      <c r="DB19" s="21">
+        <f t="shared" ref="DB19" si="155">DA19+1</f>
         <v>213</v>
       </c>
-      <c r="CY19" s="21">
-        <f t="shared" ref="CY19" si="155">CX19+1</f>
+      <c r="DC19" s="21">
+        <f t="shared" ref="DC19" si="156">DB19+1</f>
         <v>214</v>
       </c>
-      <c r="CZ19" s="21">
-        <f t="shared" ref="CZ19" si="156">CY19+1</f>
+      <c r="DD19" s="21">
+        <f t="shared" ref="DD19" si="157">DC19+1</f>
         <v>215</v>
       </c>
-      <c r="DA19" s="21">
-        <f t="shared" ref="DA19" si="157">CZ19+1</f>
+      <c r="DE19" s="21">
+        <f t="shared" ref="DE19" si="158">DD19+1</f>
         <v>216</v>
       </c>
-      <c r="DB19" s="21">
-        <f t="shared" ref="DB19" si="158">DA19+1</f>
+      <c r="DF19" s="21">
+        <f t="shared" ref="DF19" si="159">DE19+1</f>
         <v>217</v>
       </c>
-      <c r="DC19" s="21">
-        <f t="shared" ref="DC19" si="159">DB19+1</f>
+      <c r="DG19" s="21">
+        <f t="shared" ref="DG19" si="160">DF19+1</f>
         <v>218</v>
       </c>
-      <c r="DD19" s="21">
-        <f t="shared" ref="DD19" si="160">DC19+1</f>
+      <c r="DH19" s="21">
+        <f t="shared" ref="DH19" si="161">DG19+1</f>
         <v>219</v>
       </c>
-      <c r="DE19" s="21">
-        <f t="shared" ref="DE19" si="161">DD19+1</f>
+      <c r="DI19" s="21">
+        <f t="shared" ref="DI19" si="162">DH19+1</f>
         <v>220</v>
       </c>
-      <c r="DF19" s="21">
-        <f t="shared" ref="DF19" si="162">DE19+1</f>
+      <c r="DJ19" s="21">
+        <f t="shared" ref="DJ19" si="163">DI19+1</f>
         <v>221</v>
       </c>
-      <c r="DG19" s="21">
-        <f t="shared" ref="DG19" si="163">DF19+1</f>
+      <c r="DK19" s="21">
+        <f t="shared" ref="DK19" si="164">DJ19+1</f>
         <v>222</v>
       </c>
-      <c r="DH19" s="21">
-        <f t="shared" ref="DH19" si="164">DG19+1</f>
+      <c r="DL19" s="21">
+        <f t="shared" ref="DL19" si="165">DK19+1</f>
         <v>223</v>
       </c>
-      <c r="DI19" s="21">
-        <f t="shared" ref="DI19" si="165">DH19+1</f>
+      <c r="DM19" s="7">
+        <f t="shared" ref="DM19" si="166">DL19+1</f>
         <v>224</v>
-      </c>
-      <c r="DJ19" s="21">
-        <f t="shared" ref="DJ19" si="166">DI19+1</f>
-        <v>225</v>
-      </c>
-      <c r="DK19" s="21">
-        <f t="shared" ref="DK19" si="167">DJ19+1</f>
-        <v>226</v>
-      </c>
-      <c r="DL19" s="21">
-        <f t="shared" ref="DL19" si="168">DK19+1</f>
-        <v>227</v>
-      </c>
-      <c r="DM19" s="7">
-        <f t="shared" ref="DM19" si="169">DL19+1</f>
-        <v>228</v>
       </c>
     </row>
     <row r="20" spans="2:117" ht="42" customHeight="1">
@@ -6127,29 +6234,29 @@
       <c r="M20" s="9"/>
       <c r="N20" s="9"/>
       <c r="O20" s="18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="P20" s="18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="Q20" s="18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="R20" s="18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="S20" s="18"/>
       <c r="T20" s="18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="U20" s="18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="V20" s="18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="W20" s="18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="X20" s="18"/>
       <c r="Y20" s="18"/>
@@ -6158,29 +6265,29 @@
       <c r="AB20" s="18"/>
       <c r="AC20" s="18"/>
       <c r="AD20" s="18" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="AE20" s="18" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="AF20" s="18" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="AG20" s="18" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="AH20" s="18"/>
       <c r="AI20" s="18" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="AJ20" s="18" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="AK20" s="18" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="AL20" s="18" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="AM20" s="18"/>
       <c r="AN20" s="18"/>
@@ -6189,29 +6296,29 @@
       <c r="AQ20" s="18"/>
       <c r="AR20" s="18"/>
       <c r="AS20" s="18" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="AT20" s="18" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="AU20" s="18" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="AV20" s="18" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="AW20" s="18"/>
       <c r="AX20" s="19" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="AY20" s="19" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="AZ20" s="19" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="BA20" s="19" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="BB20" s="18"/>
       <c r="BC20" s="18"/>
@@ -6220,29 +6327,29 @@
       <c r="BF20" s="18"/>
       <c r="BG20" s="18"/>
       <c r="BH20" s="19" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="BI20" s="19" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="BJ20" s="19" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="BK20" s="19" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="BL20" s="18"/>
       <c r="BM20" s="19" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="BN20" s="19" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="BO20" s="19" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="BP20" s="19" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="BQ20" s="18"/>
       <c r="BR20" s="18"/>
@@ -6251,29 +6358,29 @@
       <c r="BU20" s="18"/>
       <c r="BV20" s="18"/>
       <c r="BW20" s="19" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="BX20" s="19" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="BY20" s="19" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="BZ20" s="19" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="CA20" s="18"/>
       <c r="CB20" s="19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="CC20" s="19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="CD20" s="19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="CE20" s="19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="CF20" s="9"/>
       <c r="CG20" s="9"/>
@@ -6306,16 +6413,16 @@
       <c r="DH20" s="9"/>
       <c r="DI20" s="9"/>
       <c r="DJ20" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="DK20" s="18" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="DL20" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="DM20" s="30" t="s">
-        <v>100</v>
+        <v>99</v>
+      </c>
+      <c r="DM20" s="28" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="21" spans="2:117" ht="42" customHeight="1">
@@ -6326,7 +6433,7 @@
         <v>36</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
@@ -6414,76 +6521,76 @@
       <c r="CJ21" s="9"/>
       <c r="CK21" s="9"/>
       <c r="CL21" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="CM21" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="CM21" s="1" t="s">
+      <c r="CN21" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="CN21" s="1" t="s">
+      <c r="CO21" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="CO21" s="1" t="s">
+      <c r="CP21" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="CP21" s="1" t="s">
+      <c r="CQ21" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="CQ21" s="1" t="s">
+      <c r="CR21" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="CR21" s="1" t="s">
+      <c r="CS21" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="CS21" s="1" t="s">
+      <c r="CT21" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="CT21" s="1" t="s">
+      <c r="CU21" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="CU21" s="1" t="s">
+      <c r="CV21" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="CW21" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="CX21" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="CV21" s="1" t="s">
+      <c r="CY21" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="CZ21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="DA21" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="DB21" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="DC21" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="DD21" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="DE21" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="DF21" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="DG21" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="DH21" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="CW21" s="1" t="s">
+      <c r="DI21" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="CX21" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="CY21" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="CZ21" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="DA21" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="DB21" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="DC21" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="DD21" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="DE21" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="DF21" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="DG21" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="DH21" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="DI21" s="1" t="s">
-        <v>164</v>
       </c>
       <c r="DJ21" s="9"/>
       <c r="DK21" s="9"/>
@@ -6492,7 +6599,7 @@
     </row>
     <row r="22" spans="2:117" ht="42" customHeight="1">
       <c r="B22" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C22" s="6">
         <v>36</v>
@@ -6515,14 +6622,14 @@
       <c r="Q22" s="9"/>
       <c r="R22" s="9"/>
       <c r="S22" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="T22" s="9"/>
       <c r="U22" s="9"/>
       <c r="V22" s="9"/>
       <c r="W22" s="9"/>
       <c r="X22" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="Y22" s="9"/>
       <c r="Z22" s="9"/>
@@ -6534,14 +6641,14 @@
       <c r="AF22" s="9"/>
       <c r="AG22" s="9"/>
       <c r="AH22" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="AI22" s="9"/>
       <c r="AJ22" s="9"/>
       <c r="AK22" s="9"/>
       <c r="AL22" s="9"/>
       <c r="AM22" s="9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="AN22" s="9"/>
       <c r="AO22" s="9"/>
@@ -6553,14 +6660,14 @@
       <c r="AU22" s="9"/>
       <c r="AV22" s="9"/>
       <c r="AW22" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="AX22" s="9"/>
       <c r="AY22" s="9"/>
       <c r="AZ22" s="9"/>
       <c r="BA22" s="9"/>
       <c r="BB22" s="12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="BC22" s="9"/>
       <c r="BD22" s="9"/>
@@ -6572,14 +6679,14 @@
       <c r="BJ22" s="9"/>
       <c r="BK22" s="9"/>
       <c r="BL22" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="BM22" s="9"/>
       <c r="BN22" s="9"/>
       <c r="BO22" s="9"/>
       <c r="BP22" s="9"/>
       <c r="BQ22" s="12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="BR22" s="9"/>
       <c r="BS22" s="9"/>
@@ -6591,14 +6698,14 @@
       <c r="BY22" s="9"/>
       <c r="BZ22" s="9"/>
       <c r="CA22" s="12" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="CB22" s="9"/>
       <c r="CC22" s="9"/>
       <c r="CD22" s="9"/>
       <c r="CE22" s="9"/>
       <c r="CF22" s="12" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="CG22" s="9"/>
       <c r="CH22" s="9"/>
@@ -6636,7 +6743,7 @@
     </row>
     <row r="23" spans="2:117" ht="42" customHeight="1">
       <c r="B23" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C23" s="6">
         <v>1</v>
@@ -6645,19 +6752,19 @@
         <v>5</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
@@ -6670,19 +6777,19 @@
       <c r="R23" s="9"/>
       <c r="S23" s="9"/>
       <c r="T23" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="U23" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="V23" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="W23" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="X23" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="Y23" s="9"/>
       <c r="Z23" s="9"/>
@@ -6695,19 +6802,19 @@
       <c r="AG23" s="9"/>
       <c r="AH23" s="9"/>
       <c r="AI23" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="AJ23" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="AK23" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="AL23" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="AM23" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="AN23" s="9"/>
       <c r="AO23" s="9"/>
@@ -6720,19 +6827,19 @@
       <c r="AV23" s="9"/>
       <c r="AW23" s="9"/>
       <c r="AX23" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="AY23" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="AZ23" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="BA23" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="BB23" s="12" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="BC23" s="9"/>
       <c r="BD23" s="9"/>
@@ -6745,19 +6852,19 @@
       <c r="BK23" s="9"/>
       <c r="BL23" s="9"/>
       <c r="BM23" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="BN23" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="BO23" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="BP23" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="BQ23" s="12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="BR23" s="9"/>
       <c r="BS23" s="9"/>
@@ -6770,19 +6877,19 @@
       <c r="BZ23" s="9"/>
       <c r="CA23" s="9"/>
       <c r="CB23" s="12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="CC23" s="12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="CD23" s="12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="CE23" s="12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="CF23" s="12" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="CG23" s="9"/>
       <c r="CH23" s="9"/>
@@ -6820,7 +6927,7 @@
     </row>
     <row r="24" spans="2:117" ht="42" customHeight="1" thickBot="1">
       <c r="B24" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C24" s="14">
         <v>6</v>
@@ -6834,34 +6941,34 @@
       <c r="H24" s="15"/>
       <c r="I24" s="15"/>
       <c r="J24" s="15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="K24" s="15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="L24" s="15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="M24" s="15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="N24" s="15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="O24" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="P24" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="Q24" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="R24" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="S24" s="15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="T24" s="15"/>
       <c r="U24" s="15"/>
@@ -6869,34 +6976,34 @@
       <c r="W24" s="15"/>
       <c r="X24" s="15"/>
       <c r="Y24" s="15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="Z24" s="15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="AA24" s="15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="AB24" s="15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="AC24" s="15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="AD24" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AE24" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AF24" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AG24" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AH24" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AI24" s="15"/>
       <c r="AJ24" s="15"/>
@@ -6904,34 +7011,34 @@
       <c r="AL24" s="15"/>
       <c r="AM24" s="15"/>
       <c r="AN24" s="15" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="AO24" s="15" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="AP24" s="15" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="AQ24" s="15" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="AR24" s="15" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="AS24" s="16" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="AT24" s="16" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="AU24" s="16" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="AV24" s="16" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="AW24" s="16" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="AX24" s="15"/>
       <c r="AY24" s="15"/>
@@ -6939,34 +7046,34 @@
       <c r="BA24" s="15"/>
       <c r="BB24" s="15"/>
       <c r="BC24" s="15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="BD24" s="15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="BE24" s="15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="BF24" s="15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="BG24" s="15" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="BH24" s="16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="BI24" s="16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="BJ24" s="16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="BK24" s="16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="BL24" s="16" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="BM24" s="15"/>
       <c r="BN24" s="15"/>
@@ -6974,34 +7081,34 @@
       <c r="BP24" s="15"/>
       <c r="BQ24" s="15"/>
       <c r="BR24" s="15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="BS24" s="15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="BT24" s="15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="BU24" s="15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="BV24" s="15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="BW24" s="16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="BX24" s="16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="BY24" s="16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="BZ24" s="16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="CA24" s="16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="CB24" s="15"/>
       <c r="CC24" s="15"/>
@@ -7009,19 +7116,19 @@
       <c r="CE24" s="15"/>
       <c r="CF24" s="15"/>
       <c r="CG24" s="16" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="CH24" s="16" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="CI24" s="16" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="CJ24" s="16" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="CK24" s="16" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="CL24" s="15"/>
       <c r="CM24" s="15"/>
@@ -7053,8 +7160,7 @@
       <c r="DM24" s="17"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="E1:DO1"/>
+  <mergeCells count="7">
     <mergeCell ref="E18:DM18"/>
     <mergeCell ref="B3:B8"/>
     <mergeCell ref="C3:C8"/>

</xml_diff>

<commit_message>
Working toward cholesky validation.
</commit_message>
<xml_diff>
--- a/doc/design/schedule.xlsx
+++ b/doc/design/schedule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="22960" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19960" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="165">
   <si>
     <t>sincos</t>
   </si>
@@ -721,8 +721,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="781">
+  <cellStyleXfs count="801">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1612,7 +1632,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="781">
+  <cellStyles count="801">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2003,6 +2023,16 @@
     <cellStyle name="Followed Hyperlink" xfId="776" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="778" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="780" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="782" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="784" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="786" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="788" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="790" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="792" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="794" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="796" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="798" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="800" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2393,6 +2423,16 @@
     <cellStyle name="Hyperlink" xfId="775" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="777" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="779" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="781" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="783" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="785" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="787" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="789" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="791" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="793" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="795" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="797" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="799" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2725,21 +2765,20 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:DM24"/>
+  <dimension ref="A1:DP24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="L12" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="AL1" sqref="AL1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E1" sqref="E1:DL1"/>
+      <selection pane="bottomRight" activeCell="R24" sqref="R24:T24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="4.1640625" defaultRowHeight="42" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.33203125" defaultRowHeight="42" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.33203125" style="8" customWidth="1"/>
     <col min="2" max="4" width="10.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="4.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="4.1640625" style="11"/>
+    <col min="5" max="16384" width="4.33203125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:117" s="2" customFormat="1" ht="42" customHeight="1">
@@ -4366,7 +4405,7 @@
         <v>15</v>
       </c>
       <c r="D9" s="35">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="9"/>
@@ -5622,8 +5661,8 @@
       </c>
       <c r="DM16" s="23"/>
     </row>
-    <row r="17" spans="2:117" ht="42" customHeight="1" thickBot="1"/>
-    <row r="18" spans="2:117" s="2" customFormat="1" ht="42" customHeight="1">
+    <row r="17" spans="2:120" ht="42" customHeight="1" thickBot="1"/>
+    <row r="18" spans="2:120" s="2" customFormat="1" ht="42" customHeight="1">
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -5743,7 +5782,7 @@
       <c r="DL18" s="32"/>
       <c r="DM18" s="33"/>
     </row>
-    <row r="19" spans="2:117" s="2" customFormat="1" ht="42" customHeight="1">
+    <row r="19" spans="2:120" s="2" customFormat="1" ht="42" customHeight="1">
       <c r="B19" s="20" t="s">
         <v>100</v>
       </c>
@@ -6206,7 +6245,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="20" spans="2:117" ht="42" customHeight="1">
+    <row r="20" spans="2:120" ht="42" customHeight="1">
       <c r="B20" s="5" t="s">
         <v>2</v>
       </c>
@@ -6214,170 +6253,170 @@
         <v>15</v>
       </c>
       <c r="D20" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
       <c r="N20" s="9"/>
-      <c r="O20" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="P20" s="18" t="s">
-        <v>133</v>
-      </c>
+      <c r="O20" s="9"/>
       <c r="Q20" s="18" t="s">
         <v>133</v>
       </c>
       <c r="R20" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="S20" s="18"/>
+      <c r="S20" s="18" t="s">
+        <v>133</v>
+      </c>
       <c r="T20" s="18" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="U20" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="V20" s="18" t="s">
-        <v>144</v>
-      </c>
+        <v>133</v>
+      </c>
+      <c r="V20" s="18"/>
       <c r="W20" s="18" t="s">
         <v>144</v>
       </c>
-      <c r="X20" s="18"/>
-      <c r="Y20" s="18"/>
-      <c r="Z20" s="18"/>
+      <c r="X20" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="Y20" s="18" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z20" s="18" t="s">
+        <v>144</v>
+      </c>
       <c r="AA20" s="18"/>
       <c r="AB20" s="18"/>
       <c r="AC20" s="18"/>
-      <c r="AD20" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="AE20" s="18" t="s">
-        <v>134</v>
-      </c>
-      <c r="AF20" s="18" t="s">
-        <v>134</v>
-      </c>
+      <c r="AD20" s="18"/>
+      <c r="AE20" s="18"/>
+      <c r="AF20" s="18"/>
       <c r="AG20" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="AH20" s="18"/>
+      <c r="AH20" s="18" t="s">
+        <v>134</v>
+      </c>
       <c r="AI20" s="18" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="AJ20" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="AK20" s="18" t="s">
-        <v>147</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="AK20" s="18"/>
       <c r="AL20" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="AM20" s="18"/>
-      <c r="AN20" s="18"/>
-      <c r="AO20" s="18"/>
+      <c r="AM20" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="AN20" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="AO20" s="18" t="s">
+        <v>147</v>
+      </c>
       <c r="AP20" s="18"/>
       <c r="AQ20" s="18"/>
       <c r="AR20" s="18"/>
-      <c r="AS20" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="AT20" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="AU20" s="18" t="s">
-        <v>137</v>
-      </c>
+      <c r="AS20" s="18"/>
+      <c r="AT20" s="18"/>
+      <c r="AU20" s="18"/>
       <c r="AV20" s="18" t="s">
         <v>137</v>
       </c>
-      <c r="AW20" s="18"/>
-      <c r="AX20" s="19" t="s">
-        <v>150</v>
-      </c>
-      <c r="AY20" s="19" t="s">
-        <v>150</v>
-      </c>
-      <c r="AZ20" s="19" t="s">
-        <v>150</v>
-      </c>
+      <c r="AW20" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="AX20" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="AY20" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="AZ20" s="18"/>
       <c r="BA20" s="19" t="s">
         <v>150</v>
       </c>
-      <c r="BB20" s="18"/>
-      <c r="BC20" s="18"/>
-      <c r="BD20" s="18"/>
+      <c r="BB20" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="BC20" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="BD20" s="19" t="s">
+        <v>150</v>
+      </c>
       <c r="BE20" s="18"/>
       <c r="BF20" s="18"/>
       <c r="BG20" s="18"/>
-      <c r="BH20" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="BI20" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="BJ20" s="19" t="s">
-        <v>139</v>
-      </c>
+      <c r="BH20" s="18"/>
+      <c r="BI20" s="18"/>
+      <c r="BJ20" s="18"/>
       <c r="BK20" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="BL20" s="18"/>
+      <c r="BL20" s="19" t="s">
+        <v>139</v>
+      </c>
       <c r="BM20" s="19" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="BN20" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="BO20" s="19" t="s">
-        <v>153</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="BO20" s="18"/>
       <c r="BP20" s="19" t="s">
         <v>153</v>
       </c>
-      <c r="BQ20" s="18"/>
-      <c r="BR20" s="18"/>
-      <c r="BS20" s="18"/>
+      <c r="BQ20" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="BR20" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="BS20" s="19" t="s">
+        <v>153</v>
+      </c>
       <c r="BT20" s="18"/>
       <c r="BU20" s="18"/>
       <c r="BV20" s="18"/>
-      <c r="BW20" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="BX20" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="BY20" s="19" t="s">
-        <v>141</v>
-      </c>
+      <c r="BW20" s="18"/>
+      <c r="BX20" s="18"/>
+      <c r="BY20" s="18"/>
       <c r="BZ20" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="CA20" s="18"/>
+      <c r="CA20" s="19" t="s">
+        <v>141</v>
+      </c>
       <c r="CB20" s="19" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="CC20" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="CD20" s="19" t="s">
-        <v>156</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="CD20" s="18"/>
       <c r="CE20" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="CF20" s="9"/>
-      <c r="CG20" s="9"/>
-      <c r="CH20" s="9"/>
+      <c r="CF20" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="CG20" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="CH20" s="19" t="s">
+        <v>156</v>
+      </c>
       <c r="CI20" s="9"/>
       <c r="CJ20" s="9"/>
       <c r="CK20" s="9"/>
@@ -6405,20 +6444,23 @@
       <c r="DG20" s="9"/>
       <c r="DH20" s="9"/>
       <c r="DI20" s="9"/>
-      <c r="DJ20" s="18" t="s">
+      <c r="DJ20" s="9"/>
+      <c r="DK20" s="9"/>
+      <c r="DL20" s="9"/>
+      <c r="DM20" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="DK20" s="18" t="s">
+      <c r="DN20" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="DL20" s="18" t="s">
+      <c r="DO20" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="DM20" s="28" t="s">
+      <c r="DP20" s="28" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="2:117" ht="42" customHeight="1">
+    <row r="21" spans="2:120" ht="42" customHeight="1">
       <c r="B21" s="5" t="s">
         <v>9</v>
       </c>
@@ -6433,17 +6475,14 @@
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
       <c r="K21" s="9"/>
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
       <c r="N21" s="9"/>
       <c r="O21" s="9"/>
-      <c r="P21" s="9"/>
       <c r="Q21" s="9"/>
       <c r="R21" s="9"/>
       <c r="S21" s="9"/>
-      <c r="T21" s="9"/>
       <c r="U21" s="9"/>
       <c r="V21" s="9"/>
       <c r="W21" s="9"/>
@@ -6513,84 +6552,87 @@
       <c r="CI21" s="9"/>
       <c r="CJ21" s="9"/>
       <c r="CK21" s="9"/>
-      <c r="CL21" s="1" t="s">
+      <c r="CL21" s="9"/>
+      <c r="CM21" s="9"/>
+      <c r="CN21" s="9"/>
+      <c r="CO21" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="CM21" s="1" t="s">
+      <c r="CP21" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="CN21" s="1" t="s">
+      <c r="CQ21" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="CO21" s="1" t="s">
+      <c r="CR21" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="CP21" s="1" t="s">
+      <c r="CS21" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="CQ21" s="1" t="s">
+      <c r="CT21" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="CR21" s="1" t="s">
+      <c r="CU21" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="CS21" s="1" t="s">
+      <c r="CV21" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="CT21" s="1" t="s">
+      <c r="CW21" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="CU21" s="1" t="s">
+      <c r="CX21" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="CV21" s="1" t="s">
+      <c r="CY21" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="CW21" s="1" t="s">
+      <c r="CZ21" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="CX21" s="1" t="s">
+      <c r="DA21" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="CY21" s="1" t="s">
+      <c r="DB21" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="CZ21" s="1" t="s">
+      <c r="DC21" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="DA21" s="1" t="s">
+      <c r="DD21" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="DB21" s="1" t="s">
+      <c r="DE21" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="DC21" s="1" t="s">
+      <c r="DF21" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="DD21" s="1" t="s">
+      <c r="DG21" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="DE21" s="1" t="s">
+      <c r="DH21" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="DF21" s="1" t="s">
+      <c r="DI21" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="DG21" s="1" t="s">
+      <c r="DJ21" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="DH21" s="1" t="s">
+      <c r="DK21" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="DI21" s="1" t="s">
+      <c r="DL21" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="DJ21" s="9"/>
-      <c r="DK21" s="9"/>
-      <c r="DL21" s="9"/>
-      <c r="DM21" s="10"/>
+      <c r="DM21" s="9"/>
+      <c r="DN21" s="9"/>
+      <c r="DO21" s="9"/>
+      <c r="DP21" s="10"/>
     </row>
-    <row r="22" spans="2:117" ht="42" customHeight="1">
+    <row r="22" spans="2:120" ht="42" customHeight="1">
       <c r="B22" s="5" t="s">
         <v>76</v>
       </c>
@@ -6605,104 +6647,101 @@
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
       <c r="K22" s="9"/>
       <c r="L22" s="9"/>
       <c r="M22" s="9"/>
       <c r="N22" s="9"/>
       <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
       <c r="Q22" s="9"/>
       <c r="R22" s="9"/>
-      <c r="S22" s="9" t="s">
+      <c r="S22" s="9"/>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="T22" s="9"/>
-      <c r="U22" s="9"/>
-      <c r="V22" s="9"/>
       <c r="W22" s="9"/>
-      <c r="X22" s="9" t="s">
-        <v>145</v>
-      </c>
+      <c r="X22" s="9"/>
       <c r="Y22" s="9"/>
       <c r="Z22" s="9"/>
-      <c r="AA22" s="9"/>
+      <c r="AA22" s="9" t="s">
+        <v>145</v>
+      </c>
       <c r="AB22" s="9"/>
       <c r="AC22" s="9"/>
       <c r="AD22" s="9"/>
       <c r="AE22" s="9"/>
       <c r="AF22" s="9"/>
       <c r="AG22" s="9"/>
-      <c r="AH22" s="9" t="s">
-        <v>136</v>
-      </c>
+      <c r="AH22" s="9"/>
       <c r="AI22" s="9"/>
       <c r="AJ22" s="9"/>
-      <c r="AK22" s="9"/>
+      <c r="AK22" s="9" t="s">
+        <v>136</v>
+      </c>
       <c r="AL22" s="9"/>
-      <c r="AM22" s="9" t="s">
-        <v>148</v>
-      </c>
+      <c r="AM22" s="9"/>
       <c r="AN22" s="9"/>
       <c r="AO22" s="9"/>
-      <c r="AP22" s="9"/>
+      <c r="AP22" s="9" t="s">
+        <v>148</v>
+      </c>
       <c r="AQ22" s="9"/>
       <c r="AR22" s="9"/>
       <c r="AS22" s="9"/>
       <c r="AT22" s="9"/>
       <c r="AU22" s="9"/>
       <c r="AV22" s="9"/>
-      <c r="AW22" s="9" t="s">
-        <v>138</v>
-      </c>
+      <c r="AW22" s="9"/>
       <c r="AX22" s="9"/>
       <c r="AY22" s="9"/>
-      <c r="AZ22" s="9"/>
+      <c r="AZ22" s="9" t="s">
+        <v>138</v>
+      </c>
       <c r="BA22" s="9"/>
-      <c r="BB22" s="12" t="s">
-        <v>151</v>
-      </c>
+      <c r="BB22" s="9"/>
       <c r="BC22" s="9"/>
       <c r="BD22" s="9"/>
-      <c r="BE22" s="9"/>
+      <c r="BE22" s="12" t="s">
+        <v>151</v>
+      </c>
       <c r="BF22" s="9"/>
       <c r="BG22" s="9"/>
       <c r="BH22" s="9"/>
       <c r="BI22" s="9"/>
       <c r="BJ22" s="9"/>
       <c r="BK22" s="9"/>
-      <c r="BL22" s="12" t="s">
-        <v>140</v>
-      </c>
+      <c r="BL22" s="9"/>
       <c r="BM22" s="9"/>
       <c r="BN22" s="9"/>
-      <c r="BO22" s="9"/>
+      <c r="BO22" s="12" t="s">
+        <v>140</v>
+      </c>
       <c r="BP22" s="9"/>
-      <c r="BQ22" s="12" t="s">
-        <v>154</v>
-      </c>
+      <c r="BQ22" s="9"/>
       <c r="BR22" s="9"/>
       <c r="BS22" s="9"/>
-      <c r="BT22" s="9"/>
+      <c r="BT22" s="12" t="s">
+        <v>154</v>
+      </c>
       <c r="BU22" s="9"/>
       <c r="BV22" s="9"/>
       <c r="BW22" s="9"/>
       <c r="BX22" s="9"/>
       <c r="BY22" s="9"/>
       <c r="BZ22" s="9"/>
-      <c r="CA22" s="12" t="s">
-        <v>142</v>
-      </c>
+      <c r="CA22" s="9"/>
       <c r="CB22" s="9"/>
       <c r="CC22" s="9"/>
-      <c r="CD22" s="9"/>
+      <c r="CD22" s="12" t="s">
+        <v>142</v>
+      </c>
       <c r="CE22" s="9"/>
-      <c r="CF22" s="12" t="s">
-        <v>157</v>
-      </c>
+      <c r="CF22" s="9"/>
       <c r="CG22" s="9"/>
       <c r="CH22" s="9"/>
-      <c r="CI22" s="9"/>
+      <c r="CI22" s="12" t="s">
+        <v>157</v>
+      </c>
       <c r="CJ22" s="9"/>
       <c r="CK22" s="9"/>
       <c r="CL22" s="9"/>
@@ -6732,9 +6771,12 @@
       <c r="DJ22" s="9"/>
       <c r="DK22" s="9"/>
       <c r="DL22" s="9"/>
-      <c r="DM22" s="10"/>
+      <c r="DM22" s="9"/>
+      <c r="DN22" s="9"/>
+      <c r="DO22" s="9"/>
+      <c r="DP22" s="10"/>
     </row>
-    <row r="23" spans="2:117" ht="42" customHeight="1">
+    <row r="23" spans="2:120" ht="42" customHeight="1">
       <c r="B23" s="5" t="s">
         <v>77</v>
       </c>
@@ -6742,7 +6784,7 @@
         <v>1</v>
       </c>
       <c r="D23" s="6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>122</v>
@@ -6759,34 +6801,34 @@
       <c r="I23" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="J23" s="9"/>
+      <c r="J23" s="9" t="s">
+        <v>122</v>
+      </c>
       <c r="K23" s="9"/>
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
       <c r="N23" s="9"/>
       <c r="O23" s="9"/>
-      <c r="P23" s="9"/>
       <c r="Q23" s="9"/>
       <c r="R23" s="9"/>
       <c r="S23" s="9"/>
-      <c r="T23" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="U23" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="V23" s="9" t="s">
-        <v>123</v>
-      </c>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9"/>
       <c r="W23" s="9" t="s">
         <v>123</v>
       </c>
       <c r="X23" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="Y23" s="9"/>
-      <c r="Z23" s="9"/>
-      <c r="AA23" s="9"/>
+      <c r="Y23" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="Z23" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="AA23" s="9" t="s">
+        <v>123</v>
+      </c>
       <c r="AB23" s="9"/>
       <c r="AC23" s="9"/>
       <c r="AD23" s="9"/>
@@ -6794,24 +6836,24 @@
       <c r="AF23" s="9"/>
       <c r="AG23" s="9"/>
       <c r="AH23" s="9"/>
-      <c r="AI23" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="AJ23" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="AK23" s="9" t="s">
-        <v>124</v>
-      </c>
+      <c r="AI23" s="9"/>
+      <c r="AJ23" s="9"/>
+      <c r="AK23" s="9"/>
       <c r="AL23" s="9" t="s">
         <v>124</v>
       </c>
       <c r="AM23" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="AN23" s="9"/>
-      <c r="AO23" s="9"/>
-      <c r="AP23" s="9"/>
+      <c r="AN23" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="AO23" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="AP23" s="9" t="s">
+        <v>124</v>
+      </c>
       <c r="AQ23" s="9"/>
       <c r="AR23" s="9"/>
       <c r="AS23" s="9"/>
@@ -6819,24 +6861,24 @@
       <c r="AU23" s="9"/>
       <c r="AV23" s="9"/>
       <c r="AW23" s="9"/>
-      <c r="AX23" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="AY23" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="AZ23" s="12" t="s">
-        <v>125</v>
-      </c>
+      <c r="AX23" s="9"/>
+      <c r="AY23" s="9"/>
+      <c r="AZ23" s="9"/>
       <c r="BA23" s="12" t="s">
         <v>125</v>
       </c>
       <c r="BB23" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="BC23" s="9"/>
-      <c r="BD23" s="9"/>
-      <c r="BE23" s="9"/>
+      <c r="BC23" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="BD23" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="BE23" s="12" t="s">
+        <v>125</v>
+      </c>
       <c r="BF23" s="9"/>
       <c r="BG23" s="9"/>
       <c r="BH23" s="9"/>
@@ -6844,24 +6886,24 @@
       <c r="BJ23" s="9"/>
       <c r="BK23" s="9"/>
       <c r="BL23" s="9"/>
-      <c r="BM23" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="BN23" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="BO23" s="12" t="s">
-        <v>126</v>
-      </c>
+      <c r="BM23" s="9"/>
+      <c r="BN23" s="9"/>
+      <c r="BO23" s="9"/>
       <c r="BP23" s="12" t="s">
         <v>126</v>
       </c>
       <c r="BQ23" s="12" t="s">
         <v>126</v>
       </c>
-      <c r="BR23" s="9"/>
-      <c r="BS23" s="9"/>
-      <c r="BT23" s="9"/>
+      <c r="BR23" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="BS23" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="BT23" s="12" t="s">
+        <v>126</v>
+      </c>
       <c r="BU23" s="9"/>
       <c r="BV23" s="9"/>
       <c r="BW23" s="9"/>
@@ -6869,24 +6911,24 @@
       <c r="BY23" s="9"/>
       <c r="BZ23" s="9"/>
       <c r="CA23" s="9"/>
-      <c r="CB23" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="CC23" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="CD23" s="12" t="s">
-        <v>127</v>
-      </c>
+      <c r="CB23" s="9"/>
+      <c r="CC23" s="9"/>
+      <c r="CD23" s="9"/>
       <c r="CE23" s="12" t="s">
         <v>127</v>
       </c>
       <c r="CF23" s="12" t="s">
         <v>127</v>
       </c>
-      <c r="CG23" s="9"/>
-      <c r="CH23" s="9"/>
-      <c r="CI23" s="9"/>
+      <c r="CG23" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="CH23" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="CI23" s="12" t="s">
+        <v>127</v>
+      </c>
       <c r="CJ23" s="9"/>
       <c r="CK23" s="9"/>
       <c r="CL23" s="9"/>
@@ -6916,9 +6958,12 @@
       <c r="DJ23" s="9"/>
       <c r="DK23" s="9"/>
       <c r="DL23" s="9"/>
-      <c r="DM23" s="10"/>
+      <c r="DM23" s="9"/>
+      <c r="DN23" s="9"/>
+      <c r="DO23" s="9"/>
+      <c r="DP23" s="10"/>
     </row>
-    <row r="24" spans="2:117" ht="42" customHeight="1" thickBot="1">
+    <row r="24" spans="2:120" ht="42" customHeight="1" thickBot="1">
       <c r="B24" s="13" t="s">
         <v>78</v>
       </c>
@@ -6926,16 +6971,13 @@
         <v>6</v>
       </c>
       <c r="D24" s="14">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E24" s="15"/>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
       <c r="H24" s="15"/>
       <c r="I24" s="15"/>
-      <c r="J24" s="15" t="s">
-        <v>128</v>
-      </c>
       <c r="K24" s="15" t="s">
         <v>128</v>
       </c>
@@ -6949,10 +6991,10 @@
         <v>128</v>
       </c>
       <c r="O24" s="15" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="P24" s="15" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="Q24" s="15" t="s">
         <v>143</v>
@@ -6963,20 +7005,20 @@
       <c r="S24" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="T24" s="15"/>
-      <c r="U24" s="15"/>
-      <c r="V24" s="15"/>
+      <c r="T24" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="U24" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="V24" s="15" t="s">
+        <v>143</v>
+      </c>
       <c r="W24" s="15"/>
       <c r="X24" s="15"/>
-      <c r="Y24" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="Z24" s="15" t="s">
-        <v>129</v>
-      </c>
-      <c r="AA24" s="15" t="s">
-        <v>129</v>
-      </c>
+      <c r="Y24" s="15"/>
+      <c r="Z24" s="15"/>
+      <c r="AA24" s="15"/>
       <c r="AB24" s="15" t="s">
         <v>129</v>
       </c>
@@ -6984,13 +7026,13 @@
         <v>129</v>
       </c>
       <c r="AD24" s="15" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="AE24" s="15" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="AF24" s="15" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
       <c r="AG24" s="15" t="s">
         <v>146</v>
@@ -6998,34 +7040,34 @@
       <c r="AH24" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="AI24" s="15"/>
-      <c r="AJ24" s="15"/>
-      <c r="AK24" s="15"/>
+      <c r="AI24" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="AJ24" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="AK24" s="15" t="s">
+        <v>146</v>
+      </c>
       <c r="AL24" s="15"/>
       <c r="AM24" s="15"/>
-      <c r="AN24" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="AO24" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="AP24" s="15" t="s">
-        <v>130</v>
-      </c>
+      <c r="AN24" s="15"/>
+      <c r="AO24" s="15"/>
+      <c r="AP24" s="15"/>
       <c r="AQ24" s="15" t="s">
         <v>130</v>
       </c>
       <c r="AR24" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="AS24" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="AT24" s="16" t="s">
-        <v>149</v>
-      </c>
-      <c r="AU24" s="16" t="s">
-        <v>149</v>
+      <c r="AS24" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="AT24" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="AU24" s="15" t="s">
+        <v>130</v>
       </c>
       <c r="AV24" s="16" t="s">
         <v>149</v>
@@ -7033,34 +7075,34 @@
       <c r="AW24" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="AX24" s="15"/>
-      <c r="AY24" s="15"/>
-      <c r="AZ24" s="15"/>
+      <c r="AX24" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="AY24" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="AZ24" s="16" t="s">
+        <v>149</v>
+      </c>
       <c r="BA24" s="15"/>
       <c r="BB24" s="15"/>
-      <c r="BC24" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="BD24" s="15" t="s">
-        <v>131</v>
-      </c>
-      <c r="BE24" s="15" t="s">
-        <v>131</v>
-      </c>
+      <c r="BC24" s="15"/>
+      <c r="BD24" s="15"/>
+      <c r="BE24" s="15"/>
       <c r="BF24" s="15" t="s">
         <v>131</v>
       </c>
       <c r="BG24" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="BH24" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="BI24" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="BJ24" s="16" t="s">
-        <v>152</v>
+      <c r="BH24" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="BI24" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="BJ24" s="15" t="s">
+        <v>131</v>
       </c>
       <c r="BK24" s="16" t="s">
         <v>152</v>
@@ -7068,34 +7110,34 @@
       <c r="BL24" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="BM24" s="15"/>
-      <c r="BN24" s="15"/>
-      <c r="BO24" s="15"/>
+      <c r="BM24" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="BN24" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="BO24" s="16" t="s">
+        <v>152</v>
+      </c>
       <c r="BP24" s="15"/>
       <c r="BQ24" s="15"/>
-      <c r="BR24" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="BS24" s="15" t="s">
-        <v>132</v>
-      </c>
-      <c r="BT24" s="15" t="s">
-        <v>132</v>
-      </c>
+      <c r="BR24" s="15"/>
+      <c r="BS24" s="15"/>
+      <c r="BT24" s="15"/>
       <c r="BU24" s="15" t="s">
         <v>132</v>
       </c>
       <c r="BV24" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="BW24" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="BX24" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="BY24" s="16" t="s">
-        <v>155</v>
+      <c r="BW24" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="BX24" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="BY24" s="15" t="s">
+        <v>132</v>
       </c>
       <c r="BZ24" s="16" t="s">
         <v>155</v>
@@ -7103,29 +7145,35 @@
       <c r="CA24" s="16" t="s">
         <v>155</v>
       </c>
-      <c r="CB24" s="15"/>
-      <c r="CC24" s="15"/>
-      <c r="CD24" s="15"/>
+      <c r="CB24" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="CC24" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="CD24" s="16" t="s">
+        <v>155</v>
+      </c>
       <c r="CE24" s="15"/>
       <c r="CF24" s="15"/>
-      <c r="CG24" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="CH24" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="CI24" s="16" t="s">
-        <v>158</v>
-      </c>
+      <c r="CG24" s="15"/>
+      <c r="CH24" s="15"/>
+      <c r="CI24" s="15"/>
       <c r="CJ24" s="16" t="s">
         <v>158</v>
       </c>
       <c r="CK24" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="CL24" s="15"/>
-      <c r="CM24" s="15"/>
-      <c r="CN24" s="15"/>
+      <c r="CL24" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="CM24" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="CN24" s="16" t="s">
+        <v>158</v>
+      </c>
       <c r="CO24" s="15"/>
       <c r="CP24" s="15"/>
       <c r="CQ24" s="15"/>
@@ -7150,7 +7198,10 @@
       <c r="DJ24" s="15"/>
       <c r="DK24" s="15"/>
       <c r="DL24" s="15"/>
-      <c r="DM24" s="17"/>
+      <c r="DM24" s="15"/>
+      <c r="DN24" s="15"/>
+      <c r="DO24" s="15"/>
+      <c r="DP24" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Cholesky unit now passes validataion.
</commit_message>
<xml_diff>
--- a/doc/design/schedule.xlsx
+++ b/doc/design/schedule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19960" tabRatio="500"/>
+    <workbookView xWindow="-38400" yWindow="600" windowWidth="33600" windowHeight="19960" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2768,10 +2768,10 @@
   <dimension ref="A1:DP24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="L12" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E17" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="AL1" sqref="AL1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R24" sqref="R24:T24"/>
+      <selection pane="bottomRight" activeCell="W24" sqref="W24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.33203125" defaultRowHeight="42" customHeight="1" x14ac:dyDescent="0"/>
@@ -5793,456 +5793,456 @@
         <v>10</v>
       </c>
       <c r="E19" s="21">
-        <f>MAX(2:2)</f>
-        <v>112</v>
+        <f>MAX(2:2)+1</f>
+        <v>113</v>
       </c>
       <c r="F19" s="21">
         <f t="shared" ref="F19" si="56">E19+1</f>
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G19" s="21">
         <f t="shared" ref="G19" si="57">F19+1</f>
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H19" s="21">
         <f t="shared" ref="H19" si="58">G19+1</f>
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I19" s="21">
         <f t="shared" ref="I19" si="59">H19+1</f>
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="J19" s="21">
         <f t="shared" ref="J19" si="60">I19+1</f>
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="K19" s="21">
         <f t="shared" ref="K19" si="61">J19+1</f>
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="L19" s="21">
         <f t="shared" ref="L19" si="62">K19+1</f>
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="M19" s="21">
         <f t="shared" ref="M19" si="63">L19+1</f>
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="N19" s="21">
         <f t="shared" ref="N19" si="64">M19+1</f>
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="O19" s="21">
         <f t="shared" ref="O19" si="65">N19+1</f>
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="P19" s="21">
         <f t="shared" ref="P19" si="66">O19+1</f>
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="Q19" s="21">
         <f t="shared" ref="Q19" si="67">P19+1</f>
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="R19" s="21">
         <f t="shared" ref="R19" si="68">Q19+1</f>
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="S19" s="21">
         <f t="shared" ref="S19" si="69">R19+1</f>
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="T19" s="21">
         <f t="shared" ref="T19" si="70">S19+1</f>
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="U19" s="21">
         <f t="shared" ref="U19" si="71">T19+1</f>
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="V19" s="21">
         <f t="shared" ref="V19" si="72">U19+1</f>
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="W19" s="21">
         <f t="shared" ref="W19" si="73">V19+1</f>
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="X19" s="21">
         <f t="shared" ref="X19" si="74">W19+1</f>
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="Y19" s="21">
         <f t="shared" ref="Y19" si="75">X19+1</f>
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="Z19" s="21">
         <f t="shared" ref="Z19" si="76">Y19+1</f>
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AA19" s="21">
         <f t="shared" ref="AA19" si="77">Z19+1</f>
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="AB19" s="21">
         <f t="shared" ref="AB19" si="78">AA19+1</f>
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="AC19" s="21">
         <f t="shared" ref="AC19" si="79">AB19+1</f>
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="AD19" s="21">
         <f t="shared" ref="AD19" si="80">AC19+1</f>
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AE19" s="21">
         <f t="shared" ref="AE19" si="81">AD19+1</f>
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="AF19" s="21">
         <f t="shared" ref="AF19" si="82">AE19+1</f>
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="AG19" s="21">
         <f t="shared" ref="AG19" si="83">AF19+1</f>
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="AH19" s="21">
         <f t="shared" ref="AH19" si="84">AG19+1</f>
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="AI19" s="21">
         <f t="shared" ref="AI19" si="85">AH19+1</f>
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="AJ19" s="21">
         <f t="shared" ref="AJ19" si="86">AI19+1</f>
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="AK19" s="21">
         <f t="shared" ref="AK19" si="87">AJ19+1</f>
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="AL19" s="21">
         <f t="shared" ref="AL19" si="88">AK19+1</f>
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="AM19" s="21">
         <f t="shared" ref="AM19" si="89">AL19+1</f>
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="AN19" s="21">
         <f t="shared" ref="AN19" si="90">AM19+1</f>
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AO19" s="21">
         <f t="shared" ref="AO19" si="91">AN19+1</f>
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="AP19" s="21">
         <f t="shared" ref="AP19" si="92">AO19+1</f>
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AQ19" s="21">
         <f t="shared" ref="AQ19" si="93">AP19+1</f>
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="AR19" s="21">
         <f t="shared" ref="AR19" si="94">AQ19+1</f>
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="AS19" s="21">
         <f t="shared" ref="AS19" si="95">AR19+1</f>
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AT19" s="21">
         <f t="shared" ref="AT19" si="96">AS19+1</f>
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AU19" s="21">
         <f t="shared" ref="AU19" si="97">AT19+1</f>
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="AV19" s="21">
         <f t="shared" ref="AV19" si="98">AU19+1</f>
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="AW19" s="21">
         <f t="shared" ref="AW19" si="99">AV19+1</f>
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="AX19" s="21">
         <f t="shared" ref="AX19" si="100">AW19+1</f>
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="AY19" s="21">
         <f t="shared" ref="AY19" si="101">AX19+1</f>
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="AZ19" s="21">
         <f t="shared" ref="AZ19" si="102">AY19+1</f>
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="BA19" s="21">
         <f t="shared" ref="BA19" si="103">AZ19+1</f>
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="BB19" s="21">
         <f t="shared" ref="BB19" si="104">BA19+1</f>
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="BC19" s="21">
         <f t="shared" ref="BC19" si="105">BB19+1</f>
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="BD19" s="21">
         <f t="shared" ref="BD19" si="106">BC19+1</f>
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="BE19" s="21">
         <f t="shared" ref="BE19" si="107">BD19+1</f>
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="BF19" s="21">
         <f t="shared" ref="BF19" si="108">BE19+1</f>
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="BG19" s="21">
         <f t="shared" ref="BG19" si="109">BF19+1</f>
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="BH19" s="21">
         <f t="shared" ref="BH19" si="110">BG19+1</f>
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="BI19" s="21">
         <f t="shared" ref="BI19" si="111">BH19+1</f>
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="BJ19" s="21">
         <f t="shared" ref="BJ19" si="112">BI19+1</f>
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="BK19" s="21">
         <f t="shared" ref="BK19" si="113">BJ19+1</f>
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="BL19" s="21">
         <f t="shared" ref="BL19" si="114">BK19+1</f>
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="BM19" s="21">
         <f t="shared" ref="BM19" si="115">BL19+1</f>
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="BN19" s="21">
         <f t="shared" ref="BN19" si="116">BM19+1</f>
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="BO19" s="21">
         <f t="shared" ref="BO19" si="117">BN19+1</f>
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="BP19" s="21">
         <f t="shared" ref="BP19" si="118">BO19+1</f>
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="BQ19" s="21">
         <f t="shared" ref="BQ19" si="119">BP19+1</f>
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="BR19" s="21">
         <f t="shared" ref="BR19" si="120">BQ19+1</f>
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="BS19" s="21">
         <f t="shared" ref="BS19" si="121">BR19+1</f>
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="BT19" s="21">
         <f t="shared" ref="BT19" si="122">BS19+1</f>
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="BU19" s="21">
         <f t="shared" ref="BU19" si="123">BT19+1</f>
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="BV19" s="21">
         <f t="shared" ref="BV19" si="124">BU19+1</f>
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="BW19" s="21">
         <f t="shared" ref="BW19" si="125">BV19+1</f>
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="BX19" s="21">
         <f t="shared" ref="BX19" si="126">BW19+1</f>
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="BY19" s="21">
         <f t="shared" ref="BY19" si="127">BX19+1</f>
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="BZ19" s="21">
         <f t="shared" ref="BZ19" si="128">BY19+1</f>
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="CA19" s="21">
         <f t="shared" ref="CA19" si="129">BZ19+1</f>
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="CB19" s="21">
         <f t="shared" ref="CB19" si="130">CA19+1</f>
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="CC19" s="21">
         <f t="shared" ref="CC19" si="131">CB19+1</f>
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="CD19" s="21">
         <f t="shared" ref="CD19" si="132">CC19+1</f>
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="CE19" s="21">
         <f t="shared" ref="CE19" si="133">CD19+1</f>
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="CF19" s="21">
         <f t="shared" ref="CF19" si="134">CE19+1</f>
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="CG19" s="21">
         <f t="shared" ref="CG19" si="135">CF19+1</f>
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="CH19" s="21">
         <f t="shared" ref="CH19" si="136">CG19+1</f>
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="CI19" s="21">
         <f t="shared" ref="CI19" si="137">CH19+1</f>
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="CJ19" s="21">
         <f t="shared" ref="CJ19" si="138">CI19+1</f>
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="CK19" s="21">
         <f t="shared" ref="CK19" si="139">CJ19+1</f>
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="CL19" s="21">
         <f t="shared" ref="CL19" si="140">CK19+1</f>
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="CM19" s="21">
         <f t="shared" ref="CM19" si="141">CL19+1</f>
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="CN19" s="21">
         <f t="shared" ref="CN19" si="142">CM19+1</f>
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="CO19" s="21">
         <f t="shared" ref="CO19" si="143">CN19+1</f>
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="CP19" s="21">
         <f t="shared" ref="CP19" si="144">CO19+1</f>
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="CQ19" s="21">
         <f t="shared" ref="CQ19" si="145">CP19+1</f>
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="CR19" s="21">
         <f>CQ19+1</f>
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="CS19" s="21">
         <f t="shared" ref="CS19" si="146">CR19+1</f>
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="CT19" s="21">
         <f t="shared" ref="CT19" si="147">CS19+1</f>
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="CU19" s="21">
         <f t="shared" ref="CU19" si="148">CT19+1</f>
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="CV19" s="21">
         <f t="shared" ref="CV19" si="149">CU19+1</f>
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="CW19" s="21">
         <f t="shared" ref="CW19" si="150">CV19+1</f>
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="CX19" s="21">
         <f t="shared" ref="CX19" si="151">CW19+1</f>
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="CY19" s="21">
         <f t="shared" ref="CY19" si="152">CX19+1</f>
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="CZ19" s="21">
         <f t="shared" ref="CZ19" si="153">CY19+1</f>
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="DA19" s="21">
         <f t="shared" ref="DA19" si="154">CZ19+1</f>
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="DB19" s="21">
         <f t="shared" ref="DB19" si="155">DA19+1</f>
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="DC19" s="21">
         <f t="shared" ref="DC19" si="156">DB19+1</f>
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="DD19" s="21">
         <f t="shared" ref="DD19" si="157">DC19+1</f>
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="DE19" s="21">
         <f t="shared" ref="DE19" si="158">DD19+1</f>
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="DF19" s="21">
         <f t="shared" ref="DF19" si="159">DE19+1</f>
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="DG19" s="21">
         <f t="shared" ref="DG19" si="160">DF19+1</f>
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="DH19" s="21">
         <f t="shared" ref="DH19" si="161">DG19+1</f>
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="DI19" s="21">
         <f t="shared" ref="DI19" si="162">DH19+1</f>
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="DJ19" s="21">
         <f t="shared" ref="DJ19" si="163">DI19+1</f>
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="DK19" s="21">
         <f t="shared" ref="DK19" si="164">DJ19+1</f>
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="DL19" s="21">
         <f t="shared" ref="DL19" si="165">DK19+1</f>
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="DM19" s="7">
         <f t="shared" ref="DM19" si="166">DL19+1</f>
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="20" spans="2:120" ht="42" customHeight="1">

</xml_diff>

<commit_message>
Top level hardware integration. Next, assess fixed point accuracy.
</commit_message>
<xml_diff>
--- a/doc/design/schedule.xlsx
+++ b/doc/design/schedule.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19960" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="165">
   <si>
     <t>sincos</t>
   </si>
@@ -725,19 +725,19 @@
         <color auto="1"/>
       </left>
       <right/>
-      <top style="thin">
+      <top/>
+      <bottom style="thin">
         <color auto="1"/>
-      </top>
-      <bottom/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top/>
+      <bottom style="thin">
         <color auto="1"/>
-      </top>
-      <bottom/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -745,14 +745,14 @@
       <right style="medium">
         <color auto="1"/>
       </right>
-      <top style="thin">
+      <top/>
+      <bottom style="thin">
         <color auto="1"/>
-      </top>
-      <bottom/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="851">
+  <cellStyleXfs count="867">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1604,8 +1604,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1673,12 +1689,6 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1686,6 +1696,36 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1700,29 +1740,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="851">
+  <cellStyles count="867">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2148,6 +2167,14 @@
     <cellStyle name="Followed Hyperlink" xfId="846" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="848" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="850" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="852" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="854" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="856" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="858" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="860" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="862" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="864" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="866" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2573,6 +2600,14 @@
     <cellStyle name="Hyperlink" xfId="845" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="847" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="849" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="851" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="853" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="855" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="857" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="859" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="861" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="863" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="865" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2905,13 +2940,13 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:EE29"/>
+  <dimension ref="A1:EG29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E22" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E11" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="AL1" sqref="AL1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B30" sqref="B30"/>
+      <selection pane="bottomRight" activeCell="E18" sqref="E18:EG18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.33203125" defaultRowHeight="42" customHeight="1" x14ac:dyDescent="0"/>
@@ -2925,572 +2960,572 @@
       <c r="B1" s="3"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="28"/>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="28"/>
-      <c r="AD1" s="28"/>
-      <c r="AE1" s="28"/>
-      <c r="AF1" s="28"/>
-      <c r="AG1" s="28"/>
-      <c r="AH1" s="28"/>
-      <c r="AI1" s="28"/>
-      <c r="AJ1" s="28"/>
-      <c r="AK1" s="28"/>
-      <c r="AL1" s="28"/>
-      <c r="AM1" s="28"/>
-      <c r="AN1" s="28"/>
-      <c r="AO1" s="28"/>
-      <c r="AP1" s="28"/>
-      <c r="AQ1" s="28"/>
-      <c r="AR1" s="28"/>
-      <c r="AS1" s="28"/>
-      <c r="AT1" s="28"/>
-      <c r="AU1" s="28"/>
-      <c r="AV1" s="28"/>
-      <c r="AW1" s="28"/>
-      <c r="AX1" s="28"/>
-      <c r="AY1" s="28"/>
-      <c r="AZ1" s="28"/>
-      <c r="BA1" s="28"/>
-      <c r="BB1" s="28"/>
-      <c r="BC1" s="28"/>
-      <c r="BD1" s="28"/>
-      <c r="BE1" s="28"/>
-      <c r="BF1" s="28"/>
-      <c r="BG1" s="28"/>
-      <c r="BH1" s="28"/>
-      <c r="BI1" s="28"/>
-      <c r="BJ1" s="28"/>
-      <c r="BK1" s="28"/>
-      <c r="BL1" s="28"/>
-      <c r="BM1" s="28"/>
-      <c r="BN1" s="28"/>
-      <c r="BO1" s="28"/>
-      <c r="BP1" s="28"/>
-      <c r="BQ1" s="28"/>
-      <c r="BR1" s="28"/>
-      <c r="BS1" s="28"/>
-      <c r="BT1" s="28"/>
-      <c r="BU1" s="28"/>
-      <c r="BV1" s="28"/>
-      <c r="BW1" s="28"/>
-      <c r="BX1" s="28"/>
-      <c r="BY1" s="28"/>
-      <c r="BZ1" s="28"/>
-      <c r="CA1" s="28"/>
-      <c r="CB1" s="28"/>
-      <c r="CC1" s="28"/>
-      <c r="CD1" s="28"/>
-      <c r="CE1" s="28"/>
-      <c r="CF1" s="28"/>
-      <c r="CG1" s="28"/>
-      <c r="CH1" s="28"/>
-      <c r="CI1" s="28"/>
-      <c r="CJ1" s="28"/>
-      <c r="CK1" s="28"/>
-      <c r="CL1" s="28"/>
-      <c r="CM1" s="28"/>
-      <c r="CN1" s="28"/>
-      <c r="CO1" s="28"/>
-      <c r="CP1" s="28"/>
-      <c r="CQ1" s="28"/>
-      <c r="CR1" s="28"/>
-      <c r="CS1" s="28"/>
-      <c r="CT1" s="28"/>
-      <c r="CU1" s="28"/>
-      <c r="CV1" s="28"/>
-      <c r="CW1" s="28"/>
-      <c r="CX1" s="28"/>
-      <c r="CY1" s="28"/>
-      <c r="CZ1" s="28"/>
-      <c r="DA1" s="28"/>
-      <c r="DB1" s="28"/>
-      <c r="DC1" s="28"/>
-      <c r="DD1" s="28"/>
-      <c r="DE1" s="28"/>
-      <c r="DF1" s="28"/>
-      <c r="DG1" s="28"/>
-      <c r="DH1" s="28"/>
-      <c r="DI1" s="28"/>
-      <c r="DJ1" s="28"/>
-      <c r="DK1" s="28"/>
-      <c r="DL1" s="29"/>
-      <c r="DM1" s="25"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36"/>
+      <c r="W1" s="36"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="36"/>
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="36"/>
+      <c r="AC1" s="36"/>
+      <c r="AD1" s="36"/>
+      <c r="AE1" s="36"/>
+      <c r="AF1" s="36"/>
+      <c r="AG1" s="36"/>
+      <c r="AH1" s="36"/>
+      <c r="AI1" s="36"/>
+      <c r="AJ1" s="36"/>
+      <c r="AK1" s="36"/>
+      <c r="AL1" s="36"/>
+      <c r="AM1" s="36"/>
+      <c r="AN1" s="36"/>
+      <c r="AO1" s="36"/>
+      <c r="AP1" s="36"/>
+      <c r="AQ1" s="36"/>
+      <c r="AR1" s="36"/>
+      <c r="AS1" s="36"/>
+      <c r="AT1" s="36"/>
+      <c r="AU1" s="36"/>
+      <c r="AV1" s="36"/>
+      <c r="AW1" s="36"/>
+      <c r="AX1" s="36"/>
+      <c r="AY1" s="36"/>
+      <c r="AZ1" s="36"/>
+      <c r="BA1" s="36"/>
+      <c r="BB1" s="36"/>
+      <c r="BC1" s="36"/>
+      <c r="BD1" s="36"/>
+      <c r="BE1" s="36"/>
+      <c r="BF1" s="36"/>
+      <c r="BG1" s="36"/>
+      <c r="BH1" s="36"/>
+      <c r="BI1" s="36"/>
+      <c r="BJ1" s="36"/>
+      <c r="BK1" s="36"/>
+      <c r="BL1" s="36"/>
+      <c r="BM1" s="36"/>
+      <c r="BN1" s="36"/>
+      <c r="BO1" s="36"/>
+      <c r="BP1" s="36"/>
+      <c r="BQ1" s="36"/>
+      <c r="BR1" s="36"/>
+      <c r="BS1" s="36"/>
+      <c r="BT1" s="36"/>
+      <c r="BU1" s="36"/>
+      <c r="BV1" s="36"/>
+      <c r="BW1" s="36"/>
+      <c r="BX1" s="36"/>
+      <c r="BY1" s="36"/>
+      <c r="BZ1" s="36"/>
+      <c r="CA1" s="36"/>
+      <c r="CB1" s="36"/>
+      <c r="CC1" s="36"/>
+      <c r="CD1" s="36"/>
+      <c r="CE1" s="36"/>
+      <c r="CF1" s="36"/>
+      <c r="CG1" s="36"/>
+      <c r="CH1" s="36"/>
+      <c r="CI1" s="36"/>
+      <c r="CJ1" s="36"/>
+      <c r="CK1" s="36"/>
+      <c r="CL1" s="36"/>
+      <c r="CM1" s="36"/>
+      <c r="CN1" s="36"/>
+      <c r="CO1" s="36"/>
+      <c r="CP1" s="36"/>
+      <c r="CQ1" s="36"/>
+      <c r="CR1" s="36"/>
+      <c r="CS1" s="36"/>
+      <c r="CT1" s="36"/>
+      <c r="CU1" s="36"/>
+      <c r="CV1" s="36"/>
+      <c r="CW1" s="36"/>
+      <c r="CX1" s="36"/>
+      <c r="CY1" s="36"/>
+      <c r="CZ1" s="36"/>
+      <c r="DA1" s="36"/>
+      <c r="DB1" s="36"/>
+      <c r="DC1" s="36"/>
+      <c r="DD1" s="36"/>
+      <c r="DE1" s="36"/>
+      <c r="DF1" s="36"/>
+      <c r="DG1" s="36"/>
+      <c r="DH1" s="36"/>
+      <c r="DI1" s="36"/>
+      <c r="DJ1" s="36"/>
+      <c r="DK1" s="36"/>
+      <c r="DL1" s="37"/>
+      <c r="DM1" s="23"/>
     </row>
     <row r="2" spans="2:117" s="2" customFormat="1" ht="42" customHeight="1">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="24" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="24">
+      <c r="E2" s="25">
         <v>1</v>
       </c>
-      <c r="F2" s="24">
+      <c r="F2" s="25">
         <f>E2+1</f>
         <v>2</v>
       </c>
-      <c r="G2" s="24">
+      <c r="G2" s="25">
         <f t="shared" ref="G2:BR2" si="0">F2+1</f>
         <v>3</v>
       </c>
-      <c r="H2" s="24">
+      <c r="H2" s="25">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="I2" s="24">
+      <c r="I2" s="25">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="J2" s="24">
+      <c r="J2" s="25">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="K2" s="24">
+      <c r="K2" s="25">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="L2" s="24">
+      <c r="L2" s="25">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="M2" s="24">
+      <c r="M2" s="25">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="N2" s="24">
+      <c r="N2" s="25">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="O2" s="24">
+      <c r="O2" s="25">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="P2" s="24">
+      <c r="P2" s="25">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="Q2" s="24">
+      <c r="Q2" s="25">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="R2" s="24">
+      <c r="R2" s="25">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="S2" s="24">
+      <c r="S2" s="25">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="T2" s="24">
+      <c r="T2" s="25">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="U2" s="24">
+      <c r="U2" s="25">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="V2" s="24">
+      <c r="V2" s="25">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="W2" s="24">
+      <c r="W2" s="25">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="X2" s="24">
+      <c r="X2" s="25">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="Y2" s="24">
+      <c r="Y2" s="25">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="Z2" s="24">
+      <c r="Z2" s="25">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="AA2" s="24">
+      <c r="AA2" s="25">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="AB2" s="24">
+      <c r="AB2" s="25">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AC2" s="24">
+      <c r="AC2" s="25">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="AD2" s="24">
+      <c r="AD2" s="25">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="AE2" s="24">
+      <c r="AE2" s="25">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="AF2" s="24">
+      <c r="AF2" s="25">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="AG2" s="24">
+      <c r="AG2" s="25">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="AH2" s="24">
+      <c r="AH2" s="25">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="AI2" s="24">
+      <c r="AI2" s="25">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="AJ2" s="24">
+      <c r="AJ2" s="25">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="AK2" s="24">
+      <c r="AK2" s="25">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="AL2" s="24">
+      <c r="AL2" s="25">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="AM2" s="24">
+      <c r="AM2" s="25">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="AN2" s="24">
+      <c r="AN2" s="25">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="AO2" s="24">
+      <c r="AO2" s="25">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="AP2" s="24">
+      <c r="AP2" s="25">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="AQ2" s="24">
+      <c r="AQ2" s="25">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="AR2" s="24">
+      <c r="AR2" s="25">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="AS2" s="24">
+      <c r="AS2" s="25">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="AT2" s="24">
+      <c r="AT2" s="25">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="AU2" s="24">
+      <c r="AU2" s="25">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="AV2" s="24">
+      <c r="AV2" s="25">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="AW2" s="24">
+      <c r="AW2" s="25">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="AX2" s="24">
+      <c r="AX2" s="25">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="AY2" s="24">
+      <c r="AY2" s="25">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="AZ2" s="24">
+      <c r="AZ2" s="25">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="BA2" s="24">
+      <c r="BA2" s="25">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="BB2" s="24">
+      <c r="BB2" s="25">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="BC2" s="24">
+      <c r="BC2" s="25">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="BD2" s="24">
+      <c r="BD2" s="25">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="BE2" s="24">
+      <c r="BE2" s="25">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="BF2" s="24">
+      <c r="BF2" s="25">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="BG2" s="24">
+      <c r="BG2" s="25">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="BH2" s="24">
+      <c r="BH2" s="25">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="BI2" s="24">
+      <c r="BI2" s="25">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-      <c r="BJ2" s="24">
+      <c r="BJ2" s="25">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="BK2" s="24">
+      <c r="BK2" s="25">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="BL2" s="24">
+      <c r="BL2" s="25">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="BM2" s="24">
+      <c r="BM2" s="25">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="BN2" s="24">
+      <c r="BN2" s="25">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="BO2" s="24">
+      <c r="BO2" s="25">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="BP2" s="24">
+      <c r="BP2" s="25">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="BQ2" s="24">
+      <c r="BQ2" s="25">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-      <c r="BR2" s="24">
+      <c r="BR2" s="25">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="BS2" s="24">
+      <c r="BS2" s="25">
         <f t="shared" ref="BS2:BZ2" si="1">BR2+1</f>
         <v>67</v>
       </c>
-      <c r="BT2" s="24">
+      <c r="BT2" s="25">
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
-      <c r="BU2" s="24">
+      <c r="BU2" s="25">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-      <c r="BV2" s="24">
+      <c r="BV2" s="25">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
-      <c r="BW2" s="24">
+      <c r="BW2" s="25">
         <f t="shared" si="1"/>
         <v>71</v>
       </c>
-      <c r="BX2" s="24">
+      <c r="BX2" s="25">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
-      <c r="BY2" s="24">
+      <c r="BY2" s="25">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
-      <c r="BZ2" s="24">
+      <c r="BZ2" s="25">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
-      <c r="CA2" s="24">
+      <c r="CA2" s="25">
         <f t="shared" ref="CA2" si="2">BZ2+1</f>
         <v>75</v>
       </c>
-      <c r="CB2" s="24">
+      <c r="CB2" s="25">
         <f t="shared" ref="CB2" si="3">CA2+1</f>
         <v>76</v>
       </c>
-      <c r="CC2" s="24">
+      <c r="CC2" s="25">
         <f t="shared" ref="CC2" si="4">CB2+1</f>
         <v>77</v>
       </c>
-      <c r="CD2" s="24">
+      <c r="CD2" s="25">
         <f t="shared" ref="CD2" si="5">CC2+1</f>
         <v>78</v>
       </c>
-      <c r="CE2" s="24">
+      <c r="CE2" s="25">
         <f t="shared" ref="CE2" si="6">CD2+1</f>
         <v>79</v>
       </c>
-      <c r="CF2" s="24">
+      <c r="CF2" s="25">
         <f t="shared" ref="CF2" si="7">CE2+1</f>
         <v>80</v>
       </c>
-      <c r="CG2" s="24">
+      <c r="CG2" s="25">
         <f t="shared" ref="CG2" si="8">CF2+1</f>
         <v>81</v>
       </c>
-      <c r="CH2" s="24">
+      <c r="CH2" s="25">
         <f t="shared" ref="CH2" si="9">CG2+1</f>
         <v>82</v>
       </c>
-      <c r="CI2" s="24">
+      <c r="CI2" s="25">
         <f t="shared" ref="CI2" si="10">CH2+1</f>
         <v>83</v>
       </c>
-      <c r="CJ2" s="24">
+      <c r="CJ2" s="25">
         <f t="shared" ref="CJ2" si="11">CI2+1</f>
         <v>84</v>
       </c>
-      <c r="CK2" s="24">
+      <c r="CK2" s="25">
         <f t="shared" ref="CK2" si="12">CJ2+1</f>
         <v>85</v>
       </c>
-      <c r="CL2" s="24">
+      <c r="CL2" s="25">
         <f t="shared" ref="CL2" si="13">CK2+1</f>
         <v>86</v>
       </c>
-      <c r="CM2" s="24">
+      <c r="CM2" s="25">
         <f t="shared" ref="CM2" si="14">CL2+1</f>
         <v>87</v>
       </c>
-      <c r="CN2" s="24">
+      <c r="CN2" s="25">
         <f t="shared" ref="CN2" si="15">CM2+1</f>
         <v>88</v>
       </c>
-      <c r="CO2" s="24">
+      <c r="CO2" s="25">
         <f t="shared" ref="CO2" si="16">CN2+1</f>
         <v>89</v>
       </c>
-      <c r="CP2" s="24">
+      <c r="CP2" s="25">
         <f t="shared" ref="CP2" si="17">CO2+1</f>
         <v>90</v>
       </c>
-      <c r="CQ2" s="24">
+      <c r="CQ2" s="25">
         <f t="shared" ref="CQ2" si="18">CP2+1</f>
         <v>91</v>
       </c>
-      <c r="CR2" s="24">
+      <c r="CR2" s="25">
         <f t="shared" ref="CR2" si="19">CQ2+1</f>
         <v>92</v>
       </c>
-      <c r="CS2" s="24">
+      <c r="CS2" s="25">
         <f t="shared" ref="CS2" si="20">CR2+1</f>
         <v>93</v>
       </c>
-      <c r="CT2" s="24">
+      <c r="CT2" s="25">
         <f t="shared" ref="CT2" si="21">CS2+1</f>
         <v>94</v>
       </c>
-      <c r="CU2" s="24">
+      <c r="CU2" s="25">
         <f t="shared" ref="CU2" si="22">CT2+1</f>
         <v>95</v>
       </c>
-      <c r="CV2" s="24">
+      <c r="CV2" s="25">
         <f t="shared" ref="CV2" si="23">CU2+1</f>
         <v>96</v>
       </c>
-      <c r="CW2" s="24">
+      <c r="CW2" s="25">
         <f t="shared" ref="CW2" si="24">CV2+1</f>
         <v>97</v>
       </c>
-      <c r="CX2" s="24">
+      <c r="CX2" s="25">
         <f t="shared" ref="CX2" si="25">CW2+1</f>
         <v>98</v>
       </c>
-      <c r="CY2" s="24">
+      <c r="CY2" s="25">
         <f t="shared" ref="CY2" si="26">CX2+1</f>
         <v>99</v>
       </c>
-      <c r="CZ2" s="24">
+      <c r="CZ2" s="25">
         <f t="shared" ref="CZ2" si="27">CY2+1</f>
         <v>100</v>
       </c>
-      <c r="DA2" s="24">
+      <c r="DA2" s="25">
         <f t="shared" ref="DA2" si="28">CZ2+1</f>
         <v>101</v>
       </c>
-      <c r="DB2" s="24">
+      <c r="DB2" s="25">
         <f t="shared" ref="DB2" si="29">DA2+1</f>
         <v>102</v>
       </c>
-      <c r="DC2" s="24">
+      <c r="DC2" s="25">
         <f t="shared" ref="DC2" si="30">DB2+1</f>
         <v>103</v>
       </c>
-      <c r="DD2" s="24">
+      <c r="DD2" s="25">
         <f t="shared" ref="DD2" si="31">DC2+1</f>
         <v>104</v>
       </c>
-      <c r="DE2" s="24">
+      <c r="DE2" s="25">
         <f t="shared" ref="DE2" si="32">DD2+1</f>
         <v>105</v>
       </c>
-      <c r="DF2" s="24">
+      <c r="DF2" s="25">
         <f t="shared" ref="DF2" si="33">DE2+1</f>
         <v>106</v>
       </c>
-      <c r="DG2" s="24">
+      <c r="DG2" s="25">
         <f t="shared" ref="DG2" si="34">DF2+1</f>
         <v>107</v>
       </c>
-      <c r="DH2" s="24">
+      <c r="DH2" s="25">
         <f t="shared" ref="DH2" si="35">DG2+1</f>
         <v>108</v>
       </c>
-      <c r="DI2" s="24">
+      <c r="DI2" s="25">
         <f t="shared" ref="DI2" si="36">DH2+1</f>
         <v>109</v>
       </c>
-      <c r="DJ2" s="24">
+      <c r="DJ2" s="25">
         <f t="shared" ref="DJ2" si="37">DI2+1</f>
         <v>110</v>
       </c>
-      <c r="DK2" s="24">
+      <c r="DK2" s="25">
         <f t="shared" ref="DK2" si="38">DJ2+1</f>
         <v>111</v>
       </c>
@@ -3501,13 +3536,13 @@
       <c r="DM2" s="17"/>
     </row>
     <row r="3" spans="2:117" ht="42" customHeight="1">
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="31">
+      <c r="C3" s="39">
         <v>2</v>
       </c>
-      <c r="D3" s="31">
+      <c r="D3" s="39">
         <v>23</v>
       </c>
       <c r="E3" s="7" t="s">
@@ -3692,9 +3727,9 @@
       <c r="DM3" s="18"/>
     </row>
     <row r="4" spans="2:117" ht="42" customHeight="1">
-      <c r="B4" s="30"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7" t="s">
         <v>4</v>
@@ -3866,9 +3901,9 @@
       <c r="DM4" s="18"/>
     </row>
     <row r="5" spans="2:117" ht="42" customHeight="1">
-      <c r="B5" s="30"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7" t="s">
@@ -4044,9 +4079,9 @@
       <c r="DM5" s="18"/>
     </row>
     <row r="6" spans="2:117" ht="42" customHeight="1">
-      <c r="B6" s="30"/>
-      <c r="C6" s="31"/>
-      <c r="D6" s="31"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -4209,9 +4244,9 @@
       <c r="DM6" s="18"/>
     </row>
     <row r="7" spans="2:117" ht="42" customHeight="1">
-      <c r="B7" s="30"/>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -4373,9 +4408,9 @@
       <c r="DM7" s="18"/>
     </row>
     <row r="8" spans="2:117" ht="42" customHeight="1">
-      <c r="B8" s="30"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="39"/>
+      <c r="D8" s="39"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
@@ -4538,13 +4573,13 @@
       <c r="DM8" s="18"/>
     </row>
     <row r="9" spans="2:117" ht="42" customHeight="1">
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="31">
+      <c r="C9" s="39">
         <v>15</v>
       </c>
-      <c r="D9" s="31">
+      <c r="D9" s="39">
         <v>5</v>
       </c>
       <c r="E9" s="7"/>
@@ -4724,9 +4759,9 @@
       <c r="DM9" s="18"/>
     </row>
     <row r="10" spans="2:117" ht="42" customHeight="1">
-      <c r="B10" s="30"/>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="39"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
@@ -4853,9 +4888,9 @@
       <c r="DM10" s="18"/>
     </row>
     <row r="11" spans="2:117" ht="42" customHeight="1">
-      <c r="B11" s="30"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="39"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
@@ -4984,9 +5019,9 @@
       <c r="DM11" s="18"/>
     </row>
     <row r="12" spans="2:117" ht="42" customHeight="1">
-      <c r="B12" s="30"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
@@ -5112,9 +5147,9 @@
       <c r="DM12" s="18"/>
     </row>
     <row r="13" spans="2:117" ht="42" customHeight="1">
-      <c r="B13" s="30"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="39"/>
+      <c r="D13" s="39"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
@@ -5242,9 +5277,9 @@
       <c r="DM13" s="18"/>
     </row>
     <row r="14" spans="2:117" ht="42" customHeight="1">
-      <c r="B14" s="30"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="39"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
@@ -5370,13 +5405,13 @@
       <c r="DM14" s="18"/>
     </row>
     <row r="15" spans="2:117" ht="42" customHeight="1">
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="24">
+      <c r="C15" s="25">
         <v>36</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="D15" s="25" t="s">
         <v>163</v>
       </c>
       <c r="E15" s="7"/>
@@ -5769,7 +5804,9 @@
       <c r="CL16" s="13"/>
       <c r="CM16" s="13"/>
       <c r="CN16" s="13"/>
-      <c r="CO16" s="13"/>
+      <c r="CO16" s="13" t="s">
+        <v>102</v>
+      </c>
       <c r="CP16" s="13" t="s">
         <v>102</v>
       </c>
@@ -5795,946 +5832,958 @@
       <c r="DH16" s="13"/>
       <c r="DI16" s="13"/>
       <c r="DJ16" s="13"/>
-      <c r="DK16" s="13"/>
-      <c r="DL16" s="15" t="s">
+      <c r="DK16" s="13" t="s">
         <v>105</v>
       </c>
+      <c r="DL16" s="15"/>
       <c r="DM16" s="18"/>
     </row>
-    <row r="17" spans="2:135" ht="42" customHeight="1" thickBot="1"/>
-    <row r="18" spans="2:135" s="2" customFormat="1" ht="42" customHeight="1">
+    <row r="17" spans="2:137" ht="42" customHeight="1" thickBot="1"/>
+    <row r="18" spans="2:137" s="2" customFormat="1" ht="42" customHeight="1">
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="28" t="s">
+      <c r="E18" s="36" t="s">
         <v>101</v>
       </c>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="28"/>
-      <c r="N18" s="28"/>
-      <c r="O18" s="28"/>
-      <c r="P18" s="28"/>
-      <c r="Q18" s="28"/>
-      <c r="R18" s="28"/>
-      <c r="S18" s="28"/>
-      <c r="T18" s="28"/>
-      <c r="U18" s="28"/>
-      <c r="V18" s="28"/>
-      <c r="W18" s="28"/>
-      <c r="X18" s="28"/>
-      <c r="Y18" s="28"/>
-      <c r="Z18" s="28"/>
-      <c r="AA18" s="28"/>
-      <c r="AB18" s="28"/>
-      <c r="AC18" s="28"/>
-      <c r="AD18" s="28"/>
-      <c r="AE18" s="28"/>
-      <c r="AF18" s="28"/>
-      <c r="AG18" s="28"/>
-      <c r="AH18" s="28"/>
-      <c r="AI18" s="28"/>
-      <c r="AJ18" s="28"/>
-      <c r="AK18" s="28"/>
-      <c r="AL18" s="28"/>
-      <c r="AM18" s="28"/>
-      <c r="AN18" s="28"/>
-      <c r="AO18" s="28"/>
-      <c r="AP18" s="28"/>
-      <c r="AQ18" s="28"/>
-      <c r="AR18" s="28"/>
-      <c r="AS18" s="28"/>
-      <c r="AT18" s="28"/>
-      <c r="AU18" s="28"/>
-      <c r="AV18" s="28"/>
-      <c r="AW18" s="28"/>
-      <c r="AX18" s="28"/>
-      <c r="AY18" s="28"/>
-      <c r="AZ18" s="28"/>
-      <c r="BA18" s="28"/>
-      <c r="BB18" s="28"/>
-      <c r="BC18" s="28"/>
-      <c r="BD18" s="28"/>
-      <c r="BE18" s="28"/>
-      <c r="BF18" s="28"/>
-      <c r="BG18" s="28"/>
-      <c r="BH18" s="28"/>
-      <c r="BI18" s="28"/>
-      <c r="BJ18" s="28"/>
-      <c r="BK18" s="28"/>
-      <c r="BL18" s="28"/>
-      <c r="BM18" s="28"/>
-      <c r="BN18" s="28"/>
-      <c r="BO18" s="28"/>
-      <c r="BP18" s="28"/>
-      <c r="BQ18" s="28"/>
-      <c r="BR18" s="28"/>
-      <c r="BS18" s="28"/>
-      <c r="BT18" s="28"/>
-      <c r="BU18" s="28"/>
-      <c r="BV18" s="28"/>
-      <c r="BW18" s="28"/>
-      <c r="BX18" s="28"/>
-      <c r="BY18" s="28"/>
-      <c r="BZ18" s="28"/>
-      <c r="CA18" s="28"/>
-      <c r="CB18" s="28"/>
-      <c r="CC18" s="28"/>
-      <c r="CD18" s="28"/>
-      <c r="CE18" s="28"/>
-      <c r="CF18" s="28"/>
-      <c r="CG18" s="28"/>
-      <c r="CH18" s="28"/>
-      <c r="CI18" s="28"/>
-      <c r="CJ18" s="28"/>
-      <c r="CK18" s="28"/>
-      <c r="CL18" s="28"/>
-      <c r="CM18" s="28"/>
-      <c r="CN18" s="28"/>
-      <c r="CO18" s="28"/>
-      <c r="CP18" s="28"/>
-      <c r="CQ18" s="28"/>
-      <c r="CR18" s="28"/>
-      <c r="CS18" s="28"/>
-      <c r="CT18" s="28"/>
-      <c r="CU18" s="28"/>
-      <c r="CV18" s="28"/>
-      <c r="CW18" s="28"/>
-      <c r="CX18" s="28"/>
-      <c r="CY18" s="28"/>
-      <c r="CZ18" s="28"/>
-      <c r="DA18" s="28"/>
-      <c r="DB18" s="28"/>
-      <c r="DC18" s="28"/>
-      <c r="DD18" s="28"/>
-      <c r="DE18" s="28"/>
-      <c r="DF18" s="28"/>
-      <c r="DG18" s="28"/>
-      <c r="DH18" s="28"/>
-      <c r="DI18" s="28"/>
-      <c r="DJ18" s="28"/>
-      <c r="DK18" s="28"/>
-      <c r="DL18" s="28"/>
-      <c r="DM18" s="28"/>
-      <c r="DN18" s="28"/>
-      <c r="DO18" s="28"/>
-      <c r="DP18" s="28"/>
-      <c r="DQ18" s="28"/>
-      <c r="DR18" s="28"/>
-      <c r="DS18" s="28"/>
-      <c r="DT18" s="28"/>
-      <c r="DU18" s="28"/>
-      <c r="DV18" s="28"/>
-      <c r="DW18" s="28"/>
-      <c r="DX18" s="28"/>
-      <c r="DY18" s="28"/>
-      <c r="DZ18" s="28"/>
-      <c r="EA18" s="28"/>
-      <c r="EB18" s="28"/>
-      <c r="EC18" s="28"/>
-      <c r="ED18" s="28"/>
-      <c r="EE18" s="29"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="36"/>
+      <c r="M18" s="36"/>
+      <c r="N18" s="36"/>
+      <c r="O18" s="36"/>
+      <c r="P18" s="36"/>
+      <c r="Q18" s="36"/>
+      <c r="R18" s="36"/>
+      <c r="S18" s="36"/>
+      <c r="T18" s="36"/>
+      <c r="U18" s="36"/>
+      <c r="V18" s="36"/>
+      <c r="W18" s="36"/>
+      <c r="X18" s="36"/>
+      <c r="Y18" s="36"/>
+      <c r="Z18" s="36"/>
+      <c r="AA18" s="36"/>
+      <c r="AB18" s="36"/>
+      <c r="AC18" s="36"/>
+      <c r="AD18" s="36"/>
+      <c r="AE18" s="36"/>
+      <c r="AF18" s="36"/>
+      <c r="AG18" s="36"/>
+      <c r="AH18" s="36"/>
+      <c r="AI18" s="36"/>
+      <c r="AJ18" s="36"/>
+      <c r="AK18" s="36"/>
+      <c r="AL18" s="36"/>
+      <c r="AM18" s="36"/>
+      <c r="AN18" s="36"/>
+      <c r="AO18" s="36"/>
+      <c r="AP18" s="36"/>
+      <c r="AQ18" s="36"/>
+      <c r="AR18" s="36"/>
+      <c r="AS18" s="36"/>
+      <c r="AT18" s="36"/>
+      <c r="AU18" s="36"/>
+      <c r="AV18" s="36"/>
+      <c r="AW18" s="36"/>
+      <c r="AX18" s="36"/>
+      <c r="AY18" s="36"/>
+      <c r="AZ18" s="36"/>
+      <c r="BA18" s="36"/>
+      <c r="BB18" s="36"/>
+      <c r="BC18" s="36"/>
+      <c r="BD18" s="36"/>
+      <c r="BE18" s="36"/>
+      <c r="BF18" s="36"/>
+      <c r="BG18" s="36"/>
+      <c r="BH18" s="36"/>
+      <c r="BI18" s="36"/>
+      <c r="BJ18" s="36"/>
+      <c r="BK18" s="36"/>
+      <c r="BL18" s="36"/>
+      <c r="BM18" s="36"/>
+      <c r="BN18" s="36"/>
+      <c r="BO18" s="36"/>
+      <c r="BP18" s="36"/>
+      <c r="BQ18" s="36"/>
+      <c r="BR18" s="36"/>
+      <c r="BS18" s="36"/>
+      <c r="BT18" s="36"/>
+      <c r="BU18" s="36"/>
+      <c r="BV18" s="36"/>
+      <c r="BW18" s="36"/>
+      <c r="BX18" s="36"/>
+      <c r="BY18" s="36"/>
+      <c r="BZ18" s="36"/>
+      <c r="CA18" s="36"/>
+      <c r="CB18" s="36"/>
+      <c r="CC18" s="36"/>
+      <c r="CD18" s="36"/>
+      <c r="CE18" s="36"/>
+      <c r="CF18" s="36"/>
+      <c r="CG18" s="36"/>
+      <c r="CH18" s="36"/>
+      <c r="CI18" s="36"/>
+      <c r="CJ18" s="36"/>
+      <c r="CK18" s="36"/>
+      <c r="CL18" s="36"/>
+      <c r="CM18" s="36"/>
+      <c r="CN18" s="36"/>
+      <c r="CO18" s="36"/>
+      <c r="CP18" s="36"/>
+      <c r="CQ18" s="36"/>
+      <c r="CR18" s="36"/>
+      <c r="CS18" s="36"/>
+      <c r="CT18" s="36"/>
+      <c r="CU18" s="36"/>
+      <c r="CV18" s="36"/>
+      <c r="CW18" s="36"/>
+      <c r="CX18" s="36"/>
+      <c r="CY18" s="36"/>
+      <c r="CZ18" s="36"/>
+      <c r="DA18" s="36"/>
+      <c r="DB18" s="36"/>
+      <c r="DC18" s="36"/>
+      <c r="DD18" s="36"/>
+      <c r="DE18" s="36"/>
+      <c r="DF18" s="36"/>
+      <c r="DG18" s="36"/>
+      <c r="DH18" s="36"/>
+      <c r="DI18" s="36"/>
+      <c r="DJ18" s="36"/>
+      <c r="DK18" s="36"/>
+      <c r="DL18" s="36"/>
+      <c r="DM18" s="36"/>
+      <c r="DN18" s="36"/>
+      <c r="DO18" s="36"/>
+      <c r="DP18" s="36"/>
+      <c r="DQ18" s="36"/>
+      <c r="DR18" s="36"/>
+      <c r="DS18" s="36"/>
+      <c r="DT18" s="36"/>
+      <c r="DU18" s="36"/>
+      <c r="DV18" s="36"/>
+      <c r="DW18" s="36"/>
+      <c r="DX18" s="36"/>
+      <c r="DY18" s="36"/>
+      <c r="DZ18" s="36"/>
+      <c r="EA18" s="36"/>
+      <c r="EB18" s="36"/>
+      <c r="EC18" s="36"/>
+      <c r="ED18" s="36"/>
+      <c r="EE18" s="36"/>
+      <c r="EF18" s="36"/>
+      <c r="EG18" s="37"/>
     </row>
-    <row r="19" spans="2:135" s="2" customFormat="1" ht="42" customHeight="1" thickBot="1">
-      <c r="B19" s="32" t="s">
+    <row r="19" spans="2:137" s="2" customFormat="1" ht="42" customHeight="1" thickBot="1">
+      <c r="B19" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="33" t="s">
+      <c r="D19" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="33">
+      <c r="E19" s="12">
         <f>MAX(2:2)+1</f>
         <v>113</v>
       </c>
-      <c r="F19" s="33">
+      <c r="F19" s="12">
         <f t="shared" ref="F19" si="56">E19+1</f>
         <v>114</v>
       </c>
-      <c r="G19" s="33">
+      <c r="G19" s="12">
         <f t="shared" ref="G19" si="57">F19+1</f>
         <v>115</v>
       </c>
-      <c r="H19" s="33">
+      <c r="H19" s="12">
         <f t="shared" ref="H19" si="58">G19+1</f>
         <v>116</v>
       </c>
-      <c r="I19" s="33">
+      <c r="I19" s="12">
         <f t="shared" ref="I19" si="59">H19+1</f>
         <v>117</v>
       </c>
-      <c r="J19" s="33">
+      <c r="J19" s="12">
         <f t="shared" ref="J19" si="60">I19+1</f>
         <v>118</v>
       </c>
-      <c r="K19" s="33">
+      <c r="K19" s="12">
         <f t="shared" ref="K19" si="61">J19+1</f>
         <v>119</v>
       </c>
-      <c r="L19" s="33">
+      <c r="L19" s="12">
         <f t="shared" ref="L19" si="62">K19+1</f>
         <v>120</v>
       </c>
-      <c r="M19" s="33">
+      <c r="M19" s="12">
         <f t="shared" ref="M19" si="63">L19+1</f>
         <v>121</v>
       </c>
-      <c r="N19" s="33">
+      <c r="N19" s="12">
         <f t="shared" ref="N19" si="64">M19+1</f>
         <v>122</v>
       </c>
-      <c r="O19" s="33">
+      <c r="O19" s="12">
         <f t="shared" ref="O19" si="65">N19+1</f>
         <v>123</v>
       </c>
-      <c r="P19" s="33">
+      <c r="P19" s="12">
         <f t="shared" ref="P19" si="66">O19+1</f>
         <v>124</v>
       </c>
-      <c r="Q19" s="33">
+      <c r="Q19" s="12">
         <f t="shared" ref="Q19" si="67">P19+1</f>
         <v>125</v>
       </c>
-      <c r="R19" s="33">
+      <c r="R19" s="12">
         <f t="shared" ref="R19" si="68">Q19+1</f>
         <v>126</v>
       </c>
-      <c r="S19" s="33">
+      <c r="S19" s="12">
         <f t="shared" ref="S19" si="69">R19+1</f>
         <v>127</v>
       </c>
-      <c r="T19" s="33">
+      <c r="T19" s="12">
         <f t="shared" ref="T19" si="70">S19+1</f>
         <v>128</v>
       </c>
-      <c r="U19" s="33">
+      <c r="U19" s="12">
         <f t="shared" ref="U19" si="71">T19+1</f>
         <v>129</v>
       </c>
-      <c r="V19" s="33">
+      <c r="V19" s="12">
         <f t="shared" ref="V19" si="72">U19+1</f>
         <v>130</v>
       </c>
-      <c r="W19" s="33">
+      <c r="W19" s="12">
         <f t="shared" ref="W19" si="73">V19+1</f>
         <v>131</v>
       </c>
-      <c r="X19" s="33">
+      <c r="X19" s="12">
         <f t="shared" ref="X19" si="74">W19+1</f>
         <v>132</v>
       </c>
-      <c r="Y19" s="33">
+      <c r="Y19" s="12">
         <f t="shared" ref="Y19" si="75">X19+1</f>
         <v>133</v>
       </c>
-      <c r="Z19" s="33">
+      <c r="Z19" s="12">
         <f t="shared" ref="Z19" si="76">Y19+1</f>
         <v>134</v>
       </c>
-      <c r="AA19" s="33">
+      <c r="AA19" s="12">
         <f t="shared" ref="AA19" si="77">Z19+1</f>
         <v>135</v>
       </c>
-      <c r="AB19" s="33">
+      <c r="AB19" s="12">
         <f t="shared" ref="AB19" si="78">AA19+1</f>
         <v>136</v>
       </c>
-      <c r="AC19" s="33">
+      <c r="AC19" s="12">
         <f t="shared" ref="AC19" si="79">AB19+1</f>
         <v>137</v>
       </c>
-      <c r="AD19" s="33">
+      <c r="AD19" s="12">
         <f t="shared" ref="AD19" si="80">AC19+1</f>
         <v>138</v>
       </c>
-      <c r="AE19" s="33">
+      <c r="AE19" s="12">
         <f t="shared" ref="AE19" si="81">AD19+1</f>
         <v>139</v>
       </c>
-      <c r="AF19" s="33">
+      <c r="AF19" s="12">
         <f t="shared" ref="AF19" si="82">AE19+1</f>
         <v>140</v>
       </c>
-      <c r="AG19" s="33">
+      <c r="AG19" s="12">
         <f t="shared" ref="AG19" si="83">AF19+1</f>
         <v>141</v>
       </c>
-      <c r="AH19" s="33">
+      <c r="AH19" s="12">
         <f t="shared" ref="AH19" si="84">AG19+1</f>
         <v>142</v>
       </c>
-      <c r="AI19" s="33">
+      <c r="AI19" s="12">
         <f t="shared" ref="AI19" si="85">AH19+1</f>
         <v>143</v>
       </c>
-      <c r="AJ19" s="33">
+      <c r="AJ19" s="12">
         <f t="shared" ref="AJ19" si="86">AI19+1</f>
         <v>144</v>
       </c>
-      <c r="AK19" s="33">
+      <c r="AK19" s="12">
         <f t="shared" ref="AK19" si="87">AJ19+1</f>
         <v>145</v>
       </c>
-      <c r="AL19" s="33">
+      <c r="AL19" s="12">
         <f t="shared" ref="AL19" si="88">AK19+1</f>
         <v>146</v>
       </c>
-      <c r="AM19" s="33">
+      <c r="AM19" s="12">
         <f t="shared" ref="AM19" si="89">AL19+1</f>
         <v>147</v>
       </c>
-      <c r="AN19" s="33">
+      <c r="AN19" s="12">
         <f t="shared" ref="AN19" si="90">AM19+1</f>
         <v>148</v>
       </c>
-      <c r="AO19" s="33">
+      <c r="AO19" s="12">
         <f t="shared" ref="AO19" si="91">AN19+1</f>
         <v>149</v>
       </c>
-      <c r="AP19" s="33">
+      <c r="AP19" s="12">
         <f t="shared" ref="AP19" si="92">AO19+1</f>
         <v>150</v>
       </c>
-      <c r="AQ19" s="33">
+      <c r="AQ19" s="12">
         <f t="shared" ref="AQ19" si="93">AP19+1</f>
         <v>151</v>
       </c>
-      <c r="AR19" s="33">
+      <c r="AR19" s="12">
         <f t="shared" ref="AR19" si="94">AQ19+1</f>
         <v>152</v>
       </c>
-      <c r="AS19" s="33">
+      <c r="AS19" s="12">
         <f t="shared" ref="AS19" si="95">AR19+1</f>
         <v>153</v>
       </c>
-      <c r="AT19" s="33">
+      <c r="AT19" s="12">
         <f t="shared" ref="AT19" si="96">AS19+1</f>
         <v>154</v>
       </c>
-      <c r="AU19" s="33">
+      <c r="AU19" s="12">
         <f t="shared" ref="AU19" si="97">AT19+1</f>
         <v>155</v>
       </c>
-      <c r="AV19" s="33">
+      <c r="AV19" s="12">
         <f t="shared" ref="AV19" si="98">AU19+1</f>
         <v>156</v>
       </c>
-      <c r="AW19" s="33">
+      <c r="AW19" s="12">
         <f t="shared" ref="AW19" si="99">AV19+1</f>
         <v>157</v>
       </c>
-      <c r="AX19" s="33">
+      <c r="AX19" s="12">
         <f t="shared" ref="AX19" si="100">AW19+1</f>
         <v>158</v>
       </c>
-      <c r="AY19" s="33">
+      <c r="AY19" s="12">
         <f t="shared" ref="AY19" si="101">AX19+1</f>
         <v>159</v>
       </c>
-      <c r="AZ19" s="33">
+      <c r="AZ19" s="12">
         <f t="shared" ref="AZ19" si="102">AY19+1</f>
         <v>160</v>
       </c>
-      <c r="BA19" s="33">
+      <c r="BA19" s="12">
         <f t="shared" ref="BA19" si="103">AZ19+1</f>
         <v>161</v>
       </c>
-      <c r="BB19" s="33">
+      <c r="BB19" s="12">
         <f t="shared" ref="BB19" si="104">BA19+1</f>
         <v>162</v>
       </c>
-      <c r="BC19" s="33">
+      <c r="BC19" s="12">
         <f t="shared" ref="BC19" si="105">BB19+1</f>
         <v>163</v>
       </c>
-      <c r="BD19" s="33">
+      <c r="BD19" s="12">
         <f t="shared" ref="BD19" si="106">BC19+1</f>
         <v>164</v>
       </c>
-      <c r="BE19" s="33">
+      <c r="BE19" s="12">
         <f t="shared" ref="BE19" si="107">BD19+1</f>
         <v>165</v>
       </c>
-      <c r="BF19" s="33">
+      <c r="BF19" s="12">
         <f t="shared" ref="BF19" si="108">BE19+1</f>
         <v>166</v>
       </c>
-      <c r="BG19" s="33">
+      <c r="BG19" s="12">
         <f t="shared" ref="BG19" si="109">BF19+1</f>
         <v>167</v>
       </c>
-      <c r="BH19" s="33">
+      <c r="BH19" s="12">
         <f t="shared" ref="BH19" si="110">BG19+1</f>
         <v>168</v>
       </c>
-      <c r="BI19" s="33">
+      <c r="BI19" s="12">
         <f t="shared" ref="BI19" si="111">BH19+1</f>
         <v>169</v>
       </c>
-      <c r="BJ19" s="33">
+      <c r="BJ19" s="12">
         <f t="shared" ref="BJ19" si="112">BI19+1</f>
         <v>170</v>
       </c>
-      <c r="BK19" s="33">
+      <c r="BK19" s="12">
         <f t="shared" ref="BK19" si="113">BJ19+1</f>
         <v>171</v>
       </c>
-      <c r="BL19" s="33">
+      <c r="BL19" s="12">
         <f t="shared" ref="BL19" si="114">BK19+1</f>
         <v>172</v>
       </c>
-      <c r="BM19" s="33">
+      <c r="BM19" s="12">
         <f t="shared" ref="BM19" si="115">BL19+1</f>
         <v>173</v>
       </c>
-      <c r="BN19" s="33">
+      <c r="BN19" s="12">
         <f t="shared" ref="BN19" si="116">BM19+1</f>
         <v>174</v>
       </c>
-      <c r="BO19" s="33">
+      <c r="BO19" s="12">
         <f t="shared" ref="BO19" si="117">BN19+1</f>
         <v>175</v>
       </c>
-      <c r="BP19" s="33">
+      <c r="BP19" s="12">
         <f t="shared" ref="BP19" si="118">BO19+1</f>
         <v>176</v>
       </c>
-      <c r="BQ19" s="33">
+      <c r="BQ19" s="12">
         <f t="shared" ref="BQ19" si="119">BP19+1</f>
         <v>177</v>
       </c>
-      <c r="BR19" s="33">
+      <c r="BR19" s="12">
         <f t="shared" ref="BR19" si="120">BQ19+1</f>
         <v>178</v>
       </c>
-      <c r="BS19" s="33">
+      <c r="BS19" s="12">
         <f t="shared" ref="BS19" si="121">BR19+1</f>
         <v>179</v>
       </c>
-      <c r="BT19" s="33">
+      <c r="BT19" s="12">
         <f t="shared" ref="BT19" si="122">BS19+1</f>
         <v>180</v>
       </c>
-      <c r="BU19" s="33">
+      <c r="BU19" s="12">
         <f t="shared" ref="BU19" si="123">BT19+1</f>
         <v>181</v>
       </c>
-      <c r="BV19" s="33">
+      <c r="BV19" s="12">
         <f t="shared" ref="BV19" si="124">BU19+1</f>
         <v>182</v>
       </c>
-      <c r="BW19" s="33">
+      <c r="BW19" s="12">
         <f t="shared" ref="BW19" si="125">BV19+1</f>
         <v>183</v>
       </c>
-      <c r="BX19" s="33">
+      <c r="BX19" s="12">
         <f t="shared" ref="BX19" si="126">BW19+1</f>
         <v>184</v>
       </c>
-      <c r="BY19" s="33">
+      <c r="BY19" s="12">
         <f t="shared" ref="BY19" si="127">BX19+1</f>
         <v>185</v>
       </c>
-      <c r="BZ19" s="33">
+      <c r="BZ19" s="12">
         <f t="shared" ref="BZ19" si="128">BY19+1</f>
         <v>186</v>
       </c>
-      <c r="CA19" s="33">
+      <c r="CA19" s="12">
         <f t="shared" ref="CA19" si="129">BZ19+1</f>
         <v>187</v>
       </c>
-      <c r="CB19" s="33">
+      <c r="CB19" s="12">
         <f t="shared" ref="CB19" si="130">CA19+1</f>
         <v>188</v>
       </c>
-      <c r="CC19" s="33">
+      <c r="CC19" s="12">
         <f t="shared" ref="CC19" si="131">CB19+1</f>
         <v>189</v>
       </c>
-      <c r="CD19" s="33">
+      <c r="CD19" s="12">
         <f t="shared" ref="CD19" si="132">CC19+1</f>
         <v>190</v>
       </c>
-      <c r="CE19" s="33">
+      <c r="CE19" s="12">
         <f t="shared" ref="CE19" si="133">CD19+1</f>
         <v>191</v>
       </c>
-      <c r="CF19" s="33">
+      <c r="CF19" s="12">
         <f t="shared" ref="CF19" si="134">CE19+1</f>
         <v>192</v>
       </c>
-      <c r="CG19" s="33">
+      <c r="CG19" s="12">
         <f t="shared" ref="CG19" si="135">CF19+1</f>
         <v>193</v>
       </c>
-      <c r="CH19" s="33">
+      <c r="CH19" s="12">
         <f t="shared" ref="CH19" si="136">CG19+1</f>
         <v>194</v>
       </c>
-      <c r="CI19" s="33">
+      <c r="CI19" s="12">
         <f t="shared" ref="CI19" si="137">CH19+1</f>
         <v>195</v>
       </c>
-      <c r="CJ19" s="33">
+      <c r="CJ19" s="12">
         <f t="shared" ref="CJ19" si="138">CI19+1</f>
         <v>196</v>
       </c>
-      <c r="CK19" s="33">
+      <c r="CK19" s="12">
         <f t="shared" ref="CK19" si="139">CJ19+1</f>
         <v>197</v>
       </c>
-      <c r="CL19" s="33">
+      <c r="CL19" s="12">
         <f t="shared" ref="CL19" si="140">CK19+1</f>
         <v>198</v>
       </c>
-      <c r="CM19" s="33">
+      <c r="CM19" s="12">
         <f t="shared" ref="CM19" si="141">CL19+1</f>
         <v>199</v>
       </c>
-      <c r="CN19" s="33">
+      <c r="CN19" s="12">
         <f t="shared" ref="CN19" si="142">CM19+1</f>
         <v>200</v>
       </c>
-      <c r="CO19" s="33">
+      <c r="CO19" s="12">
         <f t="shared" ref="CO19" si="143">CN19+1</f>
         <v>201</v>
       </c>
-      <c r="CP19" s="33">
+      <c r="CP19" s="12">
         <f t="shared" ref="CP19" si="144">CO19+1</f>
         <v>202</v>
       </c>
-      <c r="CQ19" s="33">
+      <c r="CQ19" s="12">
         <f t="shared" ref="CQ19" si="145">CP19+1</f>
         <v>203</v>
       </c>
-      <c r="CR19" s="33">
+      <c r="CR19" s="12">
         <f>CQ19+1</f>
         <v>204</v>
       </c>
-      <c r="CS19" s="33">
+      <c r="CS19" s="12">
         <f t="shared" ref="CS19" si="146">CR19+1</f>
         <v>205</v>
       </c>
-      <c r="CT19" s="33">
+      <c r="CT19" s="12">
         <f t="shared" ref="CT19" si="147">CS19+1</f>
         <v>206</v>
       </c>
-      <c r="CU19" s="33">
+      <c r="CU19" s="12">
         <f t="shared" ref="CU19" si="148">CT19+1</f>
         <v>207</v>
       </c>
-      <c r="CV19" s="33">
+      <c r="CV19" s="12">
         <f t="shared" ref="CV19" si="149">CU19+1</f>
         <v>208</v>
       </c>
-      <c r="CW19" s="33">
+      <c r="CW19" s="12">
         <f t="shared" ref="CW19" si="150">CV19+1</f>
         <v>209</v>
       </c>
-      <c r="CX19" s="33">
+      <c r="CX19" s="12">
         <f t="shared" ref="CX19" si="151">CW19+1</f>
         <v>210</v>
       </c>
-      <c r="CY19" s="33">
+      <c r="CY19" s="12">
         <f t="shared" ref="CY19" si="152">CX19+1</f>
         <v>211</v>
       </c>
-      <c r="CZ19" s="33">
+      <c r="CZ19" s="12">
         <f t="shared" ref="CZ19" si="153">CY19+1</f>
         <v>212</v>
       </c>
-      <c r="DA19" s="33">
+      <c r="DA19" s="12">
         <f t="shared" ref="DA19" si="154">CZ19+1</f>
         <v>213</v>
       </c>
-      <c r="DB19" s="33">
+      <c r="DB19" s="12">
         <f t="shared" ref="DB19" si="155">DA19+1</f>
         <v>214</v>
       </c>
-      <c r="DC19" s="33">
+      <c r="DC19" s="12">
         <f t="shared" ref="DC19" si="156">DB19+1</f>
         <v>215</v>
       </c>
-      <c r="DD19" s="33">
+      <c r="DD19" s="12">
         <f t="shared" ref="DD19" si="157">DC19+1</f>
         <v>216</v>
       </c>
-      <c r="DE19" s="33">
+      <c r="DE19" s="12">
         <f t="shared" ref="DE19" si="158">DD19+1</f>
         <v>217</v>
       </c>
-      <c r="DF19" s="33">
+      <c r="DF19" s="12">
         <f t="shared" ref="DF19" si="159">DE19+1</f>
         <v>218</v>
       </c>
-      <c r="DG19" s="33">
+      <c r="DG19" s="12">
         <f t="shared" ref="DG19" si="160">DF19+1</f>
         <v>219</v>
       </c>
-      <c r="DH19" s="33">
+      <c r="DH19" s="12">
         <f t="shared" ref="DH19" si="161">DG19+1</f>
         <v>220</v>
       </c>
-      <c r="DI19" s="33">
+      <c r="DI19" s="12">
         <f t="shared" ref="DI19" si="162">DH19+1</f>
         <v>221</v>
       </c>
-      <c r="DJ19" s="33">
+      <c r="DJ19" s="12">
         <f t="shared" ref="DJ19" si="163">DI19+1</f>
         <v>222</v>
       </c>
-      <c r="DK19" s="33">
+      <c r="DK19" s="12">
         <f t="shared" ref="DK19" si="164">DJ19+1</f>
         <v>223</v>
       </c>
-      <c r="DL19" s="33">
+      <c r="DL19" s="12">
         <f t="shared" ref="DL19" si="165">DK19+1</f>
         <v>224</v>
       </c>
-      <c r="DM19" s="33">
+      <c r="DM19" s="12">
         <f t="shared" ref="DM19" si="166">DL19+1</f>
         <v>225</v>
       </c>
-      <c r="DN19" s="33">
+      <c r="DN19" s="12">
         <f t="shared" ref="DN19" si="167">DM19+1</f>
         <v>226</v>
       </c>
-      <c r="DO19" s="33">
+      <c r="DO19" s="12">
         <f t="shared" ref="DO19" si="168">DN19+1</f>
         <v>227</v>
       </c>
-      <c r="DP19" s="33">
+      <c r="DP19" s="12">
         <f t="shared" ref="DP19" si="169">DO19+1</f>
         <v>228</v>
       </c>
-      <c r="DQ19" s="33">
+      <c r="DQ19" s="12">
         <f t="shared" ref="DQ19" si="170">DP19+1</f>
         <v>229</v>
       </c>
-      <c r="DR19" s="33">
+      <c r="DR19" s="12">
         <f t="shared" ref="DR19" si="171">DQ19+1</f>
         <v>230</v>
       </c>
-      <c r="DS19" s="33">
+      <c r="DS19" s="12">
         <f t="shared" ref="DS19" si="172">DR19+1</f>
         <v>231</v>
       </c>
-      <c r="DT19" s="33">
+      <c r="DT19" s="12">
         <f t="shared" ref="DT19" si="173">DS19+1</f>
         <v>232</v>
       </c>
-      <c r="DU19" s="33">
+      <c r="DU19" s="12">
         <f t="shared" ref="DU19" si="174">DT19+1</f>
         <v>233</v>
       </c>
-      <c r="DV19" s="33">
+      <c r="DV19" s="12">
         <f t="shared" ref="DV19" si="175">DU19+1</f>
         <v>234</v>
       </c>
-      <c r="DW19" s="33">
+      <c r="DW19" s="12">
         <f t="shared" ref="DW19" si="176">DV19+1</f>
         <v>235</v>
       </c>
-      <c r="DX19" s="33">
+      <c r="DX19" s="12">
         <f t="shared" ref="DX19" si="177">DW19+1</f>
         <v>236</v>
       </c>
-      <c r="DY19" s="33">
+      <c r="DY19" s="12">
         <f t="shared" ref="DY19" si="178">DX19+1</f>
         <v>237</v>
       </c>
-      <c r="DZ19" s="33">
+      <c r="DZ19" s="12">
         <f t="shared" ref="DZ19" si="179">DY19+1</f>
         <v>238</v>
       </c>
-      <c r="EA19" s="33">
+      <c r="EA19" s="12">
         <f t="shared" ref="EA19" si="180">DZ19+1</f>
         <v>239</v>
       </c>
-      <c r="EB19" s="33">
+      <c r="EB19" s="12">
         <f t="shared" ref="EB19" si="181">EA19+1</f>
         <v>240</v>
       </c>
-      <c r="EC19" s="33">
+      <c r="EC19" s="12">
         <f t="shared" ref="EC19" si="182">EB19+1</f>
         <v>241</v>
       </c>
-      <c r="ED19" s="33">
+      <c r="ED19" s="12">
         <f t="shared" ref="ED19" si="183">EC19+1</f>
         <v>242</v>
       </c>
-      <c r="EE19" s="34">
-        <f t="shared" ref="EE19" si="184">ED19+1</f>
+      <c r="EE19" s="12">
+        <f t="shared" ref="EE19:EG19" si="184">ED19+1</f>
         <v>243</v>
       </c>
+      <c r="EF19" s="12">
+        <f t="shared" si="184"/>
+        <v>244</v>
+      </c>
+      <c r="EG19" s="33">
+        <f t="shared" si="184"/>
+        <v>245</v>
+      </c>
     </row>
-    <row r="20" spans="2:135" ht="42" customHeight="1">
-      <c r="B20" s="3" t="s">
+    <row r="20" spans="2:137" ht="42" customHeight="1">
+      <c r="B20" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="30">
         <v>15</v>
       </c>
-      <c r="D20" s="4">
+      <c r="D20" s="30">
         <v>5</v>
       </c>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="35"/>
-      <c r="J20" s="35"/>
-      <c r="K20" s="35"/>
-      <c r="L20" s="35"/>
-      <c r="M20" s="35"/>
-      <c r="N20" s="35"/>
-      <c r="O20" s="35"/>
-      <c r="P20" s="35"/>
-      <c r="Q20" s="35" t="s">
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
+      <c r="I20" s="31"/>
+      <c r="J20" s="31"/>
+      <c r="K20" s="31"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="31"/>
+      <c r="N20" s="31"/>
+      <c r="O20" s="31"/>
+      <c r="P20" s="31"/>
+      <c r="Q20" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="R20" s="35" t="s">
+      <c r="R20" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="S20" s="35" t="s">
+      <c r="S20" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="T20" s="35" t="s">
+      <c r="T20" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="U20" s="35" t="s">
+      <c r="U20" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="V20" s="35"/>
-      <c r="W20" s="35" t="s">
+      <c r="V20" s="34"/>
+      <c r="W20" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="X20" s="35" t="s">
+      <c r="X20" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="Y20" s="35" t="s">
+      <c r="Y20" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="Z20" s="35" t="s">
+      <c r="Z20" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="AA20" s="35" t="s">
+      <c r="AA20" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="AB20" s="35"/>
-      <c r="AC20" s="35"/>
-      <c r="AD20" s="35"/>
-      <c r="AE20" s="35"/>
-      <c r="AF20" s="35"/>
-      <c r="AG20" s="35"/>
-      <c r="AH20" s="35"/>
-      <c r="AI20" s="35" t="s">
+      <c r="AB20" s="34"/>
+      <c r="AC20" s="34"/>
+      <c r="AD20" s="34"/>
+      <c r="AE20" s="34"/>
+      <c r="AF20" s="34"/>
+      <c r="AG20" s="34"/>
+      <c r="AH20" s="34"/>
+      <c r="AI20" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="AJ20" s="35" t="s">
+      <c r="AJ20" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="AK20" s="35" t="s">
+      <c r="AK20" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="AL20" s="35" t="s">
+      <c r="AL20" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="AM20" s="35" t="s">
+      <c r="AM20" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="AN20" s="35"/>
-      <c r="AO20" s="35" t="s">
+      <c r="AN20" s="34"/>
+      <c r="AO20" s="34" t="s">
         <v>147</v>
       </c>
-      <c r="AP20" s="35" t="s">
+      <c r="AP20" s="34" t="s">
         <v>147</v>
       </c>
-      <c r="AQ20" s="35" t="s">
+      <c r="AQ20" s="34" t="s">
         <v>147</v>
       </c>
-      <c r="AR20" s="35" t="s">
+      <c r="AR20" s="34" t="s">
         <v>147</v>
       </c>
-      <c r="AS20" s="35" t="s">
+      <c r="AS20" s="34" t="s">
         <v>147</v>
       </c>
-      <c r="AT20" s="35"/>
-      <c r="AU20" s="35"/>
-      <c r="AV20" s="35"/>
-      <c r="AW20" s="35"/>
-      <c r="AX20" s="35"/>
-      <c r="AY20" s="35"/>
-      <c r="AZ20" s="35"/>
-      <c r="BA20" s="35" t="s">
+      <c r="AT20" s="34"/>
+      <c r="AU20" s="34"/>
+      <c r="AV20" s="34"/>
+      <c r="AW20" s="34"/>
+      <c r="AX20" s="34"/>
+      <c r="AY20" s="34"/>
+      <c r="AZ20" s="34"/>
+      <c r="BA20" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="BB20" s="35" t="s">
+      <c r="BB20" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="BC20" s="35" t="s">
+      <c r="BC20" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="BD20" s="35" t="s">
+      <c r="BD20" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="BE20" s="35" t="s">
+      <c r="BE20" s="34" t="s">
         <v>137</v>
       </c>
-      <c r="BF20" s="35"/>
-      <c r="BG20" s="36" t="s">
+      <c r="BF20" s="34"/>
+      <c r="BG20" s="35" t="s">
         <v>150</v>
       </c>
-      <c r="BH20" s="36" t="s">
+      <c r="BH20" s="35" t="s">
         <v>150</v>
       </c>
-      <c r="BI20" s="36" t="s">
+      <c r="BI20" s="35" t="s">
         <v>150</v>
       </c>
-      <c r="BJ20" s="36" t="s">
+      <c r="BJ20" s="35" t="s">
         <v>150</v>
       </c>
-      <c r="BK20" s="36" t="s">
+      <c r="BK20" s="35" t="s">
         <v>150</v>
       </c>
-      <c r="BL20" s="35"/>
-      <c r="BM20" s="35"/>
-      <c r="BN20" s="35"/>
-      <c r="BO20" s="35"/>
-      <c r="BP20" s="35"/>
-      <c r="BQ20" s="35"/>
-      <c r="BR20" s="35"/>
-      <c r="BS20" s="36" t="s">
+      <c r="BL20" s="34"/>
+      <c r="BM20" s="34"/>
+      <c r="BN20" s="34"/>
+      <c r="BO20" s="34"/>
+      <c r="BP20" s="34"/>
+      <c r="BQ20" s="34"/>
+      <c r="BR20" s="34"/>
+      <c r="BS20" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="BT20" s="36" t="s">
+      <c r="BT20" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="BU20" s="36" t="s">
+      <c r="BU20" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="BV20" s="36" t="s">
+      <c r="BV20" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="BW20" s="36" t="s">
+      <c r="BW20" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="BX20" s="35"/>
-      <c r="BY20" s="36" t="s">
+      <c r="BX20" s="34"/>
+      <c r="BY20" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="BZ20" s="36" t="s">
+      <c r="BZ20" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="CA20" s="36" t="s">
+      <c r="CA20" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="CB20" s="36" t="s">
+      <c r="CB20" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="CC20" s="36" t="s">
+      <c r="CC20" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="CD20" s="35"/>
-      <c r="CE20" s="35"/>
-      <c r="CF20" s="35"/>
-      <c r="CG20" s="35"/>
-      <c r="CH20" s="35"/>
-      <c r="CI20" s="35"/>
-      <c r="CJ20" s="35"/>
-      <c r="CK20" s="36" t="s">
+      <c r="CD20" s="34"/>
+      <c r="CE20" s="34"/>
+      <c r="CF20" s="34"/>
+      <c r="CG20" s="34"/>
+      <c r="CH20" s="34"/>
+      <c r="CI20" s="34"/>
+      <c r="CJ20" s="34"/>
+      <c r="CK20" s="35" t="s">
         <v>141</v>
       </c>
-      <c r="CL20" s="36" t="s">
+      <c r="CL20" s="35" t="s">
         <v>141</v>
       </c>
-      <c r="CM20" s="36" t="s">
+      <c r="CM20" s="35" t="s">
         <v>141</v>
       </c>
-      <c r="CN20" s="36" t="s">
+      <c r="CN20" s="35" t="s">
         <v>141</v>
       </c>
-      <c r="CO20" s="36" t="s">
+      <c r="CO20" s="35" t="s">
         <v>141</v>
       </c>
-      <c r="CP20" s="35"/>
-      <c r="CQ20" s="36" t="s">
+      <c r="CP20" s="34"/>
+      <c r="CQ20" s="35" t="s">
         <v>156</v>
       </c>
-      <c r="CR20" s="36" t="s">
+      <c r="CR20" s="35" t="s">
         <v>156</v>
       </c>
-      <c r="CS20" s="36" t="s">
+      <c r="CS20" s="35" t="s">
         <v>156</v>
       </c>
-      <c r="CT20" s="36" t="s">
+      <c r="CT20" s="35" t="s">
         <v>156</v>
       </c>
-      <c r="CU20" s="36" t="s">
+      <c r="CU20" s="35" t="s">
         <v>156</v>
       </c>
-      <c r="CV20" s="35"/>
-      <c r="CW20" s="35"/>
-      <c r="CX20" s="35"/>
-      <c r="CY20" s="35"/>
-      <c r="CZ20" s="35"/>
-      <c r="DA20" s="35"/>
-      <c r="DB20" s="35"/>
-      <c r="DC20" s="35"/>
-      <c r="DD20" s="35"/>
-      <c r="DE20" s="35"/>
-      <c r="DF20" s="35"/>
-      <c r="DG20" s="35"/>
-      <c r="DH20" s="35"/>
-      <c r="DI20" s="35"/>
-      <c r="DJ20" s="35"/>
-      <c r="DK20" s="35"/>
-      <c r="DL20" s="35"/>
-      <c r="DM20" s="35"/>
-      <c r="DN20" s="35"/>
-      <c r="DO20" s="35"/>
-      <c r="DP20" s="35"/>
-      <c r="DQ20" s="35"/>
-      <c r="DR20" s="35"/>
-      <c r="DS20" s="35"/>
-      <c r="DT20" s="35"/>
-      <c r="DU20" s="35"/>
-      <c r="DV20" s="35"/>
-      <c r="DW20" s="35"/>
-      <c r="DX20" s="35"/>
-      <c r="DY20" s="35"/>
-      <c r="DZ20" s="35"/>
-      <c r="EA20" s="35" t="s">
+      <c r="CV20" s="31"/>
+      <c r="CW20" s="31"/>
+      <c r="CX20" s="31"/>
+      <c r="CY20" s="31"/>
+      <c r="CZ20" s="31"/>
+      <c r="DA20" s="31"/>
+      <c r="DB20" s="31"/>
+      <c r="DC20" s="31"/>
+      <c r="DD20" s="31"/>
+      <c r="DE20" s="31"/>
+      <c r="DF20" s="31"/>
+      <c r="DG20" s="31"/>
+      <c r="DH20" s="31"/>
+      <c r="DI20" s="31"/>
+      <c r="DJ20" s="31"/>
+      <c r="DK20" s="31"/>
+      <c r="DL20" s="31"/>
+      <c r="DM20" s="31"/>
+      <c r="DN20" s="31"/>
+      <c r="DO20" s="31"/>
+      <c r="DP20" s="31"/>
+      <c r="DQ20" s="31"/>
+      <c r="DR20" s="31"/>
+      <c r="DS20" s="31"/>
+      <c r="DT20" s="31"/>
+      <c r="DU20" s="31"/>
+      <c r="DV20" s="31"/>
+      <c r="DW20" s="31"/>
+      <c r="DX20" s="31"/>
+      <c r="DY20" s="31"/>
+      <c r="DZ20" s="31"/>
+      <c r="EA20" s="31"/>
+      <c r="EB20" s="31"/>
+      <c r="EC20" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="EB20" s="35" t="s">
+      <c r="ED20" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="EC20" s="35" t="s">
+      <c r="EE20" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="ED20" s="35" t="s">
+      <c r="EF20" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="EE20" s="37" t="s">
+      <c r="EG20" s="32" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="2:135" ht="42" customHeight="1">
-      <c r="B21" s="26" t="s">
+    <row r="21" spans="2:137" ht="42" customHeight="1">
+      <c r="B21" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="27">
+      <c r="C21" s="28">
         <v>36</v>
       </c>
-      <c r="D21" s="27" t="s">
+      <c r="D21" s="28" t="s">
         <v>163</v>
       </c>
       <c r="E21" s="7"/>
@@ -6839,92 +6888,94 @@
       <c r="CZ21" s="7"/>
       <c r="DA21" s="7"/>
       <c r="DB21" s="7"/>
-      <c r="DC21" s="7" t="s">
+      <c r="DC21" s="7"/>
+      <c r="DD21" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="DD21" s="7" t="s">
+      <c r="DE21" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="DE21" s="7" t="s">
+      <c r="DF21" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="DF21" s="7" t="s">
+      <c r="DG21" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="DG21" s="7" t="s">
+      <c r="DH21" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="DH21" s="7" t="s">
+      <c r="DI21" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="DI21" s="7" t="s">
+      <c r="DJ21" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="DJ21" s="7" t="s">
+      <c r="DK21" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="DK21" s="7" t="s">
+      <c r="DL21" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="DL21" s="7" t="s">
+      <c r="DM21" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="DM21" s="7" t="s">
+      <c r="DN21" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="DN21" s="7" t="s">
+      <c r="DO21" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="DO21" s="7" t="s">
+      <c r="DP21" s="7"/>
+      <c r="DQ21" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="DP21" s="7" t="s">
+      <c r="DR21" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="DQ21" s="7" t="s">
+      <c r="DS21" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="DR21" s="7" t="s">
+      <c r="DT21" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="DS21" s="7" t="s">
+      <c r="DU21" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="DT21" s="7" t="s">
+      <c r="DV21" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="DU21" s="7" t="s">
+      <c r="DW21" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="DV21" s="7" t="s">
+      <c r="DX21" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="DW21" s="7" t="s">
+      <c r="DY21" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="DX21" s="7" t="s">
+      <c r="DZ21" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="DY21" s="7" t="s">
+      <c r="EA21" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="DZ21" s="7" t="s">
+      <c r="EB21" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="EA21" s="7"/>
-      <c r="EB21" s="7"/>
       <c r="EC21" s="7"/>
       <c r="ED21" s="7"/>
-      <c r="EE21" s="8"/>
+      <c r="EE21" s="7"/>
+      <c r="EF21" s="7"/>
+      <c r="EG21" s="8"/>
     </row>
-    <row r="22" spans="2:135" ht="42" customHeight="1">
-      <c r="B22" s="26" t="s">
+    <row r="22" spans="2:137" ht="42" customHeight="1">
+      <c r="B22" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="C22" s="27">
+      <c r="C22" s="28">
         <v>36</v>
       </c>
-      <c r="D22" s="27">
+      <c r="D22" s="28">
         <v>1</v>
       </c>
       <c r="E22" s="7"/>
@@ -7077,16 +7128,18 @@
       <c r="EB22" s="7"/>
       <c r="EC22" s="7"/>
       <c r="ED22" s="7"/>
-      <c r="EE22" s="8"/>
+      <c r="EE22" s="7"/>
+      <c r="EF22" s="7"/>
+      <c r="EG22" s="8"/>
     </row>
-    <row r="23" spans="2:135" ht="42" customHeight="1">
-      <c r="B23" s="26" t="s">
+    <row r="23" spans="2:137" ht="42" customHeight="1">
+      <c r="B23" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="C23" s="27">
+      <c r="C23" s="28">
         <v>1</v>
       </c>
-      <c r="D23" s="27">
+      <c r="D23" s="28">
         <v>6</v>
       </c>
       <c r="E23" s="7" t="s">
@@ -7291,9 +7344,11 @@
       <c r="EB23" s="7"/>
       <c r="EC23" s="7"/>
       <c r="ED23" s="7"/>
-      <c r="EE23" s="8"/>
+      <c r="EE23" s="7"/>
+      <c r="EF23" s="7"/>
+      <c r="EG23" s="8"/>
     </row>
-    <row r="24" spans="2:135" ht="42" customHeight="1" thickBot="1">
+    <row r="24" spans="2:137" ht="42" customHeight="1" thickBot="1">
       <c r="B24" s="11" t="s">
         <v>78</v>
       </c>
@@ -7565,28 +7620,31 @@
       <c r="EB24" s="13"/>
       <c r="EC24" s="13"/>
       <c r="ED24" s="13"/>
-      <c r="EE24" s="15"/>
+      <c r="EE24" s="13"/>
+      <c r="EF24" s="13"/>
+      <c r="EG24" s="15"/>
     </row>
-    <row r="26" spans="2:135" ht="42" customHeight="1">
+    <row r="26" spans="2:137" ht="42" customHeight="1">
       <c r="B26" s="2">
-        <v>243</v>
+        <f>MAX(19:19)</f>
+        <v>245</v>
       </c>
     </row>
-    <row r="27" spans="2:135" ht="42" customHeight="1">
-      <c r="B27" s="38">
+    <row r="27" spans="2:137" ht="42" customHeight="1">
+      <c r="B27" s="26">
         <v>50000000</v>
       </c>
     </row>
-    <row r="28" spans="2:135" ht="42" customHeight="1">
-      <c r="B28" s="38">
+    <row r="28" spans="2:137" ht="42" customHeight="1">
+      <c r="B28" s="26">
         <f>1/B27</f>
         <v>2E-8</v>
       </c>
     </row>
-    <row r="29" spans="2:135" ht="42" customHeight="1">
-      <c r="B29" s="38">
+    <row r="29" spans="2:137" ht="42" customHeight="1">
+      <c r="B29" s="26">
         <f>B26*B28</f>
-        <v>4.8600000000000001E-6</v>
+        <v>4.9000000000000005E-6</v>
       </c>
     </row>
   </sheetData>
@@ -7598,7 +7656,7 @@
     <mergeCell ref="B9:B14"/>
     <mergeCell ref="C9:C14"/>
     <mergeCell ref="D9:D14"/>
-    <mergeCell ref="E18:EE18"/>
+    <mergeCell ref="E18:EG18"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
All implementation of ik_swift top module done. Still needs to be validated.
</commit_message>
<xml_diff>
--- a/doc/design/schedule.xlsx
+++ b/doc/design/schedule.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="165">
   <si>
     <t>sincos</t>
   </si>
@@ -752,7 +752,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="867">
+  <cellStyleXfs count="873">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1620,8 +1620,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1701,12 +1707,6 @@
     <xf numFmtId="11" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1728,6 +1728,12 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1740,8 +1746,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="867">
+  <cellStyles count="873">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2175,6 +2184,9 @@
     <cellStyle name="Followed Hyperlink" xfId="862" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="864" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="866" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="868" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="870" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="872" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2608,6 +2620,9 @@
     <cellStyle name="Hyperlink" xfId="861" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="863" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="865" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="867" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="869" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="871" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2940,20 +2955,22 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:EG29"/>
+  <dimension ref="A1:EI29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E11" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <pane xSplit="4" ySplit="2" topLeftCell="BO3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="AL1" sqref="AL1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E18" sqref="E18:EG18"/>
+      <selection pane="bottomRight" activeCell="CZ2" sqref="CZ1:CZ1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.33203125" defaultRowHeight="42" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.33203125" style="6" customWidth="1"/>
     <col min="2" max="4" width="10.33203125" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="4.33203125" style="9"/>
+    <col min="5" max="94" width="4.33203125" style="9"/>
+    <col min="95" max="95" width="4.33203125" style="9" customWidth="1"/>
+    <col min="96" max="16384" width="4.33203125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:117" s="2" customFormat="1" ht="42" customHeight="1">
@@ -5838,8 +5855,8 @@
       <c r="DL16" s="15"/>
       <c r="DM16" s="18"/>
     </row>
-    <row r="17" spans="2:137" ht="42" customHeight="1" thickBot="1"/>
-    <row r="18" spans="2:137" s="2" customFormat="1" ht="42" customHeight="1">
+    <row r="17" spans="2:139" ht="42" customHeight="1" thickBot="1"/>
+    <row r="18" spans="2:139" s="2" customFormat="1" ht="42" customHeight="1">
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
@@ -5977,9 +5994,11 @@
       <c r="ED18" s="36"/>
       <c r="EE18" s="36"/>
       <c r="EF18" s="36"/>
-      <c r="EG18" s="37"/>
+      <c r="EG18" s="36"/>
+      <c r="EH18" s="36"/>
+      <c r="EI18" s="37"/>
     </row>
-    <row r="19" spans="2:137" s="2" customFormat="1" ht="42" customHeight="1" thickBot="1">
+    <row r="19" spans="2:139" s="2" customFormat="1" ht="42" customHeight="1" thickBot="1">
       <c r="B19" s="11" t="s">
         <v>100</v>
       </c>
@@ -6514,276 +6533,276 @@
         <v>243</v>
       </c>
       <c r="EF19" s="12">
-        <f t="shared" si="184"/>
+        <f t="shared" ref="EF19" si="185">EE19+1</f>
         <v>244</v>
       </c>
-      <c r="EG19" s="33">
-        <f t="shared" si="184"/>
+      <c r="EG19" s="12">
+        <f t="shared" ref="EG19" si="186">EF19+1</f>
         <v>245</v>
       </c>
+      <c r="EH19" s="12">
+        <f t="shared" ref="EH19" si="187">EG19+1</f>
+        <v>246</v>
+      </c>
+      <c r="EI19" s="31">
+        <f t="shared" ref="EI19" si="188">EH19+1</f>
+        <v>247</v>
+      </c>
     </row>
-    <row r="20" spans="2:137" ht="42" customHeight="1">
-      <c r="B20" s="29" t="s">
+    <row r="20" spans="2:139" ht="42" customHeight="1">
+      <c r="B20" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C20" s="30">
+      <c r="C20" s="28">
         <v>15</v>
       </c>
-      <c r="D20" s="30">
+      <c r="D20" s="28">
         <v>5</v>
       </c>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="31"/>
-      <c r="L20" s="31"/>
-      <c r="M20" s="31"/>
-      <c r="N20" s="31"/>
-      <c r="O20" s="31"/>
-      <c r="P20" s="31"/>
-      <c r="Q20" s="34" t="s">
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="29"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="29"/>
+      <c r="O20" s="29"/>
+      <c r="P20" s="29"/>
+      <c r="Q20" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="R20" s="34" t="s">
+      <c r="R20" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="S20" s="34" t="s">
+      <c r="S20" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="T20" s="34" t="s">
+      <c r="T20" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="U20" s="34" t="s">
+      <c r="U20" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="V20" s="34"/>
-      <c r="W20" s="34" t="s">
+      <c r="V20" s="32"/>
+      <c r="W20" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="X20" s="34" t="s">
+      <c r="X20" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="Y20" s="34" t="s">
+      <c r="Y20" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="Z20" s="34" t="s">
+      <c r="Z20" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="AA20" s="34" t="s">
+      <c r="AA20" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="AB20" s="34"/>
-      <c r="AC20" s="34"/>
-      <c r="AD20" s="34"/>
-      <c r="AE20" s="34"/>
-      <c r="AF20" s="34"/>
-      <c r="AG20" s="34"/>
-      <c r="AH20" s="34"/>
-      <c r="AI20" s="34" t="s">
+      <c r="AB20" s="32"/>
+      <c r="AC20" s="32"/>
+      <c r="AD20" s="32"/>
+      <c r="AE20" s="32"/>
+      <c r="AF20" s="32"/>
+      <c r="AG20" s="32"/>
+      <c r="AH20" s="32"/>
+      <c r="AI20" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="AJ20" s="34" t="s">
+      <c r="AJ20" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="AK20" s="34" t="s">
+      <c r="AK20" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="AL20" s="34" t="s">
+      <c r="AL20" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="AM20" s="34" t="s">
+      <c r="AM20" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="AN20" s="34"/>
-      <c r="AO20" s="34" t="s">
+      <c r="AN20" s="32"/>
+      <c r="AO20" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="AP20" s="34" t="s">
+      <c r="AP20" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="AQ20" s="34" t="s">
+      <c r="AQ20" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="AR20" s="34" t="s">
+      <c r="AR20" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="AS20" s="34" t="s">
+      <c r="AS20" s="32" t="s">
         <v>147</v>
       </c>
-      <c r="AT20" s="34"/>
-      <c r="AU20" s="34"/>
-      <c r="AV20" s="34"/>
-      <c r="AW20" s="34"/>
-      <c r="AX20" s="34"/>
-      <c r="AY20" s="34"/>
-      <c r="AZ20" s="34"/>
-      <c r="BA20" s="34" t="s">
+      <c r="AT20" s="32"/>
+      <c r="AU20" s="32"/>
+      <c r="AV20" s="32"/>
+      <c r="AW20" s="32"/>
+      <c r="AX20" s="32"/>
+      <c r="AY20" s="32"/>
+      <c r="AZ20" s="32"/>
+      <c r="BA20" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="BB20" s="34" t="s">
+      <c r="BB20" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="BC20" s="34" t="s">
+      <c r="BC20" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="BD20" s="34" t="s">
+      <c r="BD20" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="BE20" s="34" t="s">
+      <c r="BE20" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="BF20" s="34"/>
-      <c r="BG20" s="35" t="s">
+      <c r="BF20" s="32"/>
+      <c r="BG20" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="BH20" s="35" t="s">
+      <c r="BH20" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="BI20" s="35" t="s">
+      <c r="BI20" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="BJ20" s="35" t="s">
+      <c r="BJ20" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="BK20" s="35" t="s">
+      <c r="BK20" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="BL20" s="34"/>
-      <c r="BM20" s="34"/>
-      <c r="BN20" s="34"/>
-      <c r="BO20" s="34"/>
-      <c r="BP20" s="34"/>
-      <c r="BQ20" s="34"/>
-      <c r="BR20" s="34"/>
-      <c r="BS20" s="35" t="s">
+      <c r="BL20" s="32"/>
+      <c r="BM20" s="32"/>
+      <c r="BN20" s="32"/>
+      <c r="BO20" s="32"/>
+      <c r="BP20" s="32"/>
+      <c r="BQ20" s="32"/>
+      <c r="BR20" s="32"/>
+      <c r="BS20" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="BT20" s="35" t="s">
+      <c r="BT20" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="BU20" s="35" t="s">
+      <c r="BU20" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="BV20" s="35" t="s">
+      <c r="BV20" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="BW20" s="35" t="s">
+      <c r="BW20" s="33" t="s">
         <v>139</v>
       </c>
-      <c r="BX20" s="34"/>
-      <c r="BY20" s="35" t="s">
+      <c r="BX20" s="32"/>
+      <c r="BY20" s="33" t="s">
         <v>153</v>
       </c>
-      <c r="BZ20" s="35" t="s">
+      <c r="BZ20" s="33" t="s">
         <v>153</v>
       </c>
-      <c r="CA20" s="35" t="s">
+      <c r="CA20" s="33" t="s">
         <v>153</v>
       </c>
-      <c r="CB20" s="35" t="s">
+      <c r="CB20" s="33" t="s">
         <v>153</v>
       </c>
-      <c r="CC20" s="35" t="s">
+      <c r="CC20" s="33" t="s">
         <v>153</v>
       </c>
-      <c r="CD20" s="34"/>
-      <c r="CE20" s="34"/>
-      <c r="CF20" s="34"/>
-      <c r="CG20" s="34"/>
-      <c r="CH20" s="34"/>
-      <c r="CI20" s="34"/>
-      <c r="CJ20" s="34"/>
-      <c r="CK20" s="35" t="s">
+      <c r="CD20" s="32"/>
+      <c r="CE20" s="32"/>
+      <c r="CF20" s="32"/>
+      <c r="CG20" s="32"/>
+      <c r="CH20" s="32"/>
+      <c r="CI20" s="32"/>
+      <c r="CJ20" s="32"/>
+      <c r="CK20" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="CL20" s="35" t="s">
+      <c r="CL20" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="CM20" s="35" t="s">
+      <c r="CM20" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="CN20" s="35" t="s">
+      <c r="CN20" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="CO20" s="35" t="s">
+      <c r="CO20" s="33" t="s">
         <v>141</v>
       </c>
-      <c r="CP20" s="34"/>
-      <c r="CQ20" s="35" t="s">
+      <c r="CP20" s="32"/>
+      <c r="CQ20" s="33" t="s">
         <v>156</v>
       </c>
-      <c r="CR20" s="35" t="s">
+      <c r="CR20" s="33" t="s">
         <v>156</v>
       </c>
-      <c r="CS20" s="35" t="s">
+      <c r="CS20" s="33" t="s">
         <v>156</v>
       </c>
-      <c r="CT20" s="35" t="s">
+      <c r="CT20" s="33" t="s">
         <v>156</v>
       </c>
-      <c r="CU20" s="35" t="s">
+      <c r="CU20" s="33" t="s">
         <v>156</v>
       </c>
-      <c r="CV20" s="31"/>
-      <c r="CW20" s="31"/>
-      <c r="CX20" s="31"/>
-      <c r="CY20" s="31"/>
-      <c r="CZ20" s="31"/>
-      <c r="DA20" s="31"/>
-      <c r="DB20" s="31"/>
-      <c r="DC20" s="31"/>
-      <c r="DD20" s="31"/>
-      <c r="DE20" s="31"/>
-      <c r="DF20" s="31"/>
-      <c r="DG20" s="31"/>
-      <c r="DH20" s="31"/>
-      <c r="DI20" s="31"/>
-      <c r="DJ20" s="31"/>
-      <c r="DK20" s="31"/>
-      <c r="DL20" s="31"/>
-      <c r="DM20" s="31"/>
-      <c r="DN20" s="31"/>
-      <c r="DO20" s="31"/>
-      <c r="DP20" s="31"/>
-      <c r="DQ20" s="31"/>
-      <c r="DR20" s="31"/>
-      <c r="DS20" s="31"/>
-      <c r="DT20" s="31"/>
-      <c r="DU20" s="31"/>
-      <c r="DV20" s="31"/>
-      <c r="DW20" s="31"/>
-      <c r="DX20" s="31"/>
-      <c r="DY20" s="31"/>
-      <c r="DZ20" s="31"/>
-      <c r="EA20" s="31"/>
-      <c r="EB20" s="31"/>
-      <c r="EC20" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="ED20" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="EE20" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="EF20" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="EG20" s="32" t="s">
-        <v>99</v>
-      </c>
+      <c r="CV20" s="29"/>
+      <c r="CW20" s="29"/>
+      <c r="CX20" s="29"/>
+      <c r="CY20" s="29"/>
+      <c r="CZ20" s="29"/>
+      <c r="DA20" s="29"/>
+      <c r="DB20" s="29"/>
+      <c r="DC20" s="29"/>
+      <c r="DD20" s="29"/>
+      <c r="DE20" s="29"/>
+      <c r="DF20" s="29"/>
+      <c r="DG20" s="29"/>
+      <c r="DH20" s="29"/>
+      <c r="DI20" s="29"/>
+      <c r="DJ20" s="29"/>
+      <c r="DK20" s="29"/>
+      <c r="DL20" s="29"/>
+      <c r="DM20" s="29"/>
+      <c r="DN20" s="29"/>
+      <c r="DO20" s="29"/>
+      <c r="DP20" s="29"/>
+      <c r="DQ20" s="29"/>
+      <c r="DR20" s="29"/>
+      <c r="DS20" s="29"/>
+      <c r="DT20" s="29"/>
+      <c r="DU20" s="29"/>
+      <c r="DV20" s="29"/>
+      <c r="DW20" s="29"/>
+      <c r="DX20" s="29"/>
+      <c r="DY20" s="29"/>
+      <c r="DZ20" s="29"/>
+      <c r="EA20" s="29"/>
+      <c r="EB20" s="29"/>
+      <c r="EC20" s="29"/>
+      <c r="ED20" s="29"/>
+      <c r="EE20" s="29"/>
+      <c r="EF20" s="29"/>
+      <c r="EG20" s="29"/>
+      <c r="EH20" s="29"/>
+      <c r="EI20" s="30"/>
     </row>
-    <row r="21" spans="2:137" ht="42" customHeight="1">
-      <c r="B21" s="27" t="s">
+    <row r="21" spans="2:139" ht="42" customHeight="1">
+      <c r="B21" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="C21" s="28">
+      <c r="C21" s="35">
         <v>36</v>
       </c>
-      <c r="D21" s="28" t="s">
+      <c r="D21" s="35" t="s">
         <v>163</v>
       </c>
       <c r="E21" s="7"/>
@@ -6962,20 +6981,36 @@
       <c r="EB21" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="EC21" s="7"/>
-      <c r="ED21" s="7"/>
-      <c r="EE21" s="7"/>
-      <c r="EF21" s="7"/>
-      <c r="EG21" s="8"/>
+      <c r="EC21" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="ED21" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="EE21" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="EF21" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="EG21" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="EH21" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="EI21" s="40" t="s">
+        <v>99</v>
+      </c>
     </row>
-    <row r="22" spans="2:137" ht="42" customHeight="1">
-      <c r="B22" s="27" t="s">
+    <row r="22" spans="2:139" ht="42" customHeight="1">
+      <c r="B22" s="34" t="s">
         <v>76</v>
       </c>
-      <c r="C22" s="28">
+      <c r="C22" s="35">
         <v>36</v>
       </c>
-      <c r="D22" s="28">
+      <c r="D22" s="35">
         <v>1</v>
       </c>
       <c r="E22" s="7"/>
@@ -7130,16 +7165,18 @@
       <c r="ED22" s="7"/>
       <c r="EE22" s="7"/>
       <c r="EF22" s="7"/>
-      <c r="EG22" s="8"/>
+      <c r="EG22" s="7"/>
+      <c r="EH22" s="7"/>
+      <c r="EI22" s="8"/>
     </row>
-    <row r="23" spans="2:137" ht="42" customHeight="1">
-      <c r="B23" s="27" t="s">
+    <row r="23" spans="2:139" ht="42" customHeight="1">
+      <c r="B23" s="34" t="s">
         <v>77</v>
       </c>
-      <c r="C23" s="28">
+      <c r="C23" s="35">
         <v>1</v>
       </c>
-      <c r="D23" s="28">
+      <c r="D23" s="35">
         <v>6</v>
       </c>
       <c r="E23" s="7" t="s">
@@ -7346,9 +7383,11 @@
       <c r="ED23" s="7"/>
       <c r="EE23" s="7"/>
       <c r="EF23" s="7"/>
-      <c r="EG23" s="8"/>
+      <c r="EG23" s="7"/>
+      <c r="EH23" s="7"/>
+      <c r="EI23" s="8"/>
     </row>
-    <row r="24" spans="2:137" ht="42" customHeight="1" thickBot="1">
+    <row r="24" spans="2:139" ht="42" customHeight="1" thickBot="1">
       <c r="B24" s="11" t="s">
         <v>78</v>
       </c>
@@ -7622,33 +7661,36 @@
       <c r="ED24" s="13"/>
       <c r="EE24" s="13"/>
       <c r="EF24" s="13"/>
-      <c r="EG24" s="15"/>
+      <c r="EG24" s="13"/>
+      <c r="EH24" s="13"/>
+      <c r="EI24" s="15"/>
     </row>
-    <row r="26" spans="2:137" ht="42" customHeight="1">
+    <row r="26" spans="2:139" ht="42" customHeight="1">
       <c r="B26" s="2">
         <f>MAX(19:19)</f>
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
-    <row r="27" spans="2:137" ht="42" customHeight="1">
+    <row r="27" spans="2:139" ht="42" customHeight="1">
       <c r="B27" s="26">
         <v>50000000</v>
       </c>
     </row>
-    <row r="28" spans="2:137" ht="42" customHeight="1">
+    <row r="28" spans="2:139" ht="42" customHeight="1">
       <c r="B28" s="26">
         <f>1/B27</f>
         <v>2E-8</v>
       </c>
     </row>
-    <row r="29" spans="2:137" ht="42" customHeight="1">
+    <row r="29" spans="2:139" ht="42" customHeight="1">
       <c r="B29" s="26">
         <f>B26*B28</f>
-        <v>4.9000000000000005E-6</v>
+        <v>4.9400000000000001E-6</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="E18:EI18"/>
     <mergeCell ref="E1:DL1"/>
     <mergeCell ref="B3:B8"/>
     <mergeCell ref="C3:C8"/>
@@ -7656,7 +7698,6 @@
     <mergeCell ref="B9:B14"/>
     <mergeCell ref="C9:C14"/>
     <mergeCell ref="D9:D14"/>
-    <mergeCell ref="E18:EG18"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Modifying the inverse side of hardware for new bitwidths.
</commit_message>
<xml_diff>
--- a/doc/design/schedule.xlsx
+++ b/doc/design/schedule.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="166">
   <si>
     <t>sincos</t>
   </si>
@@ -514,6 +514,9 @@
   </si>
   <si>
     <t>T03 cyc 12</t>
+  </si>
+  <si>
+    <t>T06 x Z0</t>
   </si>
 </sst>
 </file>
@@ -752,8 +755,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="873">
+  <cellStyleXfs count="875">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1734,6 +1739,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1746,11 +1754,8 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="873">
+  <cellStyles count="875">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2187,6 +2192,7 @@
     <cellStyle name="Followed Hyperlink" xfId="868" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="870" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="872" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="874" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2623,6 +2629,7 @@
     <cellStyle name="Hyperlink" xfId="867" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="869" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="871" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="873" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2958,10 +2965,10 @@
   <dimension ref="A1:EI29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="BO3" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="BN3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="AL1" sqref="AL1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CZ2" sqref="CZ1:CZ1048576"/>
+      <selection pane="bottomRight" activeCell="CB6" sqref="CB6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.33203125" defaultRowHeight="42" customHeight="1" x14ac:dyDescent="0"/>
@@ -2977,120 +2984,120 @@
       <c r="B1" s="3"/>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="36"/>
-      <c r="U1" s="36"/>
-      <c r="V1" s="36"/>
-      <c r="W1" s="36"/>
-      <c r="X1" s="36"/>
-      <c r="Y1" s="36"/>
-      <c r="Z1" s="36"/>
-      <c r="AA1" s="36"/>
-      <c r="AB1" s="36"/>
-      <c r="AC1" s="36"/>
-      <c r="AD1" s="36"/>
-      <c r="AE1" s="36"/>
-      <c r="AF1" s="36"/>
-      <c r="AG1" s="36"/>
-      <c r="AH1" s="36"/>
-      <c r="AI1" s="36"/>
-      <c r="AJ1" s="36"/>
-      <c r="AK1" s="36"/>
-      <c r="AL1" s="36"/>
-      <c r="AM1" s="36"/>
-      <c r="AN1" s="36"/>
-      <c r="AO1" s="36"/>
-      <c r="AP1" s="36"/>
-      <c r="AQ1" s="36"/>
-      <c r="AR1" s="36"/>
-      <c r="AS1" s="36"/>
-      <c r="AT1" s="36"/>
-      <c r="AU1" s="36"/>
-      <c r="AV1" s="36"/>
-      <c r="AW1" s="36"/>
-      <c r="AX1" s="36"/>
-      <c r="AY1" s="36"/>
-      <c r="AZ1" s="36"/>
-      <c r="BA1" s="36"/>
-      <c r="BB1" s="36"/>
-      <c r="BC1" s="36"/>
-      <c r="BD1" s="36"/>
-      <c r="BE1" s="36"/>
-      <c r="BF1" s="36"/>
-      <c r="BG1" s="36"/>
-      <c r="BH1" s="36"/>
-      <c r="BI1" s="36"/>
-      <c r="BJ1" s="36"/>
-      <c r="BK1" s="36"/>
-      <c r="BL1" s="36"/>
-      <c r="BM1" s="36"/>
-      <c r="BN1" s="36"/>
-      <c r="BO1" s="36"/>
-      <c r="BP1" s="36"/>
-      <c r="BQ1" s="36"/>
-      <c r="BR1" s="36"/>
-      <c r="BS1" s="36"/>
-      <c r="BT1" s="36"/>
-      <c r="BU1" s="36"/>
-      <c r="BV1" s="36"/>
-      <c r="BW1" s="36"/>
-      <c r="BX1" s="36"/>
-      <c r="BY1" s="36"/>
-      <c r="BZ1" s="36"/>
-      <c r="CA1" s="36"/>
-      <c r="CB1" s="36"/>
-      <c r="CC1" s="36"/>
-      <c r="CD1" s="36"/>
-      <c r="CE1" s="36"/>
-      <c r="CF1" s="36"/>
-      <c r="CG1" s="36"/>
-      <c r="CH1" s="36"/>
-      <c r="CI1" s="36"/>
-      <c r="CJ1" s="36"/>
-      <c r="CK1" s="36"/>
-      <c r="CL1" s="36"/>
-      <c r="CM1" s="36"/>
-      <c r="CN1" s="36"/>
-      <c r="CO1" s="36"/>
-      <c r="CP1" s="36"/>
-      <c r="CQ1" s="36"/>
-      <c r="CR1" s="36"/>
-      <c r="CS1" s="36"/>
-      <c r="CT1" s="36"/>
-      <c r="CU1" s="36"/>
-      <c r="CV1" s="36"/>
-      <c r="CW1" s="36"/>
-      <c r="CX1" s="36"/>
-      <c r="CY1" s="36"/>
-      <c r="CZ1" s="36"/>
-      <c r="DA1" s="36"/>
-      <c r="DB1" s="36"/>
-      <c r="DC1" s="36"/>
-      <c r="DD1" s="36"/>
-      <c r="DE1" s="36"/>
-      <c r="DF1" s="36"/>
-      <c r="DG1" s="36"/>
-      <c r="DH1" s="36"/>
-      <c r="DI1" s="36"/>
-      <c r="DJ1" s="36"/>
-      <c r="DK1" s="36"/>
-      <c r="DL1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="K1" s="37"/>
+      <c r="L1" s="37"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
+      <c r="O1" s="37"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
+      <c r="S1" s="37"/>
+      <c r="T1" s="37"/>
+      <c r="U1" s="37"/>
+      <c r="V1" s="37"/>
+      <c r="W1" s="37"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="37"/>
+      <c r="Z1" s="37"/>
+      <c r="AA1" s="37"/>
+      <c r="AB1" s="37"/>
+      <c r="AC1" s="37"/>
+      <c r="AD1" s="37"/>
+      <c r="AE1" s="37"/>
+      <c r="AF1" s="37"/>
+      <c r="AG1" s="37"/>
+      <c r="AH1" s="37"/>
+      <c r="AI1" s="37"/>
+      <c r="AJ1" s="37"/>
+      <c r="AK1" s="37"/>
+      <c r="AL1" s="37"/>
+      <c r="AM1" s="37"/>
+      <c r="AN1" s="37"/>
+      <c r="AO1" s="37"/>
+      <c r="AP1" s="37"/>
+      <c r="AQ1" s="37"/>
+      <c r="AR1" s="37"/>
+      <c r="AS1" s="37"/>
+      <c r="AT1" s="37"/>
+      <c r="AU1" s="37"/>
+      <c r="AV1" s="37"/>
+      <c r="AW1" s="37"/>
+      <c r="AX1" s="37"/>
+      <c r="AY1" s="37"/>
+      <c r="AZ1" s="37"/>
+      <c r="BA1" s="37"/>
+      <c r="BB1" s="37"/>
+      <c r="BC1" s="37"/>
+      <c r="BD1" s="37"/>
+      <c r="BE1" s="37"/>
+      <c r="BF1" s="37"/>
+      <c r="BG1" s="37"/>
+      <c r="BH1" s="37"/>
+      <c r="BI1" s="37"/>
+      <c r="BJ1" s="37"/>
+      <c r="BK1" s="37"/>
+      <c r="BL1" s="37"/>
+      <c r="BM1" s="37"/>
+      <c r="BN1" s="37"/>
+      <c r="BO1" s="37"/>
+      <c r="BP1" s="37"/>
+      <c r="BQ1" s="37"/>
+      <c r="BR1" s="37"/>
+      <c r="BS1" s="37"/>
+      <c r="BT1" s="37"/>
+      <c r="BU1" s="37"/>
+      <c r="BV1" s="37"/>
+      <c r="BW1" s="37"/>
+      <c r="BX1" s="37"/>
+      <c r="BY1" s="37"/>
+      <c r="BZ1" s="37"/>
+      <c r="CA1" s="37"/>
+      <c r="CB1" s="37"/>
+      <c r="CC1" s="37"/>
+      <c r="CD1" s="37"/>
+      <c r="CE1" s="37"/>
+      <c r="CF1" s="37"/>
+      <c r="CG1" s="37"/>
+      <c r="CH1" s="37"/>
+      <c r="CI1" s="37"/>
+      <c r="CJ1" s="37"/>
+      <c r="CK1" s="37"/>
+      <c r="CL1" s="37"/>
+      <c r="CM1" s="37"/>
+      <c r="CN1" s="37"/>
+      <c r="CO1" s="37"/>
+      <c r="CP1" s="37"/>
+      <c r="CQ1" s="37"/>
+      <c r="CR1" s="37"/>
+      <c r="CS1" s="37"/>
+      <c r="CT1" s="37"/>
+      <c r="CU1" s="37"/>
+      <c r="CV1" s="37"/>
+      <c r="CW1" s="37"/>
+      <c r="CX1" s="37"/>
+      <c r="CY1" s="37"/>
+      <c r="CZ1" s="37"/>
+      <c r="DA1" s="37"/>
+      <c r="DB1" s="37"/>
+      <c r="DC1" s="37"/>
+      <c r="DD1" s="37"/>
+      <c r="DE1" s="37"/>
+      <c r="DF1" s="37"/>
+      <c r="DG1" s="37"/>
+      <c r="DH1" s="37"/>
+      <c r="DI1" s="37"/>
+      <c r="DJ1" s="37"/>
+      <c r="DK1" s="37"/>
+      <c r="DL1" s="38"/>
       <c r="DM1" s="23"/>
     </row>
     <row r="2" spans="2:117" s="2" customFormat="1" ht="42" customHeight="1">
@@ -3553,13 +3560,13 @@
       <c r="DM2" s="17"/>
     </row>
     <row r="3" spans="2:117" ht="42" customHeight="1">
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="39">
+      <c r="C3" s="40">
         <v>2</v>
       </c>
-      <c r="D3" s="39">
+      <c r="D3" s="40">
         <v>23</v>
       </c>
       <c r="E3" s="7" t="s">
@@ -3744,9 +3751,9 @@
       <c r="DM3" s="18"/>
     </row>
     <row r="4" spans="2:117" ht="42" customHeight="1">
-      <c r="B4" s="38"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="40"/>
+      <c r="D4" s="40"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7" t="s">
         <v>4</v>
@@ -3918,9 +3925,9 @@
       <c r="DM4" s="18"/>
     </row>
     <row r="5" spans="2:117" ht="42" customHeight="1">
-      <c r="B5" s="38"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7" t="s">
@@ -4096,9 +4103,9 @@
       <c r="DM5" s="18"/>
     </row>
     <row r="6" spans="2:117" ht="42" customHeight="1">
-      <c r="B6" s="38"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
@@ -4261,9 +4268,9 @@
       <c r="DM6" s="18"/>
     </row>
     <row r="7" spans="2:117" ht="42" customHeight="1">
-      <c r="B7" s="38"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
+      <c r="B7" s="39"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
@@ -4425,9 +4432,9 @@
       <c r="DM7" s="18"/>
     </row>
     <row r="8" spans="2:117" ht="42" customHeight="1">
-      <c r="B8" s="38"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
+      <c r="B8" s="39"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
@@ -4590,13 +4597,13 @@
       <c r="DM8" s="18"/>
     </row>
     <row r="9" spans="2:117" ht="42" customHeight="1">
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="39">
+      <c r="C9" s="40">
         <v>15</v>
       </c>
-      <c r="D9" s="39">
+      <c r="D9" s="40">
         <v>5</v>
       </c>
       <c r="E9" s="7"/>
@@ -4744,18 +4751,28 @@
       <c r="CI9" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="CJ9" s="7"/>
-      <c r="CK9" s="7"/>
-      <c r="CL9" s="7"/>
-      <c r="CM9" s="7"/>
-      <c r="CN9" s="7"/>
-      <c r="CO9" s="7"/>
-      <c r="CP9" s="7"/>
-      <c r="CQ9" s="7"/>
-      <c r="CR9" s="7"/>
-      <c r="CS9" s="7"/>
-      <c r="CT9" s="7"/>
-      <c r="CU9" s="7"/>
+      <c r="CJ9" s="16"/>
+      <c r="CK9" s="16"/>
+      <c r="CL9" s="16"/>
+      <c r="CM9" s="16"/>
+      <c r="CN9" s="16"/>
+      <c r="CO9" s="16"/>
+      <c r="CP9" s="16"/>
+      <c r="CQ9" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="CR9" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="CS9" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="CT9" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="CU9" s="16" t="s">
+        <v>165</v>
+      </c>
       <c r="CV9" s="7"/>
       <c r="CW9" s="7"/>
       <c r="CX9" s="7"/>
@@ -4776,9 +4793,9 @@
       <c r="DM9" s="18"/>
     </row>
     <row r="10" spans="2:117" ht="42" customHeight="1">
-      <c r="B10" s="38"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
@@ -4873,18 +4890,18 @@
       <c r="CG10" s="16"/>
       <c r="CH10" s="16"/>
       <c r="CI10" s="16"/>
-      <c r="CJ10" s="7"/>
-      <c r="CK10" s="7"/>
-      <c r="CL10" s="7"/>
-      <c r="CM10" s="7"/>
-      <c r="CN10" s="7"/>
-      <c r="CO10" s="7"/>
-      <c r="CP10" s="7"/>
-      <c r="CQ10" s="7"/>
-      <c r="CR10" s="7"/>
-      <c r="CS10" s="7"/>
-      <c r="CT10" s="7"/>
-      <c r="CU10" s="7"/>
+      <c r="CJ10" s="16"/>
+      <c r="CK10" s="16"/>
+      <c r="CL10" s="16"/>
+      <c r="CM10" s="16"/>
+      <c r="CN10" s="16"/>
+      <c r="CO10" s="16"/>
+      <c r="CP10" s="16"/>
+      <c r="CQ10" s="16"/>
+      <c r="CR10" s="16"/>
+      <c r="CS10" s="16"/>
+      <c r="CT10" s="16"/>
+      <c r="CU10" s="16"/>
       <c r="CV10" s="7"/>
       <c r="CW10" s="7"/>
       <c r="CX10" s="7"/>
@@ -4905,9 +4922,9 @@
       <c r="DM10" s="18"/>
     </row>
     <row r="11" spans="2:117" ht="42" customHeight="1">
-      <c r="B11" s="38"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
@@ -5004,18 +5021,18 @@
       <c r="CG11" s="16"/>
       <c r="CH11" s="16"/>
       <c r="CI11" s="16"/>
-      <c r="CJ11" s="7"/>
-      <c r="CK11" s="7"/>
-      <c r="CL11" s="7"/>
-      <c r="CM11" s="7"/>
-      <c r="CN11" s="7"/>
-      <c r="CO11" s="7"/>
-      <c r="CP11" s="7"/>
-      <c r="CQ11" s="7"/>
-      <c r="CR11" s="7"/>
-      <c r="CS11" s="7"/>
-      <c r="CT11" s="7"/>
-      <c r="CU11" s="7"/>
+      <c r="CJ11" s="16"/>
+      <c r="CK11" s="16"/>
+      <c r="CL11" s="16"/>
+      <c r="CM11" s="16"/>
+      <c r="CN11" s="16"/>
+      <c r="CO11" s="16"/>
+      <c r="CP11" s="16"/>
+      <c r="CQ11" s="16"/>
+      <c r="CR11" s="16"/>
+      <c r="CS11" s="16"/>
+      <c r="CT11" s="16"/>
+      <c r="CU11" s="16"/>
       <c r="CV11" s="7"/>
       <c r="CW11" s="7"/>
       <c r="CX11" s="7"/>
@@ -5036,9 +5053,9 @@
       <c r="DM11" s="18"/>
     </row>
     <row r="12" spans="2:117" ht="42" customHeight="1">
-      <c r="B12" s="38"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="40"/>
+      <c r="D12" s="40"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
@@ -5132,18 +5149,18 @@
       <c r="CG12" s="16"/>
       <c r="CH12" s="16"/>
       <c r="CI12" s="16"/>
-      <c r="CJ12" s="7"/>
-      <c r="CK12" s="7"/>
-      <c r="CL12" s="7"/>
-      <c r="CM12" s="7"/>
-      <c r="CN12" s="7"/>
-      <c r="CO12" s="7"/>
-      <c r="CP12" s="7"/>
-      <c r="CQ12" s="7"/>
-      <c r="CR12" s="7"/>
-      <c r="CS12" s="7"/>
-      <c r="CT12" s="7"/>
-      <c r="CU12" s="7"/>
+      <c r="CJ12" s="16"/>
+      <c r="CK12" s="16"/>
+      <c r="CL12" s="16"/>
+      <c r="CM12" s="16"/>
+      <c r="CN12" s="16"/>
+      <c r="CO12" s="16"/>
+      <c r="CP12" s="16"/>
+      <c r="CQ12" s="16"/>
+      <c r="CR12" s="16"/>
+      <c r="CS12" s="16"/>
+      <c r="CT12" s="16"/>
+      <c r="CU12" s="16"/>
       <c r="CV12" s="7"/>
       <c r="CW12" s="7"/>
       <c r="CX12" s="7"/>
@@ -5164,9 +5181,9 @@
       <c r="DM12" s="18"/>
     </row>
     <row r="13" spans="2:117" ht="42" customHeight="1">
-      <c r="B13" s="38"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
+      <c r="B13" s="39"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
@@ -5262,18 +5279,18 @@
       <c r="CG13" s="16"/>
       <c r="CH13" s="16"/>
       <c r="CI13" s="16"/>
-      <c r="CJ13" s="7"/>
-      <c r="CK13" s="7"/>
-      <c r="CL13" s="7"/>
-      <c r="CM13" s="7"/>
-      <c r="CN13" s="7"/>
-      <c r="CO13" s="7"/>
-      <c r="CP13" s="7"/>
-      <c r="CQ13" s="7"/>
-      <c r="CR13" s="7"/>
-      <c r="CS13" s="7"/>
-      <c r="CT13" s="7"/>
-      <c r="CU13" s="7"/>
+      <c r="CJ13" s="16"/>
+      <c r="CK13" s="16"/>
+      <c r="CL13" s="16"/>
+      <c r="CM13" s="16"/>
+      <c r="CN13" s="16"/>
+      <c r="CO13" s="16"/>
+      <c r="CP13" s="16"/>
+      <c r="CQ13" s="16"/>
+      <c r="CR13" s="16"/>
+      <c r="CS13" s="16"/>
+      <c r="CT13" s="16"/>
+      <c r="CU13" s="16"/>
       <c r="CV13" s="7"/>
       <c r="CW13" s="7"/>
       <c r="CX13" s="7"/>
@@ -5294,9 +5311,9 @@
       <c r="DM13" s="18"/>
     </row>
     <row r="14" spans="2:117" ht="42" customHeight="1">
-      <c r="B14" s="38"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
+      <c r="B14" s="39"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
@@ -5390,18 +5407,18 @@
       <c r="CG14" s="16"/>
       <c r="CH14" s="16"/>
       <c r="CI14" s="16"/>
-      <c r="CJ14" s="7"/>
-      <c r="CK14" s="7"/>
-      <c r="CL14" s="7"/>
-      <c r="CM14" s="7"/>
-      <c r="CN14" s="7"/>
-      <c r="CO14" s="7"/>
-      <c r="CP14" s="7"/>
-      <c r="CQ14" s="7"/>
-      <c r="CR14" s="7"/>
-      <c r="CS14" s="7"/>
-      <c r="CT14" s="7"/>
-      <c r="CU14" s="7"/>
+      <c r="CJ14" s="16"/>
+      <c r="CK14" s="16"/>
+      <c r="CL14" s="16"/>
+      <c r="CM14" s="16"/>
+      <c r="CN14" s="16"/>
+      <c r="CO14" s="16"/>
+      <c r="CP14" s="16"/>
+      <c r="CQ14" s="16"/>
+      <c r="CR14" s="16"/>
+      <c r="CS14" s="16"/>
+      <c r="CT14" s="16"/>
+      <c r="CU14" s="16"/>
       <c r="CV14" s="7"/>
       <c r="CW14" s="7"/>
       <c r="CX14" s="7"/>
@@ -5860,143 +5877,143 @@
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="36" t="s">
+      <c r="E18" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="36"/>
-      <c r="J18" s="36"/>
-      <c r="K18" s="36"/>
-      <c r="L18" s="36"/>
-      <c r="M18" s="36"/>
-      <c r="N18" s="36"/>
-      <c r="O18" s="36"/>
-      <c r="P18" s="36"/>
-      <c r="Q18" s="36"/>
-      <c r="R18" s="36"/>
-      <c r="S18" s="36"/>
-      <c r="T18" s="36"/>
-      <c r="U18" s="36"/>
-      <c r="V18" s="36"/>
-      <c r="W18" s="36"/>
-      <c r="X18" s="36"/>
-      <c r="Y18" s="36"/>
-      <c r="Z18" s="36"/>
-      <c r="AA18" s="36"/>
-      <c r="AB18" s="36"/>
-      <c r="AC18" s="36"/>
-      <c r="AD18" s="36"/>
-      <c r="AE18" s="36"/>
-      <c r="AF18" s="36"/>
-      <c r="AG18" s="36"/>
-      <c r="AH18" s="36"/>
-      <c r="AI18" s="36"/>
-      <c r="AJ18" s="36"/>
-      <c r="AK18" s="36"/>
-      <c r="AL18" s="36"/>
-      <c r="AM18" s="36"/>
-      <c r="AN18" s="36"/>
-      <c r="AO18" s="36"/>
-      <c r="AP18" s="36"/>
-      <c r="AQ18" s="36"/>
-      <c r="AR18" s="36"/>
-      <c r="AS18" s="36"/>
-      <c r="AT18" s="36"/>
-      <c r="AU18" s="36"/>
-      <c r="AV18" s="36"/>
-      <c r="AW18" s="36"/>
-      <c r="AX18" s="36"/>
-      <c r="AY18" s="36"/>
-      <c r="AZ18" s="36"/>
-      <c r="BA18" s="36"/>
-      <c r="BB18" s="36"/>
-      <c r="BC18" s="36"/>
-      <c r="BD18" s="36"/>
-      <c r="BE18" s="36"/>
-      <c r="BF18" s="36"/>
-      <c r="BG18" s="36"/>
-      <c r="BH18" s="36"/>
-      <c r="BI18" s="36"/>
-      <c r="BJ18" s="36"/>
-      <c r="BK18" s="36"/>
-      <c r="BL18" s="36"/>
-      <c r="BM18" s="36"/>
-      <c r="BN18" s="36"/>
-      <c r="BO18" s="36"/>
-      <c r="BP18" s="36"/>
-      <c r="BQ18" s="36"/>
-      <c r="BR18" s="36"/>
-      <c r="BS18" s="36"/>
-      <c r="BT18" s="36"/>
-      <c r="BU18" s="36"/>
-      <c r="BV18" s="36"/>
-      <c r="BW18" s="36"/>
-      <c r="BX18" s="36"/>
-      <c r="BY18" s="36"/>
-      <c r="BZ18" s="36"/>
-      <c r="CA18" s="36"/>
-      <c r="CB18" s="36"/>
-      <c r="CC18" s="36"/>
-      <c r="CD18" s="36"/>
-      <c r="CE18" s="36"/>
-      <c r="CF18" s="36"/>
-      <c r="CG18" s="36"/>
-      <c r="CH18" s="36"/>
-      <c r="CI18" s="36"/>
-      <c r="CJ18" s="36"/>
-      <c r="CK18" s="36"/>
-      <c r="CL18" s="36"/>
-      <c r="CM18" s="36"/>
-      <c r="CN18" s="36"/>
-      <c r="CO18" s="36"/>
-      <c r="CP18" s="36"/>
-      <c r="CQ18" s="36"/>
-      <c r="CR18" s="36"/>
-      <c r="CS18" s="36"/>
-      <c r="CT18" s="36"/>
-      <c r="CU18" s="36"/>
-      <c r="CV18" s="36"/>
-      <c r="CW18" s="36"/>
-      <c r="CX18" s="36"/>
-      <c r="CY18" s="36"/>
-      <c r="CZ18" s="36"/>
-      <c r="DA18" s="36"/>
-      <c r="DB18" s="36"/>
-      <c r="DC18" s="36"/>
-      <c r="DD18" s="36"/>
-      <c r="DE18" s="36"/>
-      <c r="DF18" s="36"/>
-      <c r="DG18" s="36"/>
-      <c r="DH18" s="36"/>
-      <c r="DI18" s="36"/>
-      <c r="DJ18" s="36"/>
-      <c r="DK18" s="36"/>
-      <c r="DL18" s="36"/>
-      <c r="DM18" s="36"/>
-      <c r="DN18" s="36"/>
-      <c r="DO18" s="36"/>
-      <c r="DP18" s="36"/>
-      <c r="DQ18" s="36"/>
-      <c r="DR18" s="36"/>
-      <c r="DS18" s="36"/>
-      <c r="DT18" s="36"/>
-      <c r="DU18" s="36"/>
-      <c r="DV18" s="36"/>
-      <c r="DW18" s="36"/>
-      <c r="DX18" s="36"/>
-      <c r="DY18" s="36"/>
-      <c r="DZ18" s="36"/>
-      <c r="EA18" s="36"/>
-      <c r="EB18" s="36"/>
-      <c r="EC18" s="36"/>
-      <c r="ED18" s="36"/>
-      <c r="EE18" s="36"/>
-      <c r="EF18" s="36"/>
-      <c r="EG18" s="36"/>
-      <c r="EH18" s="36"/>
-      <c r="EI18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="37"/>
+      <c r="N18" s="37"/>
+      <c r="O18" s="37"/>
+      <c r="P18" s="37"/>
+      <c r="Q18" s="37"/>
+      <c r="R18" s="37"/>
+      <c r="S18" s="37"/>
+      <c r="T18" s="37"/>
+      <c r="U18" s="37"/>
+      <c r="V18" s="37"/>
+      <c r="W18" s="37"/>
+      <c r="X18" s="37"/>
+      <c r="Y18" s="37"/>
+      <c r="Z18" s="37"/>
+      <c r="AA18" s="37"/>
+      <c r="AB18" s="37"/>
+      <c r="AC18" s="37"/>
+      <c r="AD18" s="37"/>
+      <c r="AE18" s="37"/>
+      <c r="AF18" s="37"/>
+      <c r="AG18" s="37"/>
+      <c r="AH18" s="37"/>
+      <c r="AI18" s="37"/>
+      <c r="AJ18" s="37"/>
+      <c r="AK18" s="37"/>
+      <c r="AL18" s="37"/>
+      <c r="AM18" s="37"/>
+      <c r="AN18" s="37"/>
+      <c r="AO18" s="37"/>
+      <c r="AP18" s="37"/>
+      <c r="AQ18" s="37"/>
+      <c r="AR18" s="37"/>
+      <c r="AS18" s="37"/>
+      <c r="AT18" s="37"/>
+      <c r="AU18" s="37"/>
+      <c r="AV18" s="37"/>
+      <c r="AW18" s="37"/>
+      <c r="AX18" s="37"/>
+      <c r="AY18" s="37"/>
+      <c r="AZ18" s="37"/>
+      <c r="BA18" s="37"/>
+      <c r="BB18" s="37"/>
+      <c r="BC18" s="37"/>
+      <c r="BD18" s="37"/>
+      <c r="BE18" s="37"/>
+      <c r="BF18" s="37"/>
+      <c r="BG18" s="37"/>
+      <c r="BH18" s="37"/>
+      <c r="BI18" s="37"/>
+      <c r="BJ18" s="37"/>
+      <c r="BK18" s="37"/>
+      <c r="BL18" s="37"/>
+      <c r="BM18" s="37"/>
+      <c r="BN18" s="37"/>
+      <c r="BO18" s="37"/>
+      <c r="BP18" s="37"/>
+      <c r="BQ18" s="37"/>
+      <c r="BR18" s="37"/>
+      <c r="BS18" s="37"/>
+      <c r="BT18" s="37"/>
+      <c r="BU18" s="37"/>
+      <c r="BV18" s="37"/>
+      <c r="BW18" s="37"/>
+      <c r="BX18" s="37"/>
+      <c r="BY18" s="37"/>
+      <c r="BZ18" s="37"/>
+      <c r="CA18" s="37"/>
+      <c r="CB18" s="37"/>
+      <c r="CC18" s="37"/>
+      <c r="CD18" s="37"/>
+      <c r="CE18" s="37"/>
+      <c r="CF18" s="37"/>
+      <c r="CG18" s="37"/>
+      <c r="CH18" s="37"/>
+      <c r="CI18" s="37"/>
+      <c r="CJ18" s="37"/>
+      <c r="CK18" s="37"/>
+      <c r="CL18" s="37"/>
+      <c r="CM18" s="37"/>
+      <c r="CN18" s="37"/>
+      <c r="CO18" s="37"/>
+      <c r="CP18" s="37"/>
+      <c r="CQ18" s="37"/>
+      <c r="CR18" s="37"/>
+      <c r="CS18" s="37"/>
+      <c r="CT18" s="37"/>
+      <c r="CU18" s="37"/>
+      <c r="CV18" s="37"/>
+      <c r="CW18" s="37"/>
+      <c r="CX18" s="37"/>
+      <c r="CY18" s="37"/>
+      <c r="CZ18" s="37"/>
+      <c r="DA18" s="37"/>
+      <c r="DB18" s="37"/>
+      <c r="DC18" s="37"/>
+      <c r="DD18" s="37"/>
+      <c r="DE18" s="37"/>
+      <c r="DF18" s="37"/>
+      <c r="DG18" s="37"/>
+      <c r="DH18" s="37"/>
+      <c r="DI18" s="37"/>
+      <c r="DJ18" s="37"/>
+      <c r="DK18" s="37"/>
+      <c r="DL18" s="37"/>
+      <c r="DM18" s="37"/>
+      <c r="DN18" s="37"/>
+      <c r="DO18" s="37"/>
+      <c r="DP18" s="37"/>
+      <c r="DQ18" s="37"/>
+      <c r="DR18" s="37"/>
+      <c r="DS18" s="37"/>
+      <c r="DT18" s="37"/>
+      <c r="DU18" s="37"/>
+      <c r="DV18" s="37"/>
+      <c r="DW18" s="37"/>
+      <c r="DX18" s="37"/>
+      <c r="DY18" s="37"/>
+      <c r="DZ18" s="37"/>
+      <c r="EA18" s="37"/>
+      <c r="EB18" s="37"/>
+      <c r="EC18" s="37"/>
+      <c r="ED18" s="37"/>
+      <c r="EE18" s="37"/>
+      <c r="EF18" s="37"/>
+      <c r="EG18" s="37"/>
+      <c r="EH18" s="37"/>
+      <c r="EI18" s="38"/>
     </row>
     <row r="19" spans="2:139" s="2" customFormat="1" ht="42" customHeight="1" thickBot="1">
       <c r="B19" s="11" t="s">
@@ -6529,7 +6546,7 @@
         <v>242</v>
       </c>
       <c r="EE19" s="12">
-        <f t="shared" ref="EE19:EG19" si="184">ED19+1</f>
+        <f t="shared" ref="EE19" si="184">ED19+1</f>
         <v>243</v>
       </c>
       <c r="EF19" s="12">
@@ -6999,7 +7016,7 @@
       <c r="EH21" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="EI21" s="40" t="s">
+      <c r="EI21" s="36" t="s">
         <v>99</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Precision fixed through all of inverse components.
</commit_message>
<xml_diff>
--- a/doc/design/schedule.xlsx
+++ b/doc/design/schedule.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="167">
   <si>
     <t>sincos</t>
   </si>
@@ -517,6 +517,9 @@
   </si>
   <si>
     <t>T06 x Z0</t>
+  </si>
+  <si>
+    <t>T06 x Z0 accum</t>
   </si>
 </sst>
 </file>
@@ -755,8 +758,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="875">
+  <cellStyleXfs count="879">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1755,7 +1762,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="875">
+  <cellStyles count="879">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2193,6 +2200,8 @@
     <cellStyle name="Followed Hyperlink" xfId="870" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="872" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="874" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="876" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="878" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2630,6 +2639,8 @@
     <cellStyle name="Hyperlink" xfId="869" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="871" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="873" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="875" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="877" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2968,15 +2979,15 @@
       <pane xSplit="4" ySplit="2" topLeftCell="BN3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="AL1" sqref="AL1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="CB6" sqref="CB6"/>
+      <selection pane="bottomRight" activeCell="CV16" sqref="CV16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.33203125" defaultRowHeight="42" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.33203125" style="6" customWidth="1"/>
     <col min="2" max="4" width="10.33203125" style="2" customWidth="1"/>
-    <col min="5" max="94" width="4.33203125" style="9"/>
-    <col min="95" max="95" width="4.33203125" style="9" customWidth="1"/>
+    <col min="5" max="93" width="4.33203125" style="9"/>
+    <col min="94" max="95" width="4.33203125" style="9" customWidth="1"/>
     <col min="96" max="16384" width="4.33203125" style="9"/>
   </cols>
   <sheetData>
@@ -5848,8 +5859,12 @@
       <c r="CR16" s="13"/>
       <c r="CS16" s="13"/>
       <c r="CT16" s="14"/>
-      <c r="CU16" s="14"/>
-      <c r="CV16" s="13"/>
+      <c r="CU16" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="CV16" s="14" t="s">
+        <v>166</v>
+      </c>
       <c r="CW16" s="13"/>
       <c r="CX16" s="13" t="s">
         <v>104</v>

</xml_diff>